<commit_message>
Update Test case sheet
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BVT!$A$1:$J$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$D$1:$D$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mini_EPG!$A$1:$J$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Regression!$A$1:$O$442</definedName>
   </definedNames>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4718" uniqueCount="2117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4728" uniqueCount="2118">
   <si>
     <t>Name</t>
   </si>
@@ -10991,6 +10992,9 @@
   </si>
   <si>
     <t>77666_A</t>
+  </si>
+  <si>
+    <t>ankit</t>
   </si>
 </sst>
 </file>
@@ -15430,7 +15434,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -16364,7 +16368,7 @@
   <dimension ref="A1:O442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30946,124 +30950,178 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
-    <col min="3" max="3" width="149" customWidth="1"/>
-    <col min="4" max="4" width="74.44140625" customWidth="1"/>
+    <col min="1" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="6" max="6" width="149" customWidth="1"/>
+    <col min="7" max="7" width="74.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>2112</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2077</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>2084</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>2111</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>2110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2109</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>2108</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>2107</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2106</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>2105</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>2104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="165.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="165.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2103</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>2102</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="F4" s="22" t="s">
         <v>2101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>2100</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>2099</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>2098</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2097</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>2117</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>2096</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>2095</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>2094</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>2093</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>2092</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>2091</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>2090</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="F8" s="22" t="s">
         <v>2089</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Test case sheet
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -11043,7 +11043,7 @@
     <t>TM/Server/Upgrade related</t>
   </si>
   <si>
-    <t>MiniEPG Already Covered</t>
+    <t>MiniEPG already Covered</t>
   </si>
 </sst>
 </file>
@@ -32297,7 +32297,7 @@
   <autoFilter ref="A1:P442">
     <filterColumn colId="2">
       <filters>
-        <filter val="MiniEPG Covered"/>
+        <filter val="MiniEPG Already Covered"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">

</xml_diff>

<commit_message>
old test case bug fix and new test case creation
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -32314,8 +32314,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
create new test cases of EPG
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BVT!$A$1:$J$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$D$1:$D$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mini_EPG!$A$1:$J$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Regression!$A$1:$P$442</definedName>
   </definedNames>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5327" uniqueCount="2234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5333" uniqueCount="2234">
   <si>
     <t>Name</t>
   </si>
@@ -33143,8 +33144,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33262,7 +33264,9 @@
         <v>2100</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>604</v>
       </c>
@@ -33370,7 +33374,9 @@
         <v>2094</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>604</v>
       </c>
@@ -33669,6 +33675,9 @@
       <c r="B15" s="64" t="s">
         <v>2196</v>
       </c>
+      <c r="D15" t="s">
+        <v>599</v>
+      </c>
       <c r="E15" t="s">
         <v>604</v>
       </c>
@@ -34027,6 +34036,12 @@
       </c>
       <c r="B26" s="64" t="s">
         <v>2153</v>
+      </c>
+      <c r="D26" t="s">
+        <v>599</v>
+      </c>
+      <c r="E26" t="s">
+        <v>604</v>
       </c>
       <c r="F26" s="63" t="s">
         <v>2152</v>
@@ -34208,6 +34223,9 @@
       <c r="B32" s="50" t="s">
         <v>2129</v>
       </c>
+      <c r="D32" t="s">
+        <v>599</v>
+      </c>
       <c r="E32" t="s">
         <v>604</v>
       </c>
@@ -34270,6 +34288,7 @@
       <c r="T33" s="44"/>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
commit Test case and TestcaseSheet
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BVT!$A$1:$J$127</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$D$1:$D$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$A$1:$T$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mini_EPG!$A$1:$J$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Regression!$A$1:$P$442</definedName>
   </definedNames>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5333" uniqueCount="2234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5345" uniqueCount="2234">
   <si>
     <t>Name</t>
   </si>
@@ -17236,7 +17236,7 @@
   <dimension ref="A1:P442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C366" sqref="C366:C388"/>
+      <selection activeCell="C287" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33144,9 +33144,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33228,7 +33228,9 @@
         <v>2102</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E2" s="6" t="s">
         <v>598</v>
       </c>
@@ -33302,7 +33304,9 @@
         <v>2098</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>612</v>
       </c>
@@ -33338,7 +33342,9 @@
         <v>2096</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>689</v>
       </c>
@@ -33410,7 +33416,9 @@
         <v>2092</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>612</v>
       </c>
@@ -33610,6 +33618,9 @@
       <c r="B13" s="64" t="s">
         <v>2204</v>
       </c>
+      <c r="D13" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E13" t="s">
         <v>612</v>
       </c>
@@ -33712,6 +33723,9 @@
       <c r="B16" s="64" t="s">
         <v>2193</v>
       </c>
+      <c r="D16" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E16" t="s">
         <v>612</v>
       </c>
@@ -33842,6 +33856,12 @@
       <c r="B20" s="64" t="s">
         <v>2177</v>
       </c>
+      <c r="D20" t="s">
+        <v>599</v>
+      </c>
+      <c r="E20" t="s">
+        <v>598</v>
+      </c>
       <c r="F20" s="63" t="s">
         <v>2176</v>
       </c>
@@ -33873,6 +33893,12 @@
       <c r="B21" s="64" t="s">
         <v>2173</v>
       </c>
+      <c r="D21" t="s">
+        <v>599</v>
+      </c>
+      <c r="E21" t="s">
+        <v>598</v>
+      </c>
       <c r="F21" s="63" t="s">
         <v>2172</v>
       </c>
@@ -33937,6 +33963,9 @@
       </c>
       <c r="B23" s="64" t="s">
         <v>2165</v>
+      </c>
+      <c r="D23" t="s">
+        <v>599</v>
       </c>
       <c r="E23" t="s">
         <v>598</v>
@@ -34260,6 +34289,9 @@
       <c r="B33" s="50" t="s">
         <v>2129</v>
       </c>
+      <c r="D33" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="E33" t="s">
         <v>612</v>
       </c>
@@ -34288,7 +34320,6 @@
       <c r="T33" s="44"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
commit pritam test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -16313,8 +16313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33144,9 +33144,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Assigned test case to Team
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BVT!$A$1:$J$127</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$A$1:$T$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$A$1:$U$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mini_EPG!$A$1:$J$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Regression!$A$1:$P$442</definedName>
   </definedNames>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5345" uniqueCount="2234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5375" uniqueCount="2235">
   <si>
     <t>Name</t>
   </si>
@@ -11402,6 +11402,9 @@
   </si>
   <si>
     <t>S.NO.</t>
+  </si>
+  <si>
+    <t>Coverd In Regression</t>
   </si>
 </sst>
 </file>
@@ -11800,7 +11803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -12023,6 +12026,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12260,16 +12278,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>6063193</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509060</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>497418</xdr:rowOff>
+      <xdr:rowOff>328085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2742143</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3427943</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>935568</xdr:rowOff>
+      <xdr:rowOff>766235</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -12278,8 +12296,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2436073" y="5122758"/>
-          <a:ext cx="610870" cy="0"/>
+          <a:off x="17645593" y="9133418"/>
+          <a:ext cx="2918883" cy="438150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12335,10 +12353,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>6028267</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>448734</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>947207</xdr:rowOff>
+      <xdr:rowOff>769407</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2972858" cy="333375"/>
     <xdr:pic>
@@ -12363,7 +12381,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2439247" y="5122967"/>
+          <a:off x="17585267" y="9574740"/>
           <a:ext cx="2972858" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16313,8 +16331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16323,7 +16341,7 @@
     <col min="2" max="2" width="40.88671875" style="22" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="70" style="24" customWidth="1"/>
     <col min="7" max="7" width="126.109375" style="24" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" customWidth="1"/>
@@ -17235,8 +17253,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C287" sqref="C287"/>
+    <sheetView tabSelected="1" topLeftCell="G132" workbookViewId="0">
+      <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21961,7 +21979,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>193</v>
       </c>
@@ -22000,7 +22018,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>194</v>
       </c>
@@ -22039,7 +22057,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>196</v>
       </c>
@@ -22078,7 +22096,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>197</v>
       </c>
@@ -22115,7 +22133,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>199</v>
       </c>
@@ -22152,7 +22170,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>200</v>
       </c>
@@ -22189,7 +22207,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>202</v>
       </c>
@@ -22810,7 +22828,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>224</v>
       </c>
@@ -22848,7 +22866,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>225</v>
       </c>
@@ -22883,7 +22901,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>227</v>
       </c>
@@ -22921,7 +22939,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>228</v>
       </c>
@@ -22959,7 +22977,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>231</v>
       </c>
@@ -22997,7 +23015,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>232</v>
       </c>
@@ -23032,7 +23050,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>233</v>
       </c>
@@ -23067,7 +23085,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>234</v>
       </c>
@@ -23102,7 +23120,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>235</v>
       </c>
@@ -23137,7 +23155,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>236</v>
       </c>
@@ -23172,7 +23190,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>237</v>
       </c>
@@ -23280,7 +23298,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>240</v>
       </c>
@@ -23318,7 +23336,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>241</v>
       </c>
@@ -23353,7 +23371,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>242</v>
       </c>
@@ -23391,7 +23409,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>243</v>
       </c>
@@ -23426,7 +23444,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>244</v>
       </c>
@@ -23464,7 +23482,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>245</v>
       </c>
@@ -23499,7 +23517,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>246</v>
       </c>
@@ -23534,7 +23552,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>247</v>
       </c>
@@ -26671,7 +26689,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>355</v>
       </c>
@@ -26706,7 +26724,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>356</v>
       </c>
@@ -26811,7 +26829,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>362</v>
       </c>
@@ -26846,7 +26864,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>363</v>
       </c>
@@ -26916,7 +26934,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>365</v>
       </c>
@@ -27065,7 +27083,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>369</v>
       </c>
@@ -27211,7 +27229,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>373</v>
       </c>
@@ -27590,7 +27608,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>386</v>
       </c>
@@ -30422,7 +30440,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>479</v>
       </c>
@@ -30457,7 +30475,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>480</v>
       </c>
@@ -30492,7 +30510,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>481</v>
       </c>
@@ -30527,7 +30545,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="330.6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:16" ht="330.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>482</v>
       </c>
@@ -30562,7 +30580,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>483</v>
       </c>
@@ -30599,7 +30617,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>484</v>
       </c>
@@ -30634,7 +30652,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>485</v>
       </c>
@@ -30669,7 +30687,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>486</v>
       </c>
@@ -30704,7 +30722,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>487</v>
       </c>
@@ -30739,7 +30757,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>489</v>
       </c>
@@ -30774,7 +30792,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>490</v>
       </c>
@@ -30809,7 +30827,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>491</v>
       </c>
@@ -30844,7 +30862,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>492</v>
       </c>
@@ -30879,7 +30897,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>493</v>
       </c>
@@ -30914,7 +30932,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>494</v>
       </c>
@@ -30949,7 +30967,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>495</v>
       </c>
@@ -30984,7 +31002,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>498</v>
       </c>
@@ -31019,7 +31037,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>499</v>
       </c>
@@ -31054,7 +31072,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>500</v>
       </c>
@@ -31089,7 +31107,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>501</v>
       </c>
@@ -31124,7 +31142,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>503</v>
       </c>
@@ -31159,7 +31177,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>504</v>
       </c>
@@ -31194,7 +31212,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>505</v>
       </c>
@@ -33125,14 +33143,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P442">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="MiniEPG Already Covered"/>
-      </filters>
+    <filterColumn colId="4">
+      <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Rahul"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -33142,23 +33163,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="43"/>
-    <col min="3" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="73.44140625" customWidth="1"/>
-    <col min="7" max="7" width="91" style="42" customWidth="1"/>
-    <col min="8" max="8" width="65.6640625" style="42" customWidth="1"/>
+    <col min="3" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="73.44140625" customWidth="1"/>
+    <col min="8" max="8" width="91" style="42" customWidth="1"/>
+    <col min="9" max="9" width="65.6640625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="84" t="s">
         <v>2233</v>
       </c>
@@ -33172,81 +33194,86 @@
         <v>2077</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>2234</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>2084</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="G1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="I1" s="81" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="J1" s="79" t="s">
         <v>2082</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="K1" s="79" t="s">
         <v>2081</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="L1" s="79" t="s">
         <v>2080</v>
       </c>
-      <c r="L1" s="80" t="s">
+      <c r="M1" s="80" t="s">
         <v>2079</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="N1" s="80" t="s">
         <v>2078</v>
       </c>
-      <c r="N1" s="79" t="s">
+      <c r="O1" s="79" t="s">
         <v>2232</v>
       </c>
-      <c r="O1" s="79" t="s">
+      <c r="P1" s="79" t="s">
         <v>2231</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="Q1" s="79" t="s">
         <v>2230</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="R1" s="79" t="s">
         <v>2229</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="S1" s="79" t="s">
         <v>490</v>
       </c>
-      <c r="S1" s="79" t="s">
+      <c r="T1" s="79" t="s">
         <v>2228</v>
       </c>
-      <c r="T1" s="78" t="s">
+      <c r="U1" s="78" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="111.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2102</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D2" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="G2" s="77" t="s">
         <v>2101</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="H2" s="75" t="s">
         <v>2227</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="I2" s="74" t="s">
         <v>2226</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="29" t="s">
+        <v>693</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -33256,35 +33283,38 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="73"/>
-    </row>
-    <row r="3" spans="1:20" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="1"/>
+      <c r="U2" s="73"/>
+    </row>
+    <row r="3" spans="1:21" ht="121.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2100</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D3" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="G3" s="77" t="s">
         <v>2099</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="H3" s="75" t="s">
         <v>2225</v>
       </c>
-      <c r="H3" s="74" t="s">
+      <c r="I3" s="74" t="s">
         <v>2224</v>
       </c>
-      <c r="I3" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="29" t="s">
+        <v>693</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -33294,35 +33324,38 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="73"/>
-    </row>
-    <row r="4" spans="1:20" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T3" s="1"/>
+      <c r="U3" s="73"/>
+    </row>
+    <row r="4" spans="1:21" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="51">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2098</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D4" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="G4" s="77" t="s">
         <v>2097</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="H4" s="75" t="s">
         <v>2223</v>
       </c>
-      <c r="H4" s="74" t="s">
+      <c r="I4" s="74" t="s">
         <v>2222</v>
       </c>
-      <c r="I4" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="29" t="s">
+        <v>693</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -33332,35 +33365,38 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="73"/>
-    </row>
-    <row r="5" spans="1:20" ht="229.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T4" s="1"/>
+      <c r="U4" s="73"/>
+    </row>
+    <row r="5" spans="1:21" ht="229.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="51">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>2096</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D5" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="G5" s="76" t="s">
         <v>2095</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="H5" s="75" t="s">
         <v>2221</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="I5" s="74" t="s">
         <v>2220</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="29" t="s">
+        <v>693</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -33370,32 +33406,35 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="73"/>
-    </row>
-    <row r="6" spans="1:20" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T5" s="1"/>
+      <c r="U5" s="73"/>
+    </row>
+    <row r="6" spans="1:21" ht="141" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>2094</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="G6" s="76" t="s">
         <v>2093</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="H6" s="75" t="s">
         <v>2219</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="I6" s="74" t="s">
         <v>2218</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -33406,32 +33445,35 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="73"/>
-    </row>
-    <row r="7" spans="1:20" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T6" s="1"/>
+      <c r="U6" s="73"/>
+    </row>
+    <row r="7" spans="1:21" ht="192.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>2092</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D7" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="G7" s="76" t="s">
         <v>2091</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="H7" s="75" t="s">
         <v>2217</v>
       </c>
-      <c r="H7" s="74" t="s">
+      <c r="I7" s="74" t="s">
         <v>2216</v>
       </c>
-      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -33442,9 +33484,10 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="73"/>
-    </row>
-    <row r="8" spans="1:20" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T7" s="1"/>
+      <c r="U7" s="73"/>
+    </row>
+    <row r="8" spans="1:21" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="51">
         <v>7</v>
       </c>
@@ -33453,19 +33496,19 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="F8" s="76" t="s">
+      <c r="G8" s="76" t="s">
         <v>2089</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="H8" s="75" t="s">
         <v>2215</v>
       </c>
-      <c r="H8" s="74" t="s">
+      <c r="I8" s="74" t="s">
         <v>2214</v>
       </c>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -33476,31 +33519,34 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="73"/>
-    </row>
-    <row r="9" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T8" s="1"/>
+      <c r="U8" s="73"/>
+    </row>
+    <row r="9" spans="1:21" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51">
         <v>8</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>2213</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>1215</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="72" t="s">
+      <c r="H9" s="72" t="s">
         <v>279</v>
       </c>
-      <c r="H9" s="71" t="s">
+      <c r="I9" s="71" t="s">
         <v>898</v>
       </c>
-      <c r="I9" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J9" s="60"/>
+      <c r="J9" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K9" s="60"/>
       <c r="L9" s="60"/>
       <c r="M9" s="60"/>
@@ -33510,31 +33556,34 @@
       <c r="Q9" s="60"/>
       <c r="R9" s="60"/>
       <c r="S9" s="60"/>
-      <c r="T9" s="59"/>
-    </row>
-    <row r="10" spans="1:20" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T9" s="60"/>
+      <c r="U9" s="59"/>
+    </row>
+    <row r="10" spans="1:21" ht="130.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51">
         <v>9</v>
       </c>
       <c r="B10" s="64" t="s">
         <v>2212</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>1215</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="H10" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="71" t="s">
+      <c r="I10" s="71" t="s">
         <v>2211</v>
       </c>
-      <c r="I10" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J10" s="60"/>
+      <c r="J10" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K10" s="60"/>
       <c r="L10" s="60"/>
       <c r="M10" s="60"/>
@@ -33544,31 +33593,34 @@
       <c r="Q10" s="60"/>
       <c r="R10" s="60"/>
       <c r="S10" s="60"/>
-      <c r="T10" s="59"/>
-    </row>
-    <row r="11" spans="1:20" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T10" s="60"/>
+      <c r="U10" s="59"/>
+    </row>
+    <row r="11" spans="1:21" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="51">
         <v>10</v>
       </c>
       <c r="B11" s="64" t="s">
         <v>2210</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>1215</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="H11" s="70" t="s">
         <v>2209</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="I11" s="68" t="s">
         <v>286</v>
       </c>
-      <c r="I11" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J11" s="60"/>
+      <c r="J11" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K11" s="60"/>
       <c r="L11" s="60"/>
       <c r="M11" s="60"/>
@@ -33578,28 +33630,34 @@
       <c r="Q11" s="60"/>
       <c r="R11" s="60"/>
       <c r="S11" s="60"/>
-      <c r="T11" s="59"/>
-    </row>
-    <row r="12" spans="1:20" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T11" s="60"/>
+      <c r="U11" s="59"/>
+    </row>
+    <row r="12" spans="1:21" ht="88.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="51">
         <v>11</v>
       </c>
       <c r="B12" s="64" t="s">
         <v>2208</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="C12" s="87" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G12" s="63" t="s">
         <v>2207</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="H12" s="69" t="s">
         <v>2206</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="I12" s="68" t="s">
         <v>2205</v>
       </c>
-      <c r="I12" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J12" s="60"/>
+      <c r="J12" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K12" s="60"/>
       <c r="L12" s="60"/>
       <c r="M12" s="60"/>
@@ -33609,34 +33667,38 @@
       <c r="Q12" s="60"/>
       <c r="R12" s="60"/>
       <c r="S12" s="60"/>
-      <c r="T12" s="59"/>
-    </row>
-    <row r="13" spans="1:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T12" s="60"/>
+      <c r="U12" s="59"/>
+    </row>
+    <row r="13" spans="1:21" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51">
         <v>12</v>
       </c>
       <c r="B13" s="64" t="s">
         <v>2204</v>
       </c>
+      <c r="C13" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D13" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="88"/>
+      <c r="F13" t="s">
         <v>612</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="G13" s="63" t="s">
         <v>2203</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="H13" s="48" t="s">
         <v>2202</v>
       </c>
-      <c r="H13" s="68" t="s">
+      <c r="I13" s="68" t="s">
         <v>2201</v>
       </c>
-      <c r="I13" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J13" s="60"/>
+      <c r="J13" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K13" s="60"/>
       <c r="L13" s="60"/>
       <c r="M13" s="60"/>
@@ -33646,28 +33708,31 @@
       <c r="Q13" s="60"/>
       <c r="R13" s="60"/>
       <c r="S13" s="60"/>
-      <c r="T13" s="59"/>
-    </row>
-    <row r="14" spans="1:20" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T13" s="60"/>
+      <c r="U13" s="59"/>
+    </row>
+    <row r="14" spans="1:21" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51">
         <v>13</v>
       </c>
       <c r="B14" s="64" t="s">
         <v>2200</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="C14" s="87" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G14" s="63" t="s">
         <v>2199</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="H14" s="48" t="s">
         <v>2198</v>
       </c>
-      <c r="H14" s="62" t="s">
+      <c r="I14" s="62" t="s">
         <v>2197</v>
       </c>
-      <c r="I14" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J14" s="60"/>
+      <c r="J14" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K14" s="60"/>
       <c r="L14" s="60"/>
       <c r="M14" s="60"/>
@@ -33677,34 +33742,37 @@
       <c r="Q14" s="60"/>
       <c r="R14" s="60"/>
       <c r="S14" s="60"/>
-      <c r="T14" s="59"/>
-    </row>
-    <row r="15" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T14" s="60"/>
+      <c r="U14" s="59"/>
+    </row>
+    <row r="15" spans="1:21" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51">
         <v>14</v>
       </c>
       <c r="B15" s="64" t="s">
         <v>2196</v>
       </c>
+      <c r="C15" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D15" t="s">
         <v>599</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>604</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="G15" s="63" t="s">
         <v>2156</v>
       </c>
-      <c r="G15" s="48" t="s">
+      <c r="H15" s="48" t="s">
         <v>2195</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="I15" s="62" t="s">
         <v>2194</v>
       </c>
-      <c r="I15" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J15" s="60"/>
+      <c r="J15" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K15" s="60"/>
       <c r="L15" s="60"/>
       <c r="M15" s="60"/>
@@ -33714,34 +33782,38 @@
       <c r="Q15" s="60"/>
       <c r="R15" s="60"/>
       <c r="S15" s="60"/>
-      <c r="T15" s="59"/>
-    </row>
-    <row r="16" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T15" s="60"/>
+      <c r="U15" s="59"/>
+    </row>
+    <row r="16" spans="1:21" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="51">
         <v>15</v>
       </c>
       <c r="B16" s="64" t="s">
         <v>2193</v>
       </c>
+      <c r="C16" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D16" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="88"/>
+      <c r="F16" t="s">
         <v>612</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="G16" s="63" t="s">
         <v>2192</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="H16" s="48" t="s">
         <v>2191</v>
       </c>
-      <c r="H16" s="62" t="s">
+      <c r="I16" s="62" t="s">
         <v>2190</v>
       </c>
-      <c r="I16" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J16" s="60"/>
+      <c r="J16" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K16" s="60"/>
       <c r="L16" s="60"/>
       <c r="M16" s="60"/>
@@ -33751,31 +33823,31 @@
       <c r="Q16" s="60"/>
       <c r="R16" s="60"/>
       <c r="S16" s="60"/>
-      <c r="T16" s="59"/>
-    </row>
-    <row r="17" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T16" s="60"/>
+      <c r="U16" s="59"/>
+    </row>
+    <row r="17" spans="1:21" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="51">
         <v>16</v>
       </c>
       <c r="B17" s="64" t="s">
         <v>2189</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>598</v>
       </c>
-      <c r="F17" s="63" t="s">
+      <c r="G17" s="63" t="s">
         <v>2188</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="H17" s="48" t="s">
         <v>2187</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="I17" s="62" t="s">
         <v>2186</v>
       </c>
-      <c r="I17" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J17" s="60"/>
+      <c r="J17" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K17" s="60"/>
       <c r="L17" s="60"/>
       <c r="M17" s="60"/>
@@ -33785,28 +33857,31 @@
       <c r="Q17" s="60"/>
       <c r="R17" s="60"/>
       <c r="S17" s="60"/>
-      <c r="T17" s="59"/>
-    </row>
-    <row r="18" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T17" s="60"/>
+      <c r="U17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="51">
         <v>17</v>
       </c>
       <c r="B18" s="64" t="s">
         <v>2185</v>
       </c>
-      <c r="F18" s="63" t="s">
+      <c r="F18" t="s">
+        <v>612</v>
+      </c>
+      <c r="G18" s="63" t="s">
         <v>2184</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="H18" s="48" t="s">
         <v>2183</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="I18" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="I18" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J18" s="60"/>
+      <c r="J18" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K18" s="60"/>
       <c r="L18" s="60"/>
       <c r="M18" s="60"/>
@@ -33816,28 +33891,31 @@
       <c r="Q18" s="60"/>
       <c r="R18" s="60"/>
       <c r="S18" s="60"/>
-      <c r="T18" s="59"/>
-    </row>
-    <row r="19" spans="1:20" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="60"/>
+      <c r="U18" s="59"/>
+    </row>
+    <row r="19" spans="1:21" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="51">
         <v>18</v>
       </c>
       <c r="B19" s="64" t="s">
         <v>2181</v>
       </c>
-      <c r="F19" s="63" t="s">
+      <c r="F19" t="s">
+        <v>612</v>
+      </c>
+      <c r="G19" s="63" t="s">
         <v>2180</v>
       </c>
-      <c r="G19" s="67" t="s">
+      <c r="H19" s="67" t="s">
         <v>2179</v>
       </c>
-      <c r="H19" s="66" t="s">
+      <c r="I19" s="66" t="s">
         <v>2178</v>
       </c>
-      <c r="I19" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J19" s="60"/>
+      <c r="J19" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K19" s="60"/>
       <c r="L19" s="60"/>
       <c r="M19" s="60"/>
@@ -33847,34 +33925,37 @@
       <c r="Q19" s="60"/>
       <c r="R19" s="60"/>
       <c r="S19" s="60"/>
-      <c r="T19" s="59"/>
-    </row>
-    <row r="20" spans="1:20" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T19" s="60"/>
+      <c r="U19" s="59"/>
+    </row>
+    <row r="20" spans="1:21" ht="53.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="51">
         <v>19</v>
       </c>
       <c r="B20" s="64" t="s">
         <v>2177</v>
       </c>
+      <c r="C20" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D20" t="s">
         <v>599</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>598</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="G20" s="63" t="s">
         <v>2176</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="H20" s="48" t="s">
         <v>2175</v>
       </c>
-      <c r="H20" s="62" t="s">
+      <c r="I20" s="62" t="s">
         <v>2174</v>
       </c>
-      <c r="I20" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J20" s="60"/>
+      <c r="J20" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K20" s="60"/>
       <c r="L20" s="60"/>
       <c r="M20" s="60"/>
@@ -33884,34 +33965,37 @@
       <c r="Q20" s="60"/>
       <c r="R20" s="60"/>
       <c r="S20" s="60"/>
-      <c r="T20" s="59"/>
-    </row>
-    <row r="21" spans="1:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T20" s="60"/>
+      <c r="U20" s="59"/>
+    </row>
+    <row r="21" spans="1:21" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="51">
         <v>20</v>
       </c>
       <c r="B21" s="64" t="s">
         <v>2173</v>
       </c>
+      <c r="C21" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D21" t="s">
         <v>599</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>598</v>
       </c>
-      <c r="F21" s="63" t="s">
+      <c r="G21" s="63" t="s">
         <v>2172</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="H21" s="48" t="s">
         <v>2171</v>
       </c>
-      <c r="H21" s="62" t="s">
+      <c r="I21" s="62" t="s">
         <v>2170</v>
       </c>
-      <c r="I21" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J21" s="60"/>
+      <c r="J21" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K21" s="60"/>
       <c r="L21" s="60"/>
       <c r="M21" s="60"/>
@@ -33921,31 +34005,31 @@
       <c r="Q21" s="60"/>
       <c r="R21" s="60"/>
       <c r="S21" s="60"/>
-      <c r="T21" s="59"/>
-    </row>
-    <row r="22" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T21" s="60"/>
+      <c r="U21" s="59"/>
+    </row>
+    <row r="22" spans="1:21" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="51">
         <v>21</v>
       </c>
       <c r="B22" s="64" t="s">
         <v>2169</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>604</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="G22" s="63" t="s">
         <v>2168</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="H22" s="48" t="s">
         <v>2167</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="I22" s="62" t="s">
         <v>2166</v>
       </c>
-      <c r="I22" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J22" s="60"/>
+      <c r="J22" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K22" s="60"/>
       <c r="L22" s="60"/>
       <c r="M22" s="60"/>
@@ -33955,34 +34039,37 @@
       <c r="Q22" s="60"/>
       <c r="R22" s="60"/>
       <c r="S22" s="60"/>
-      <c r="T22" s="59"/>
-    </row>
-    <row r="23" spans="1:20" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T22" s="60"/>
+      <c r="U22" s="59"/>
+    </row>
+    <row r="23" spans="1:21" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="51">
         <v>22</v>
       </c>
       <c r="B23" s="64" t="s">
         <v>2165</v>
       </c>
+      <c r="C23" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D23" t="s">
         <v>599</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>598</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="G23" s="63" t="s">
         <v>2164</v>
       </c>
-      <c r="G23" s="65" t="s">
+      <c r="H23" s="65" t="s">
         <v>2163</v>
       </c>
-      <c r="H23" s="62" t="s">
+      <c r="I23" s="62" t="s">
         <v>2162</v>
       </c>
-      <c r="I23" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J23" s="60"/>
+      <c r="J23" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K23" s="60"/>
       <c r="L23" s="60"/>
       <c r="M23" s="60"/>
@@ -33992,31 +34079,31 @@
       <c r="Q23" s="60"/>
       <c r="R23" s="60"/>
       <c r="S23" s="60"/>
-      <c r="T23" s="59"/>
-    </row>
-    <row r="24" spans="1:20" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T23" s="60"/>
+      <c r="U23" s="59"/>
+    </row>
+    <row r="24" spans="1:21" ht="57" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="51">
         <v>23</v>
       </c>
       <c r="B24" s="64" t="s">
         <v>2161</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>604</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="G24" s="63" t="s">
         <v>2160</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="H24" s="48" t="s">
         <v>2159</v>
       </c>
-      <c r="H24" s="62" t="s">
+      <c r="I24" s="62" t="s">
         <v>2158</v>
       </c>
-      <c r="I24" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J24" s="60"/>
+      <c r="J24" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K24" s="60"/>
       <c r="L24" s="60"/>
       <c r="M24" s="60"/>
@@ -34026,28 +34113,31 @@
       <c r="Q24" s="60"/>
       <c r="R24" s="60"/>
       <c r="S24" s="60"/>
-      <c r="T24" s="59"/>
-    </row>
-    <row r="25" spans="1:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T24" s="60"/>
+      <c r="U24" s="59"/>
+    </row>
+    <row r="25" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="51">
         <v>24</v>
       </c>
       <c r="B25" s="64" t="s">
         <v>2157</v>
       </c>
-      <c r="F25" s="63" t="s">
+      <c r="F25" t="s">
+        <v>612</v>
+      </c>
+      <c r="G25" s="63" t="s">
         <v>2156</v>
       </c>
-      <c r="G25" s="48" t="s">
+      <c r="H25" s="48" t="s">
         <v>2155</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="I25" s="62" t="s">
         <v>2154</v>
       </c>
-      <c r="I25" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J25" s="60"/>
+      <c r="J25" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K25" s="60"/>
       <c r="L25" s="60"/>
       <c r="M25" s="60"/>
@@ -34057,34 +34147,37 @@
       <c r="Q25" s="60"/>
       <c r="R25" s="60"/>
       <c r="S25" s="60"/>
-      <c r="T25" s="59"/>
-    </row>
-    <row r="26" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T25" s="60"/>
+      <c r="U25" s="59"/>
+    </row>
+    <row r="26" spans="1:21" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="51">
         <v>25</v>
       </c>
       <c r="B26" s="64" t="s">
         <v>2153</v>
       </c>
+      <c r="C26" s="6" t="s">
+        <v>1106</v>
+      </c>
       <c r="D26" t="s">
         <v>599</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>604</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="G26" s="63" t="s">
         <v>2152</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="H26" s="48" t="s">
         <v>2151</v>
       </c>
-      <c r="H26" s="62" t="s">
+      <c r="I26" s="62" t="s">
         <v>2150</v>
       </c>
-      <c r="I26" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="J26" s="60"/>
+      <c r="J26" s="61" t="s">
+        <v>693</v>
+      </c>
       <c r="K26" s="60"/>
       <c r="L26" s="60"/>
       <c r="M26" s="60"/>
@@ -34094,24 +34187,27 @@
       <c r="Q26" s="60"/>
       <c r="R26" s="60"/>
       <c r="S26" s="60"/>
-      <c r="T26" s="59"/>
-    </row>
-    <row r="27" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T26" s="60"/>
+      <c r="U26" s="59"/>
+    </row>
+    <row r="27" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="51">
         <v>26</v>
       </c>
       <c r="B27" s="58"/>
-      <c r="F27" s="57" t="s">
+      <c r="F27" t="s">
+        <v>598</v>
+      </c>
+      <c r="G27" s="57" t="s">
         <v>2149</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="H27" s="48" t="s">
         <v>2148</v>
       </c>
-      <c r="H27" s="56" t="s">
+      <c r="I27" s="56" t="s">
         <v>2147</v>
       </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="54"/>
+      <c r="J27" s="55"/>
       <c r="K27" s="54"/>
       <c r="L27" s="54"/>
       <c r="M27" s="54"/>
@@ -34121,26 +34217,29 @@
       <c r="Q27" s="54"/>
       <c r="R27" s="54"/>
       <c r="S27" s="54"/>
-      <c r="T27" s="53"/>
-    </row>
-    <row r="28" spans="1:20" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T27" s="54"/>
+      <c r="U27" s="53"/>
+    </row>
+    <row r="28" spans="1:21" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="51">
         <v>27</v>
       </c>
       <c r="B28" s="50" t="s">
         <v>2146</v>
       </c>
-      <c r="F28" s="49" t="s">
+      <c r="F28" t="s">
+        <v>604</v>
+      </c>
+      <c r="G28" s="49" t="s">
         <v>2145</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="H28" s="48" t="s">
         <v>2144</v>
       </c>
-      <c r="H28" s="52"/>
-      <c r="I28" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J28" s="45"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K28" s="45"/>
       <c r="L28" s="45"/>
       <c r="M28" s="45"/>
@@ -34150,28 +34249,31 @@
       <c r="Q28" s="45"/>
       <c r="R28" s="45"/>
       <c r="S28" s="45"/>
-      <c r="T28" s="44"/>
-    </row>
-    <row r="29" spans="1:20" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T28" s="45"/>
+      <c r="U28" s="44"/>
+    </row>
+    <row r="29" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="51">
         <v>28</v>
       </c>
       <c r="B29" s="50" t="s">
         <v>2143</v>
       </c>
-      <c r="F29" s="49" t="s">
+      <c r="F29" t="s">
+        <v>604</v>
+      </c>
+      <c r="G29" s="49" t="s">
         <v>2142</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="H29" s="48" t="s">
         <v>2141</v>
       </c>
-      <c r="H29" s="47" t="s">
+      <c r="I29" s="47" t="s">
         <v>2140</v>
       </c>
-      <c r="I29" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J29" s="45"/>
+      <c r="J29" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
       <c r="M29" s="45"/>
@@ -34181,28 +34283,31 @@
       <c r="Q29" s="45"/>
       <c r="R29" s="45"/>
       <c r="S29" s="45"/>
-      <c r="T29" s="44"/>
-    </row>
-    <row r="30" spans="1:20" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T29" s="45"/>
+      <c r="U29" s="44"/>
+    </row>
+    <row r="30" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="51">
         <v>29</v>
       </c>
       <c r="B30" s="50" t="s">
         <v>2139</v>
       </c>
-      <c r="F30" s="49" t="s">
+      <c r="F30" t="s">
+        <v>604</v>
+      </c>
+      <c r="G30" s="49" t="s">
         <v>2138</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="H30" s="48" t="s">
         <v>2137</v>
       </c>
-      <c r="H30" s="47" t="s">
+      <c r="I30" s="47" t="s">
         <v>2136</v>
       </c>
-      <c r="I30" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J30" s="45"/>
+      <c r="J30" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
       <c r="M30" s="45"/>
@@ -34212,28 +34317,31 @@
       <c r="Q30" s="45"/>
       <c r="R30" s="45"/>
       <c r="S30" s="45"/>
-      <c r="T30" s="44"/>
-    </row>
-    <row r="31" spans="1:20" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T30" s="45"/>
+      <c r="U30" s="44"/>
+    </row>
+    <row r="31" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="51">
         <v>30</v>
       </c>
       <c r="B31" s="50" t="s">
         <v>2135</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F31" t="s">
+        <v>598</v>
+      </c>
+      <c r="G31" s="49" t="s">
         <v>2134</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="H31" s="48" t="s">
         <v>2133</v>
       </c>
-      <c r="H31" s="47" t="s">
+      <c r="I31" s="47" t="s">
         <v>2132</v>
       </c>
-      <c r="I31" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J31" s="45"/>
+      <c r="J31" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
       <c r="M31" s="45"/>
@@ -34243,34 +34351,38 @@
       <c r="Q31" s="45"/>
       <c r="R31" s="45"/>
       <c r="S31" s="45"/>
-      <c r="T31" s="44"/>
-    </row>
-    <row r="32" spans="1:20" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T31" s="45"/>
+      <c r="U31" s="44"/>
+    </row>
+    <row r="32" spans="1:21" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="51">
         <v>31</v>
       </c>
       <c r="B32" s="50" t="s">
         <v>2129</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D32" s="85" t="s">
         <v>599</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="85"/>
+      <c r="F32" t="s">
         <v>604</v>
       </c>
-      <c r="F32" s="49" t="s">
+      <c r="G32" s="49" t="s">
         <v>2131</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="H32" s="48" t="s">
         <v>2130</v>
       </c>
-      <c r="H32" s="47" t="s">
+      <c r="I32" s="47" t="s">
         <v>2126</v>
       </c>
-      <c r="I32" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J32" s="45"/>
+      <c r="J32" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K32" s="45"/>
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
@@ -34280,34 +34392,38 @@
       <c r="Q32" s="45"/>
       <c r="R32" s="45"/>
       <c r="S32" s="45"/>
-      <c r="T32" s="44"/>
-    </row>
-    <row r="33" spans="1:20" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T32" s="45"/>
+      <c r="U32" s="44"/>
+    </row>
+    <row r="33" spans="1:21" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="51">
         <v>32</v>
       </c>
       <c r="B33" s="50" t="s">
         <v>2129</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D33" s="86" t="s">
         <v>599</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="89"/>
+      <c r="F33" t="s">
         <v>612</v>
       </c>
-      <c r="F33" s="49" t="s">
+      <c r="G33" s="49" t="s">
         <v>2128</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="H33" s="48" t="s">
         <v>2127</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="I33" s="47" t="s">
         <v>2126</v>
       </c>
-      <c r="I33" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="J33" s="45"/>
+      <c r="J33" s="46" t="s">
+        <v>693</v>
+      </c>
       <c r="K33" s="45"/>
       <c r="L33" s="45"/>
       <c r="M33" s="45"/>
@@ -34317,9 +34433,23 @@
       <c r="Q33" s="45"/>
       <c r="R33" s="45"/>
       <c r="S33" s="45"/>
-      <c r="T33" s="44"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="44"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U33">
+    <filterColumn colId="2">
+      <filters blank="1">
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update new test case in xmls
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BVT!$A$1:$J$127</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$A$1:$U$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EPG!$A$1:$V$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mini_EPG!$A$1:$J$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Regression!$A$1:$P$442</definedName>
   </definedNames>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5375" uniqueCount="2235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5391" uniqueCount="2236">
   <si>
     <t>Name</t>
   </si>
@@ -11405,6 +11405,9 @@
   </si>
   <si>
     <t>Coverd In Regression</t>
+  </si>
+  <si>
+    <t>Sprint-28Aug-1 Sep</t>
   </si>
 </sst>
 </file>
@@ -11509,7 +11512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -11567,243 +11570,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11916,59 +11688,12 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -11976,13 +11701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11991,56 +11710,29 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12278,13 +11970,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>509060</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>328085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>3427943</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>766235</xdr:rowOff>
@@ -12353,7 +12045,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>448734</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>769407</xdr:rowOff>
@@ -17253,7 +16945,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G132" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
@@ -33163,28 +32855,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="43"/>
-    <col min="3" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="73.44140625" customWidth="1"/>
-    <col min="8" max="8" width="91" style="42" customWidth="1"/>
-    <col min="9" max="9" width="65.6640625" style="42" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="7" width="16.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="73.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="91" style="57" customWidth="1"/>
+    <col min="10" max="10" width="65.6640625" style="57" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:22" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2233</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="53" t="s">
         <v>417</v>
       </c>
       <c r="C1" s="41" t="s">
@@ -33194,59 +32887,62 @@
         <v>2077</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>2234</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>2084</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="J1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="K1" s="35" t="s">
         <v>2082</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="L1" s="35" t="s">
         <v>2081</v>
       </c>
-      <c r="L1" s="79" t="s">
+      <c r="M1" s="35" t="s">
         <v>2080</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="N1" s="54" t="s">
         <v>2079</v>
       </c>
-      <c r="N1" s="80" t="s">
+      <c r="O1" s="54" t="s">
         <v>2078</v>
       </c>
-      <c r="O1" s="79" t="s">
+      <c r="P1" s="35" t="s">
         <v>2232</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="Q1" s="35" t="s">
         <v>2231</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="R1" s="35" t="s">
         <v>2230</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="S1" s="35" t="s">
         <v>2229</v>
       </c>
-      <c r="S1" s="79" t="s">
+      <c r="T1" s="35" t="s">
         <v>490</v>
       </c>
-      <c r="T1" s="79" t="s">
+      <c r="U1" s="35" t="s">
         <v>2228</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="V1" s="35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="111.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51">
+    <row r="2" spans="1:22" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -33258,36 +32954,28 @@
       <c r="D2" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="G2" s="77" t="s">
+      <c r="H2" s="8" t="s">
         <v>2101</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="I2" s="51" t="s">
         <v>2227</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="J2" s="51" t="s">
         <v>2226</v>
       </c>
-      <c r="J2" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="73"/>
-    </row>
-    <row r="3" spans="1:21" ht="121.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51">
+      <c r="K2" s="29" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -33299,36 +32987,28 @@
       <c r="D3" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="H3" s="8" t="s">
         <v>2099</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="I3" s="51" t="s">
         <v>2225</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="J3" s="51" t="s">
         <v>2224</v>
       </c>
-      <c r="J3" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="73"/>
-    </row>
-    <row r="4" spans="1:21" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51">
+      <c r="K3" s="29" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -33340,36 +33020,28 @@
       <c r="D4" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="H4" s="8" t="s">
         <v>2097</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="I4" s="51" t="s">
         <v>2223</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="J4" s="51" t="s">
         <v>2222</v>
       </c>
-      <c r="J4" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="73"/>
-    </row>
-    <row r="5" spans="1:21" ht="229.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51">
+      <c r="K4" s="29" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="229.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -33381,36 +33053,28 @@
       <c r="D5" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="G5" s="76" t="s">
+      <c r="H5" s="6" t="s">
         <v>2095</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="I5" s="51" t="s">
         <v>2221</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="J5" s="51" t="s">
         <v>2220</v>
       </c>
-      <c r="J5" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="73"/>
-    </row>
-    <row r="6" spans="1:21" ht="141" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51">
+      <c r="K5" s="29" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -33422,34 +33086,25 @@
       <c r="D6" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="G6" s="76" t="s">
+      <c r="H6" s="6" t="s">
         <v>2093</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="I6" s="51" t="s">
         <v>2219</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="J6" s="51" t="s">
         <v>2218</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="73"/>
-    </row>
-    <row r="7" spans="1:21" ht="192.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51">
+    </row>
+    <row r="7" spans="1:22" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -33461,34 +33116,25 @@
       <c r="D7" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="H7" s="6" t="s">
         <v>2091</v>
       </c>
-      <c r="H7" s="75" t="s">
+      <c r="I7" s="51" t="s">
         <v>2217</v>
       </c>
-      <c r="I7" s="74" t="s">
+      <c r="J7" s="51" t="s">
         <v>2216</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="73"/>
-    </row>
-    <row r="8" spans="1:21" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51">
+    </row>
+    <row r="8" spans="1:22" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -33497,36 +33143,25 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="G8" s="76" t="s">
+      <c r="H8" s="6" t="s">
         <v>2089</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="I8" s="51" t="s">
         <v>2215</v>
       </c>
-      <c r="I8" s="74" t="s">
+      <c r="J8" s="51" t="s">
         <v>2214</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="73"/>
-    </row>
-    <row r="9" spans="1:21" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51">
+    </row>
+    <row r="9" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="45" t="s">
         <v>2213</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -33535,35 +33170,36 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="72" t="s">
+      <c r="I9" s="50" t="s">
         <v>279</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="J9" s="48" t="s">
         <v>898</v>
       </c>
-      <c r="J9" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="59"/>
-    </row>
-    <row r="10" spans="1:21" ht="130.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51">
+      <c r="K9" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+    </row>
+    <row r="10" spans="1:22" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="45" t="s">
         <v>2212</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -33572,35 +33208,36 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="69" t="s">
+      <c r="I10" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="I10" s="71" t="s">
+      <c r="J10" s="48" t="s">
         <v>2211</v>
       </c>
-      <c r="J10" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="59"/>
-    </row>
-    <row r="11" spans="1:21" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51">
+      <c r="K10" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+    </row>
+    <row r="11" spans="1:22" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="45" t="s">
         <v>2210</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -33609,72 +33246,73 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="70" t="s">
+      <c r="I11" s="49" t="s">
         <v>2209</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="J11" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="J11" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="59"/>
-    </row>
-    <row r="12" spans="1:21" ht="88.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51">
+      <c r="K11" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+    </row>
+    <row r="12" spans="1:22" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="45" t="s">
         <v>2208</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="55" t="s">
         <v>1106</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="1" t="s">
         <v>1106</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="H12" s="45" t="s">
         <v>2207</v>
       </c>
-      <c r="H12" s="69" t="s">
+      <c r="I12" s="48" t="s">
         <v>2206</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="J12" s="49" t="s">
         <v>2205</v>
       </c>
-      <c r="J12" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="59"/>
-    </row>
-    <row r="13" spans="1:21" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51">
+      <c r="K12" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+    </row>
+    <row r="13" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="45" t="s">
         <v>2204</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -33683,113 +33321,119 @@
       <c r="D13" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" t="s">
+      <c r="E13" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G13" s="63" t="s">
+      <c r="H13" s="45" t="s">
         <v>2203</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="I13" s="42" t="s">
         <v>2202</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="J13" s="49" t="s">
         <v>2201</v>
       </c>
-      <c r="J13" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="59"/>
-    </row>
-    <row r="14" spans="1:21" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51">
+      <c r="K13" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+    </row>
+    <row r="14" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="45" t="s">
         <v>2200</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="55" t="s">
         <v>1215</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="H14" s="45" t="s">
         <v>2199</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="I14" s="42" t="s">
         <v>2198</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="J14" s="42" t="s">
         <v>2197</v>
       </c>
-      <c r="J14" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="60"/>
-      <c r="U14" s="59"/>
-    </row>
-    <row r="15" spans="1:21" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51">
+      <c r="K14" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+    </row>
+    <row r="15" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="45" t="s">
         <v>2196</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G15" s="63" t="s">
+      <c r="H15" s="45" t="s">
         <v>2156</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="I15" s="42" t="s">
         <v>2195</v>
       </c>
-      <c r="I15" s="62" t="s">
+      <c r="J15" s="42" t="s">
         <v>2194</v>
       </c>
-      <c r="J15" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="59"/>
-    </row>
-    <row r="16" spans="1:21" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51">
+      <c r="K15" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+    </row>
+    <row r="16" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="45" t="s">
         <v>2193</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -33798,658 +33442,666 @@
       <c r="D16" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E16" s="88"/>
-      <c r="F16" t="s">
+      <c r="E16" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G16" s="63" t="s">
+      <c r="H16" s="45" t="s">
         <v>2192</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="I16" s="42" t="s">
         <v>2191</v>
       </c>
-      <c r="I16" s="62" t="s">
+      <c r="J16" s="42" t="s">
         <v>2190</v>
       </c>
-      <c r="J16" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="59"/>
-    </row>
-    <row r="17" spans="1:21" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51">
+      <c r="K16" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="43"/>
+    </row>
+    <row r="17" spans="1:22" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="45" t="s">
         <v>2189</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G17" s="63" t="s">
+      <c r="H17" s="45" t="s">
         <v>2188</v>
       </c>
-      <c r="H17" s="48" t="s">
+      <c r="I17" s="42" t="s">
         <v>2187</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="J17" s="42" t="s">
         <v>2186</v>
       </c>
-      <c r="J17" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="60"/>
-      <c r="U17" s="59"/>
-    </row>
-    <row r="18" spans="1:21" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51">
+      <c r="K17" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+    </row>
+    <row r="18" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="45" t="s">
         <v>2185</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G18" s="63" t="s">
+      <c r="H18" s="45" t="s">
         <v>2184</v>
       </c>
-      <c r="H18" s="48" t="s">
+      <c r="I18" s="42" t="s">
         <v>2183</v>
       </c>
-      <c r="I18" s="62" t="s">
+      <c r="J18" s="42" t="s">
         <v>2182</v>
       </c>
-      <c r="J18" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="59"/>
-    </row>
-    <row r="19" spans="1:21" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51">
+      <c r="K18" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+      <c r="U18" s="43"/>
+      <c r="V18" s="43"/>
+    </row>
+    <row r="19" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="45" t="s">
         <v>2181</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G19" s="63" t="s">
+      <c r="H19" s="45" t="s">
         <v>2180</v>
       </c>
-      <c r="H19" s="67" t="s">
+      <c r="I19" s="47" t="s">
         <v>2179</v>
       </c>
-      <c r="I19" s="66" t="s">
+      <c r="J19" s="47" t="s">
         <v>2178</v>
       </c>
-      <c r="J19" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="60"/>
-      <c r="U19" s="59"/>
-    </row>
-    <row r="20" spans="1:21" ht="53.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51">
+      <c r="K19" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
+    </row>
+    <row r="20" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="45" t="s">
         <v>2177</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="H20" s="45" t="s">
         <v>2176</v>
       </c>
-      <c r="H20" s="48" t="s">
+      <c r="I20" s="42" t="s">
         <v>2175</v>
       </c>
-      <c r="I20" s="62" t="s">
+      <c r="J20" s="42" t="s">
         <v>2174</v>
       </c>
-      <c r="J20" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="59"/>
-    </row>
-    <row r="21" spans="1:21" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51">
+      <c r="K20" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
+    </row>
+    <row r="21" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="45" t="s">
         <v>2173</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="H21" s="45" t="s">
         <v>2172</v>
       </c>
-      <c r="H21" s="48" t="s">
+      <c r="I21" s="42" t="s">
         <v>2171</v>
       </c>
-      <c r="I21" s="62" t="s">
+      <c r="J21" s="42" t="s">
         <v>2170</v>
       </c>
-      <c r="J21" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="60"/>
-      <c r="U21" s="59"/>
-    </row>
-    <row r="22" spans="1:21" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51">
+      <c r="K21" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+    </row>
+    <row r="22" spans="1:22" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="45" t="s">
         <v>2169</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="H22" s="45" t="s">
         <v>2168</v>
       </c>
-      <c r="H22" s="48" t="s">
+      <c r="I22" s="42" t="s">
         <v>2167</v>
       </c>
-      <c r="I22" s="62" t="s">
+      <c r="J22" s="42" t="s">
         <v>2166</v>
       </c>
-      <c r="J22" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="60"/>
-      <c r="T22" s="60"/>
-      <c r="U22" s="59"/>
-    </row>
-    <row r="23" spans="1:21" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="51">
+      <c r="K22" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+    </row>
+    <row r="23" spans="1:22" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="45" t="s">
         <v>2165</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="H23" s="45" t="s">
         <v>2164</v>
       </c>
-      <c r="H23" s="65" t="s">
+      <c r="I23" s="46" t="s">
         <v>2163</v>
       </c>
-      <c r="I23" s="62" t="s">
+      <c r="J23" s="42" t="s">
         <v>2162</v>
       </c>
-      <c r="J23" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="59"/>
-    </row>
-    <row r="24" spans="1:21" ht="57" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51">
+      <c r="K23" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+    </row>
+    <row r="24" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="45" t="s">
         <v>2161</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="H24" s="45" t="s">
         <v>2160</v>
       </c>
-      <c r="H24" s="48" t="s">
+      <c r="I24" s="42" t="s">
         <v>2159</v>
       </c>
-      <c r="I24" s="62" t="s">
+      <c r="J24" s="42" t="s">
         <v>2158</v>
       </c>
-      <c r="J24" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="59"/>
-    </row>
-    <row r="25" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51">
+      <c r="K24" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="43"/>
+    </row>
+    <row r="25" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="45" t="s">
         <v>2157</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G25" s="63" t="s">
+      <c r="H25" s="45" t="s">
         <v>2156</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="I25" s="42" t="s">
         <v>2155</v>
       </c>
-      <c r="I25" s="62" t="s">
+      <c r="J25" s="42" t="s">
         <v>2154</v>
       </c>
-      <c r="J25" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="59"/>
-    </row>
-    <row r="26" spans="1:21" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="51">
+      <c r="K25" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="43"/>
+    </row>
+    <row r="26" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="45" t="s">
         <v>2153</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G26" s="63" t="s">
+      <c r="H26" s="45" t="s">
         <v>2152</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="I26" s="42" t="s">
         <v>2151</v>
       </c>
-      <c r="I26" s="62" t="s">
+      <c r="J26" s="42" t="s">
         <v>2150</v>
       </c>
-      <c r="J26" s="61" t="s">
-        <v>693</v>
-      </c>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="59"/>
-    </row>
-    <row r="27" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51">
+      <c r="K26" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+    </row>
+    <row r="27" spans="1:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="F27" t="s">
+      <c r="B27" s="45"/>
+      <c r="G27" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G27" s="57" t="s">
+      <c r="H27" s="45" t="s">
         <v>2149</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="I27" s="42" t="s">
         <v>2148</v>
       </c>
-      <c r="I27" s="56" t="s">
+      <c r="J27" s="42" t="s">
         <v>2147</v>
       </c>
-      <c r="J27" s="55"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="54"/>
-      <c r="S27" s="54"/>
-      <c r="T27" s="54"/>
-      <c r="U27" s="53"/>
-    </row>
-    <row r="28" spans="1:21" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="51">
+      <c r="K27" s="44"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+    </row>
+    <row r="28" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="45" t="s">
         <v>2146</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G28" s="49" t="s">
+      <c r="H28" s="45" t="s">
         <v>2145</v>
       </c>
-      <c r="H28" s="48" t="s">
+      <c r="I28" s="42" t="s">
         <v>2144</v>
       </c>
-      <c r="I28" s="52"/>
-      <c r="J28" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="44"/>
-    </row>
-    <row r="29" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="51">
+      <c r="J28" s="56"/>
+      <c r="K28" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
+    </row>
+    <row r="29" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="45" t="s">
         <v>2143</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G29" s="49" t="s">
+      <c r="H29" s="45" t="s">
         <v>2142</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="I29" s="42" t="s">
         <v>2141</v>
       </c>
-      <c r="I29" s="47" t="s">
+      <c r="J29" s="42" t="s">
         <v>2140</v>
       </c>
-      <c r="J29" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="44"/>
-    </row>
-    <row r="30" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="51">
+      <c r="K29" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
+      <c r="U29" s="43"/>
+      <c r="V29" s="43"/>
+    </row>
+    <row r="30" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="45" t="s">
         <v>2139</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G30" s="49" t="s">
+      <c r="H30" s="45" t="s">
         <v>2138</v>
       </c>
-      <c r="H30" s="48" t="s">
+      <c r="I30" s="42" t="s">
         <v>2137</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="J30" s="42" t="s">
         <v>2136</v>
       </c>
-      <c r="J30" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="44"/>
-    </row>
-    <row r="31" spans="1:21" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="51">
+      <c r="K30" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+      <c r="U30" s="43"/>
+      <c r="V30" s="43"/>
+    </row>
+    <row r="31" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="45" t="s">
         <v>2135</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="H31" s="45" t="s">
         <v>2134</v>
       </c>
-      <c r="H31" s="48" t="s">
+      <c r="I31" s="42" t="s">
         <v>2133</v>
       </c>
-      <c r="I31" s="47" t="s">
+      <c r="J31" s="42" t="s">
         <v>2132</v>
       </c>
-      <c r="J31" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="45"/>
-      <c r="U31" s="44"/>
-    </row>
-    <row r="32" spans="1:21" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="51">
+      <c r="K31" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+      <c r="U31" s="43"/>
+      <c r="V31" s="43"/>
+    </row>
+    <row r="32" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="45" t="s">
         <v>2129</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D32" s="85" t="s">
+      <c r="D32" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E32" s="85"/>
-      <c r="F32" t="s">
+      <c r="E32" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F32" s="52"/>
+      <c r="G32" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G32" s="49" t="s">
+      <c r="H32" s="45" t="s">
         <v>2131</v>
       </c>
-      <c r="H32" s="48" t="s">
+      <c r="I32" s="42" t="s">
         <v>2130</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="J32" s="42" t="s">
         <v>2126</v>
       </c>
-      <c r="J32" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="44"/>
-    </row>
-    <row r="33" spans="1:21" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="51">
+      <c r="K32" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+    </row>
+    <row r="33" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="45" t="s">
         <v>2129</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>1106</v>
       </c>
-      <c r="D33" s="86" t="s">
+      <c r="D33" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E33" s="89"/>
-      <c r="F33" t="s">
+      <c r="E33" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F33" s="52"/>
+      <c r="G33" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="H33" s="45" t="s">
         <v>2128</v>
       </c>
-      <c r="H33" s="48" t="s">
+      <c r="I33" s="42" t="s">
         <v>2127</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="J33" s="42" t="s">
         <v>2126</v>
       </c>
-      <c r="J33" s="46" t="s">
-        <v>693</v>
-      </c>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="44"/>
+      <c r="K33" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="43"/>
+      <c r="V33" s="43"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U33">
-    <filterColumn colId="2">
-      <filters blank="1">
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit Rahul Test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Desktop\Rahul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="2239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5425" uniqueCount="2240">
   <si>
     <t>Name</t>
   </si>
@@ -11422,7 +11422,10 @@
 </t>
   </si>
   <si>
-    <t>Done</t>
+    <t>Feature not yet implemented</t>
+  </si>
+  <si>
+    <t>Sprint-1 Sep-8 Sep</t>
   </si>
 </sst>
 </file>
@@ -11590,7 +11593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11750,7 +11753,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16962,10 +16964,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="140" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B169" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22149,7 +22149,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>208</v>
       </c>
@@ -22186,7 +22186,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>209</v>
       </c>
@@ -22831,12 +22831,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>235</v>
       </c>
       <c r="B159" s="21" t="s">
         <v>1547</v>
+      </c>
+      <c r="C159" t="s">
+        <v>496</v>
+      </c>
+      <c r="D159" t="s">
+        <v>2239</v>
       </c>
       <c r="F159" s="18" t="s">
         <v>1106</v>
@@ -23047,7 +23053,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>241</v>
       </c>
@@ -23193,12 +23199,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>245</v>
       </c>
       <c r="B169" s="21" t="s">
         <v>1512</v>
+      </c>
+      <c r="C169" t="s">
+        <v>496</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>2239</v>
       </c>
       <c r="F169" s="21" t="s">
         <v>1106</v>
@@ -23306,10 +23318,10 @@
         <v>1500</v>
       </c>
       <c r="C172" t="s">
-        <v>2238</v>
-      </c>
-      <c r="D172" s="58">
-        <v>42986</v>
+        <v>496</v>
+      </c>
+      <c r="D172" s="58" t="s">
+        <v>2239</v>
       </c>
       <c r="F172" s="18" t="s">
         <v>1106</v>
@@ -23446,7 +23458,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>252</v>
       </c>
@@ -23670,10 +23682,10 @@
         <v>1492</v>
       </c>
       <c r="C182" t="s">
-        <v>2238</v>
-      </c>
-      <c r="D182" s="59">
-        <v>42986</v>
+        <v>496</v>
+      </c>
+      <c r="D182" s="58" t="s">
+        <v>2239</v>
       </c>
       <c r="F182" s="18" t="s">
         <v>1106</v>
@@ -26379,7 +26391,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>354</v>
       </c>
@@ -26449,7 +26461,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>356</v>
       </c>
@@ -26624,7 +26636,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>364</v>
       </c>
@@ -27410,10 +27422,10 @@
         <v>1156</v>
       </c>
       <c r="C289" t="s">
-        <v>2238</v>
-      </c>
-      <c r="D289" s="58">
-        <v>42986</v>
+        <v>496</v>
+      </c>
+      <c r="D289" s="58" t="s">
+        <v>2239</v>
       </c>
       <c r="F289" s="18" t="s">
         <v>1106</v>
@@ -27443,7 +27455,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>389</v>
       </c>
@@ -27478,7 +27490,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>390</v>
       </c>
@@ -27513,7 +27525,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>391</v>
       </c>
@@ -27548,7 +27560,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>392</v>
       </c>
@@ -27583,7 +27595,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>393</v>
       </c>
@@ -27700,7 +27712,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>396</v>
       </c>
@@ -27776,7 +27788,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="299" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>398</v>
       </c>
@@ -27811,7 +27823,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>399</v>
       </c>
@@ -27846,7 +27858,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="301" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>400</v>
       </c>
@@ -31071,20 +31083,26 @@
         <v>691</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>509</v>
       </c>
       <c r="B392" s="21" t="s">
         <v>839</v>
       </c>
-      <c r="C392" s="28"/>
-      <c r="D392" s="28"/>
+      <c r="C392" s="28" t="s">
+        <v>496</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>2239</v>
+      </c>
       <c r="F392" s="21" t="s">
         <v>1106</v>
       </c>
       <c r="G392" s="21"/>
-      <c r="H392" s="21"/>
+      <c r="H392" s="21" t="s">
+        <v>612</v>
+      </c>
       <c r="I392" s="21" t="s">
         <v>838</v>
       </c>
@@ -32875,19 +32893,13 @@
   </sheetData>
   <autoFilter ref="A1:P442">
     <filterColumn colId="2">
-      <filters blank="1"/>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="5">
+    <filterColumn colId="3">
       <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Ankit"/>
+        <filter val="Sprint-1 Sep-8 Sep"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -32900,12 +32912,12 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
@@ -33566,7 +33578,7 @@
         <v>2184</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>1106</v>
+        <v>2238</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>612</v>
@@ -33595,7 +33607,7 @@
       <c r="U18" s="43"/>
       <c r="V18" s="43"/>
     </row>
-    <row r="19" spans="1:22" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -33604,6 +33616,12 @@
       </c>
       <c r="C19" s="55" t="s">
         <v>1106</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2239</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>612</v>
@@ -33808,6 +33826,12 @@
       <c r="C24" s="55" t="s">
         <v>1106</v>
       </c>
+      <c r="D24" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>2239</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>604</v>
       </c>
@@ -33835,7 +33859,7 @@
       <c r="U24" s="43"/>
       <c r="V24" s="43"/>
     </row>
-    <row r="25" spans="1:22" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -33844,6 +33868,12 @@
       </c>
       <c r="C25" s="55" t="s">
         <v>1106</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2239</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>612</v>
@@ -33948,7 +33978,7 @@
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
     </row>
-    <row r="28" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -33993,6 +34023,12 @@
       <c r="C29" s="55" t="s">
         <v>1106</v>
       </c>
+      <c r="D29" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>2239</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>604</v>
       </c>
@@ -34020,7 +34056,7 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
     </row>
-    <row r="30" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -34195,6 +34231,7 @@
     <filterColumn colId="6">
       <filters>
         <filter val="Ankit"/>
+        <filter val="Rahul"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
commit Tet case update sheet
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5425" uniqueCount="2240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5437" uniqueCount="2241">
   <si>
     <t>Name</t>
   </si>
@@ -11426,6 +11426,9 @@
   </si>
   <si>
     <t>Sprint-1 Sep-8 Sep</t>
+  </si>
+  <si>
+    <t>Sprint 1-Sep  - 8Sep</t>
   </si>
 </sst>
 </file>
@@ -11593,7 +11596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11752,7 +11755,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16964,8 +16966,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView topLeftCell="B169" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="A444" sqref="A444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22842,7 +22844,7 @@
         <v>496</v>
       </c>
       <c r="D159" t="s">
-        <v>2239</v>
+        <v>2240</v>
       </c>
       <c r="F159" s="18" t="s">
         <v>1106</v>
@@ -23209,8 +23211,8 @@
       <c r="C169" t="s">
         <v>496</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>2239</v>
+      <c r="D169" t="s">
+        <v>2240</v>
       </c>
       <c r="F169" s="21" t="s">
         <v>1106</v>
@@ -23320,8 +23322,8 @@
       <c r="C172" t="s">
         <v>496</v>
       </c>
-      <c r="D172" s="58" t="s">
-        <v>2239</v>
+      <c r="D172" t="s">
+        <v>2240</v>
       </c>
       <c r="F172" s="18" t="s">
         <v>1106</v>
@@ -23684,8 +23686,8 @@
       <c r="C182" t="s">
         <v>496</v>
       </c>
-      <c r="D182" s="58" t="s">
-        <v>2239</v>
+      <c r="D182" t="s">
+        <v>2240</v>
       </c>
       <c r="F182" s="18" t="s">
         <v>1106</v>
@@ -25850,12 +25852,15 @@
         <v>691</v>
       </c>
     </row>
-    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>337</v>
       </c>
       <c r="B245" s="21" t="s">
         <v>1300</v>
+      </c>
+      <c r="D245" t="s">
+        <v>2240</v>
       </c>
       <c r="F245" s="18" t="s">
         <v>1106</v>
@@ -26461,19 +26466,25 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>356</v>
       </c>
       <c r="B262" s="18" t="s">
         <v>1246</v>
       </c>
+      <c r="C262" t="s">
+        <v>496</v>
+      </c>
+      <c r="D262" t="s">
+        <v>2240</v>
+      </c>
       <c r="F262" s="18" t="s">
         <v>1106</v>
       </c>
       <c r="G262" s="18"/>
       <c r="H262" s="18" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="I262" s="18" t="s">
         <v>1245</v>
@@ -27424,8 +27435,8 @@
       <c r="C289" t="s">
         <v>496</v>
       </c>
-      <c r="D289" s="58" t="s">
-        <v>2239</v>
+      <c r="D289" t="s">
+        <v>2240</v>
       </c>
       <c r="F289" s="18" t="s">
         <v>1106</v>
@@ -27560,19 +27571,25 @@
         <v>691</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>392</v>
       </c>
       <c r="B293" s="18" t="s">
         <v>1142</v>
       </c>
+      <c r="C293" t="s">
+        <v>496</v>
+      </c>
+      <c r="D293" t="s">
+        <v>2240</v>
+      </c>
       <c r="F293" s="18" t="s">
         <v>1106</v>
       </c>
       <c r="G293" s="18"/>
       <c r="H293" s="18" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="I293" s="18" t="s">
         <v>1141</v>
@@ -31093,8 +31110,8 @@
       <c r="C392" s="28" t="s">
         <v>496</v>
       </c>
-      <c r="D392" s="1" t="s">
-        <v>2239</v>
+      <c r="D392" t="s">
+        <v>2240</v>
       </c>
       <c r="F392" s="21" t="s">
         <v>1106</v>
@@ -32892,13 +32909,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P442">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
+        <filter val="Sprint 1-Sep  - 8Sep"/>
         <filter val="Sprint-1 Sep-8 Sep"/>
       </filters>
     </filterColumn>
@@ -32912,9 +32925,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32999,7 +33012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="111.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -33098,7 +33111,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="229.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="229.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -33201,7 +33214,9 @@
       <c r="C8" s="55" t="s">
         <v>1106</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>494</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
@@ -33217,7 +33232,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -33255,7 +33270,7 @@
       <c r="U9" s="43"/>
       <c r="V9" s="43"/>
     </row>
-    <row r="10" spans="1:22" ht="130.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -33293,7 +33308,7 @@
       <c r="U10" s="43"/>
       <c r="V10" s="43"/>
     </row>
-    <row r="11" spans="1:22" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -33331,7 +33346,7 @@
       <c r="U11" s="43"/>
       <c r="V11" s="43"/>
     </row>
-    <row r="12" spans="1:22" ht="88.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -33412,7 +33427,7 @@
       <c r="U13" s="43"/>
       <c r="V13" s="43"/>
     </row>
-    <row r="14" spans="1:22" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -33533,7 +33548,7 @@
       <c r="U16" s="43"/>
       <c r="V16" s="43"/>
     </row>
-    <row r="17" spans="1:22" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -33542,6 +33557,12 @@
       </c>
       <c r="C17" s="55" t="s">
         <v>1106</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>2239</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>598</v>
@@ -33570,7 +33591,7 @@
       <c r="U17" s="43"/>
       <c r="V17" s="43"/>
     </row>
-    <row r="18" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -33650,7 +33671,7 @@
       <c r="U19" s="43"/>
       <c r="V19" s="43"/>
     </row>
-    <row r="20" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="53.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -33693,7 +33714,7 @@
       <c r="U20" s="43"/>
       <c r="V20" s="43"/>
     </row>
-    <row r="21" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -33736,7 +33757,7 @@
       <c r="U21" s="43"/>
       <c r="V21" s="43"/>
     </row>
-    <row r="22" spans="1:22" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -33773,7 +33794,7 @@
       <c r="U22" s="43"/>
       <c r="V22" s="43"/>
     </row>
-    <row r="23" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -33945,13 +33966,19 @@
       <c r="U26" s="43"/>
       <c r="V26" s="43"/>
     </row>
-    <row r="27" spans="1:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="43.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="B27" s="45"/>
       <c r="C27" s="55" t="s">
         <v>1106</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>2239</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>598</v>
@@ -33978,7 +34005,7 @@
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
     </row>
-    <row r="28" spans="1:22" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -34056,7 +34083,7 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
     </row>
-    <row r="30" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -34103,6 +34130,12 @@
       <c r="C31" s="55" t="s">
         <v>1106</v>
       </c>
+      <c r="D31" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>494</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>598</v>
       </c>
@@ -34220,15 +34253,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V33">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Pritam"/>
-      </filters>
+    <filterColumn colId="3">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit bug fixes of BVT
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5537" uniqueCount="2241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5540" uniqueCount="2242">
   <si>
     <t>Name</t>
   </si>
@@ -11429,6 +11429,9 @@
   </si>
   <si>
     <t>No(Upsellable functionbality not working )</t>
+  </si>
+  <si>
+    <t>NO(Change sorting category is depend on TM)</t>
   </si>
 </sst>
 </file>
@@ -11596,7 +11599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11755,6 +11758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16966,9 +16970,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K224" sqref="K224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18771,7 +18775,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>92</v>
       </c>
@@ -20817,6 +20821,9 @@
       </c>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
+      <c r="E104" t="s">
+        <v>1206</v>
+      </c>
       <c r="F104" s="18" t="s">
         <v>1106</v>
       </c>
@@ -20919,7 +20926,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>156</v>
       </c>
@@ -20929,7 +20936,7 @@
       <c r="C107" s="27"/>
       <c r="D107" s="27"/>
       <c r="F107" s="18" t="s">
-        <v>1106</v>
+        <v>2241</v>
       </c>
       <c r="G107" s="18"/>
       <c r="H107" s="18" t="s">
@@ -25122,6 +25129,9 @@
       <c r="B222" s="21" t="s">
         <v>516</v>
       </c>
+      <c r="E222" t="s">
+        <v>1206</v>
+      </c>
       <c r="F222" s="21" t="s">
         <v>1106</v>
       </c>
@@ -25157,6 +25167,9 @@
       <c r="B223" s="18" t="s">
         <v>559</v>
       </c>
+      <c r="E223" t="s">
+        <v>1206</v>
+      </c>
       <c r="F223" s="18" t="s">
         <v>1106</v>
       </c>
@@ -25186,37 +25199,40 @@
       </c>
     </row>
     <row r="224" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A224">
+      <c r="A224" s="58">
         <v>313</v>
       </c>
-      <c r="B224" s="21" t="s">
+      <c r="B224" s="4" t="s">
         <v>1365</v>
       </c>
-      <c r="F224" s="21" t="s">
+      <c r="C224" s="58"/>
+      <c r="D224" s="58"/>
+      <c r="E224" s="58"/>
+      <c r="F224" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="G224" s="21"/>
-      <c r="H224" s="21" t="s">
+      <c r="G224" s="4"/>
+      <c r="H224" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="I224" s="21" t="s">
+      <c r="I224" s="4" t="s">
         <v>1364</v>
       </c>
-      <c r="J224" s="21" t="s">
+      <c r="J224" s="4" t="s">
         <v>1363</v>
       </c>
-      <c r="K224" s="21" t="s">
+      <c r="K224" s="4" t="s">
         <v>1362</v>
       </c>
-      <c r="L224" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="M224" s="21" t="s">
-        <v>692</v>
-      </c>
-      <c r="N224" s="29"/>
-      <c r="O224" s="29"/>
-      <c r="P224" s="29" t="s">
+      <c r="L224" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M224" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="N224" s="3"/>
+      <c r="O224" s="3"/>
+      <c r="P224" s="3" t="s">
         <v>691</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create new test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5540" uniqueCount="2242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="2243">
   <si>
     <t>Name</t>
   </si>
@@ -11432,6 +11432,9 @@
   </si>
   <si>
     <t>NO(Change sorting category is depend on TM)</t>
+  </si>
+  <si>
+    <t>Time has been coverded as automation but for date updation is not a part of Automation.</t>
   </si>
 </sst>
 </file>
@@ -12458,8 +12461,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:J127"/>
+    <sheetView topLeftCell="E38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12506,7 +12509,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>418</v>
       </c>
@@ -12536,7 +12539,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>419</v>
       </c>
@@ -12566,7 +12569,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>420</v>
       </c>
@@ -12596,7 +12599,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>421</v>
       </c>
@@ -12626,7 +12629,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>423</v>
       </c>
@@ -12656,7 +12659,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>424</v>
       </c>
@@ -12718,7 +12721,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>426</v>
       </c>
@@ -12750,7 +12753,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>427</v>
       </c>
@@ -12780,7 +12783,7 @@
       </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>428</v>
       </c>
@@ -12838,7 +12841,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>430</v>
       </c>
@@ -12868,7 +12871,7 @@
       </c>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>431</v>
       </c>
@@ -13814,7 +13817,7 @@
       </c>
       <c r="J45" s="17"/>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" s="2" customFormat="1" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>440</v>
       </c>
@@ -13844,7 +13847,7 @@
       </c>
       <c r="J46" s="17"/>
     </row>
-    <row r="47" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="9" t="s">
         <v>496</v>
@@ -13872,7 +13875,7 @@
       </c>
       <c r="J47" s="17"/>
     </row>
-    <row r="48" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="9" t="s">
         <v>496</v>
@@ -13900,7 +13903,7 @@
       </c>
       <c r="J48" s="17"/>
     </row>
-    <row r="49" spans="1:10" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="9" t="s">
         <v>496</v>
@@ -13928,7 +13931,7 @@
       </c>
       <c r="J49" s="17"/>
     </row>
-    <row r="50" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="9" t="s">
         <v>496</v>
@@ -13956,7 +13959,7 @@
       </c>
       <c r="J50" s="17"/>
     </row>
-    <row r="51" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="9" t="s">
         <v>496</v>
@@ -14014,7 +14017,7 @@
       </c>
       <c r="J52" s="17"/>
     </row>
-    <row r="53" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="9" t="s">
         <v>496</v>
@@ -14042,7 +14045,7 @@
       </c>
       <c r="J53" s="17"/>
     </row>
-    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="9" t="s">
         <v>496</v>
@@ -14240,7 +14243,7 @@
       </c>
       <c r="J60" s="17"/>
     </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="93" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>480</v>
       </c>
@@ -14328,7 +14331,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="2" customFormat="1" ht="93" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" s="2" customFormat="1" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>483</v>
       </c>
@@ -14358,7 +14361,7 @@
       </c>
       <c r="J64" s="17"/>
     </row>
-    <row r="65" spans="1:10" s="2" customFormat="1" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" s="2" customFormat="1" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>484</v>
       </c>
@@ -14388,7 +14391,7 @@
       </c>
       <c r="J65" s="17"/>
     </row>
-    <row r="66" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>442</v>
       </c>
@@ -14418,7 +14421,7 @@
       </c>
       <c r="J66" s="17"/>
     </row>
-    <row r="67" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>443</v>
       </c>
@@ -14448,7 +14451,7 @@
       </c>
       <c r="J67" s="17"/>
     </row>
-    <row r="68" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>444</v>
       </c>
@@ -14560,7 +14563,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="9" t="s">
         <v>496</v>
@@ -14590,7 +14593,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="9" t="s">
         <v>496</v>
@@ -14862,7 +14865,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="9" t="s">
         <v>496</v>
@@ -14890,7 +14893,7 @@
       </c>
       <c r="J83" s="17"/>
     </row>
-    <row r="84" spans="1:10" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="9" t="s">
         <v>496</v>
@@ -14918,7 +14921,7 @@
       </c>
       <c r="J84" s="17"/>
     </row>
-    <row r="85" spans="1:10" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="9" t="s">
         <v>496</v>
@@ -14946,7 +14949,7 @@
       </c>
       <c r="J85" s="17"/>
     </row>
-    <row r="86" spans="1:10" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="9" t="s">
         <v>496</v>
@@ -14974,7 +14977,7 @@
       </c>
       <c r="J86" s="17"/>
     </row>
-    <row r="87" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="9" t="s">
         <v>496</v>
@@ -15082,7 +15085,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>451</v>
       </c>
@@ -15170,7 +15173,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>454</v>
       </c>
@@ -15200,7 +15203,7 @@
       </c>
       <c r="J94" s="17"/>
     </row>
-    <row r="95" spans="1:10" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>455</v>
       </c>
@@ -15230,7 +15233,7 @@
       </c>
       <c r="J95" s="17"/>
     </row>
-    <row r="96" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>456</v>
       </c>
@@ -15288,7 +15291,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>458</v>
       </c>
@@ -15484,7 +15487,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="93" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
       <c r="B105" s="9" t="s">
         <v>496</v>
@@ -15510,7 +15513,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" spans="1:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" ht="98.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="9" t="s">
         <v>496</v>
@@ -15534,7 +15537,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="9" t="s">
         <v>496</v>
@@ -15678,7 +15681,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="9" t="s">
         <v>496</v>
@@ -15702,7 +15705,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="9" t="s">
         <v>496</v>
@@ -15743,7 +15746,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="9" t="s">
         <v>496</v>
@@ -15767,7 +15770,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="9" t="s">
         <v>496</v>
@@ -15791,7 +15794,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="9" t="s">
         <v>496</v>
@@ -15983,7 +15986,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="9" t="s">
         <v>496</v>
@@ -16007,7 +16010,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="9" t="s">
         <v>496</v>
@@ -16036,6 +16039,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="Completed"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Ankit"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -16970,9 +16978,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K224" sqref="K224"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K290" sqref="K290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18826,7 +18834,7 @@
       </c>
       <c r="G50" s="21"/>
       <c r="H50" s="21" t="s">
-        <v>604</v>
+        <v>494</v>
       </c>
       <c r="I50" s="21" t="s">
         <v>1932</v>
@@ -20812,7 +20820,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>153</v>
       </c>
@@ -22095,7 +22103,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>205</v>
       </c>
@@ -22135,7 +22143,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>206</v>
       </c>
@@ -22175,7 +22183,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="357" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="357" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>207</v>
       </c>
@@ -22412,7 +22420,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>213</v>
       </c>
@@ -22450,7 +22458,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>214</v>
       </c>
@@ -23559,7 +23567,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>253</v>
       </c>
@@ -23597,7 +23605,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>256</v>
       </c>
@@ -25122,7 +25130,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>311</v>
       </c>
@@ -25160,7 +25168,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>312</v>
       </c>
@@ -26473,37 +26481,40 @@
       </c>
     </row>
     <row r="259" spans="1:16" ht="27" x14ac:dyDescent="0.3">
-      <c r="A259">
+      <c r="A259" s="58">
         <v>352</v>
       </c>
-      <c r="B259" s="18" t="s">
+      <c r="B259" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="F259" s="18" t="s">
+      <c r="C259" s="58"/>
+      <c r="D259" s="58"/>
+      <c r="E259" s="58"/>
+      <c r="F259" s="3" t="s">
         <v>1106</v>
       </c>
-      <c r="G259" s="18"/>
-      <c r="H259" s="18" t="s">
+      <c r="G259" s="3"/>
+      <c r="H259" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="I259" s="18" t="s">
+      <c r="I259" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="J259" s="18" t="s">
+      <c r="J259" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="K259" s="18" t="s">
+      <c r="K259" s="3" t="s">
         <v>1253</v>
       </c>
-      <c r="L259" s="18" t="s">
-        <v>693</v>
-      </c>
-      <c r="M259" s="18" t="s">
-        <v>692</v>
-      </c>
-      <c r="N259" s="18"/>
-      <c r="O259" s="18"/>
-      <c r="P259" s="18" t="s">
+      <c r="L259" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M259" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="N259" s="3"/>
+      <c r="O259" s="3"/>
+      <c r="P259" s="3" t="s">
         <v>691</v>
       </c>
     </row>
@@ -27439,37 +27450,40 @@
       </c>
     </row>
     <row r="286" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
-      <c r="A286">
+      <c r="A286" s="58">
         <v>385</v>
       </c>
-      <c r="B286" s="21" t="s">
+      <c r="B286" s="4" t="s">
         <v>1167</v>
       </c>
-      <c r="F286" s="21" t="s">
+      <c r="C286" s="58"/>
+      <c r="D286" s="58"/>
+      <c r="E286" s="58"/>
+      <c r="F286" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="G286" s="21"/>
-      <c r="H286" s="21" t="s">
+      <c r="G286" s="4"/>
+      <c r="H286" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="I286" s="21" t="s">
+      <c r="I286" s="4" t="s">
         <v>1166</v>
       </c>
-      <c r="J286" s="21" t="s">
+      <c r="J286" s="4" t="s">
         <v>1165</v>
       </c>
-      <c r="K286" s="21" t="s">
+      <c r="K286" s="4" t="s">
         <v>1161</v>
       </c>
-      <c r="L286" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="M286" s="21" t="s">
-        <v>692</v>
-      </c>
-      <c r="N286" s="29"/>
-      <c r="O286" s="29"/>
-      <c r="P286" s="29" t="s">
+      <c r="L286" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M286" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="N286" s="3"/>
+      <c r="O286" s="3"/>
+      <c r="P286" s="3" t="s">
         <v>691</v>
       </c>
     </row>
@@ -27510,37 +27524,40 @@
       </c>
     </row>
     <row r="288" spans="1:16" ht="93" x14ac:dyDescent="0.3">
-      <c r="A288">
+      <c r="A288" s="58">
         <v>387</v>
       </c>
-      <c r="B288" s="21" t="s">
+      <c r="B288" s="4" t="s">
         <v>1160</v>
       </c>
-      <c r="F288" s="21" t="s">
+      <c r="C288" s="58"/>
+      <c r="D288" s="58"/>
+      <c r="E288" s="58"/>
+      <c r="F288" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="G288" s="21"/>
-      <c r="H288" s="21" t="s">
+      <c r="G288" s="4"/>
+      <c r="H288" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="I288" s="21" t="s">
+      <c r="I288" s="4" t="s">
         <v>1159</v>
       </c>
-      <c r="J288" s="21" t="s">
+      <c r="J288" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="K288" s="21" t="s">
+      <c r="K288" s="4" t="s">
         <v>1157</v>
       </c>
-      <c r="L288" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="M288" s="21" t="s">
-        <v>692</v>
-      </c>
-      <c r="N288" s="29"/>
-      <c r="O288" s="29"/>
-      <c r="P288" s="29" t="s">
+      <c r="L288" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M288" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="N288" s="3"/>
+      <c r="O288" s="3"/>
+      <c r="P288" s="3" t="s">
         <v>691</v>
       </c>
     </row>
@@ -27621,37 +27638,42 @@
       </c>
     </row>
     <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A291">
+      <c r="A291" s="58">
         <v>390</v>
       </c>
-      <c r="B291" s="18" t="s">
+      <c r="B291" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="F291" s="18" t="s">
+      <c r="C291" s="58"/>
+      <c r="D291" s="58"/>
+      <c r="E291" s="58"/>
+      <c r="F291" s="3" t="s">
         <v>1106</v>
       </c>
-      <c r="G291" s="18"/>
-      <c r="H291" s="18" t="s">
+      <c r="G291" s="3" t="s">
+        <v>2242</v>
+      </c>
+      <c r="H291" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="I291" s="18" t="s">
+      <c r="I291" s="3" t="s">
         <v>1149</v>
       </c>
-      <c r="J291" s="18" t="s">
+      <c r="J291" s="3" t="s">
         <v>1148</v>
       </c>
-      <c r="K291" s="18" t="s">
+      <c r="K291" s="3" t="s">
         <v>1147</v>
       </c>
-      <c r="L291" s="18" t="s">
-        <v>693</v>
-      </c>
-      <c r="M291" s="18" t="s">
-        <v>692</v>
-      </c>
-      <c r="N291" s="18"/>
-      <c r="O291" s="18"/>
-      <c r="P291" s="18" t="s">
+      <c r="L291" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M291" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="N291" s="3"/>
+      <c r="O291" s="3"/>
+      <c r="P291" s="3" t="s">
         <v>691</v>
       </c>
     </row>
@@ -33129,6 +33151,9 @@
   </sheetData>
   <autoFilter ref="A1:P442">
     <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="4">
       <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="5">

</xml_diff>

<commit_message>
Creation of Test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="2243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5546" uniqueCount="2244">
   <si>
     <t>Name</t>
   </si>
@@ -11435,6 +11435,9 @@
   </si>
   <si>
     <t>Time has been coverded as automation but for date updation is not a part of Automation.</t>
+  </si>
+  <si>
+    <t>Sprint 8 Sep - 15 Sep</t>
   </si>
 </sst>
 </file>
@@ -16057,7 +16060,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16966,7 +16969,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J42"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -16975,12 +16977,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K290" sqref="K290"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="D291" sqref="D291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17048,7 +17048,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -17085,7 +17085,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -17122,7 +17122,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>41</v>
       </c>
@@ -17159,7 +17159,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>42</v>
       </c>
@@ -17196,7 +17196,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>43</v>
       </c>
@@ -17233,7 +17233,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>44</v>
       </c>
@@ -17270,7 +17270,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>45</v>
       </c>
@@ -17307,7 +17307,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>46</v>
       </c>
@@ -17344,7 +17344,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>47</v>
       </c>
@@ -17381,7 +17381,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>48</v>
       </c>
@@ -17416,7 +17416,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>49</v>
       </c>
@@ -17451,7 +17451,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>54</v>
       </c>
@@ -17488,7 +17488,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>55</v>
       </c>
@@ -17525,7 +17525,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>56</v>
       </c>
@@ -17562,7 +17562,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>57</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>58</v>
       </c>
@@ -17636,7 +17636,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>59</v>
       </c>
@@ -17673,7 +17673,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>60</v>
       </c>
@@ -17710,7 +17710,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>61</v>
       </c>
@@ -17747,7 +17747,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>62</v>
       </c>
@@ -17784,7 +17784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>63</v>
       </c>
@@ -17821,7 +17821,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>64</v>
       </c>
@@ -17858,7 +17858,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>65</v>
       </c>
@@ -17895,7 +17895,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>67</v>
       </c>
@@ -17932,7 +17932,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>68</v>
       </c>
@@ -17969,7 +17969,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>69</v>
       </c>
@@ -18006,7 +18006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>70</v>
       </c>
@@ -18043,7 +18043,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>71</v>
       </c>
@@ -18080,7 +18080,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>72</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>73</v>
       </c>
@@ -18154,7 +18154,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>74</v>
       </c>
@@ -18191,7 +18191,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>75</v>
       </c>
@@ -18228,7 +18228,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>76</v>
       </c>
@@ -18265,7 +18265,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>77</v>
       </c>
@@ -18302,7 +18302,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>78</v>
       </c>
@@ -18339,7 +18339,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>79</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>80</v>
       </c>
@@ -18413,7 +18413,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>82</v>
       </c>
@@ -18450,7 +18450,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>83</v>
       </c>
@@ -18487,7 +18487,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>84</v>
       </c>
@@ -18524,7 +18524,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>85</v>
       </c>
@@ -18561,7 +18561,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>86</v>
       </c>
@@ -18598,7 +18598,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>87</v>
       </c>
@@ -18635,7 +18635,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>88</v>
       </c>
@@ -18672,7 +18672,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>89</v>
       </c>
@@ -18709,7 +18709,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>90</v>
       </c>
@@ -18746,7 +18746,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>91</v>
       </c>
@@ -18754,14 +18754,16 @@
         <v>1941</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>604</v>
+        <v>494</v>
       </c>
       <c r="D48" s="28"/>
       <c r="F48" s="21" t="s">
         <v>1106</v>
       </c>
       <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="H48" s="21" t="s">
+        <v>604</v>
+      </c>
       <c r="I48" s="21" t="s">
         <v>1940</v>
       </c>
@@ -18783,7 +18785,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>92</v>
       </c>
@@ -19079,7 +19081,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>100</v>
       </c>
@@ -19116,7 +19118,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>101</v>
       </c>
@@ -19153,7 +19155,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>102</v>
       </c>
@@ -19190,7 +19192,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>103</v>
       </c>
@@ -19227,7 +19229,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>104</v>
       </c>
@@ -19264,7 +19266,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>105</v>
       </c>
@@ -19301,7 +19303,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>106</v>
       </c>
@@ -19338,7 +19340,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>107</v>
       </c>
@@ -19375,7 +19377,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>108</v>
       </c>
@@ -19412,7 +19414,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>109</v>
       </c>
@@ -19449,7 +19451,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>110</v>
       </c>
@@ -19486,7 +19488,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>111</v>
       </c>
@@ -19523,7 +19525,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>112</v>
       </c>
@@ -19560,7 +19562,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>113</v>
       </c>
@@ -19597,7 +19599,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>114</v>
       </c>
@@ -19634,7 +19636,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>115</v>
       </c>
@@ -19671,7 +19673,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>116</v>
       </c>
@@ -19708,7 +19710,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>117</v>
       </c>
@@ -19745,7 +19747,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>118</v>
       </c>
@@ -19782,7 +19784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>119</v>
       </c>
@@ -19819,7 +19821,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>120</v>
       </c>
@@ -19856,7 +19858,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>121</v>
       </c>
@@ -19893,7 +19895,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>122</v>
       </c>
@@ -19930,7 +19932,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>123</v>
       </c>
@@ -19967,7 +19969,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>127</v>
       </c>
@@ -20004,7 +20006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>128</v>
       </c>
@@ -20041,7 +20043,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>129</v>
       </c>
@@ -20078,7 +20080,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>130</v>
       </c>
@@ -20117,7 +20119,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>131</v>
       </c>
@@ -20154,7 +20156,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>132</v>
       </c>
@@ -20191,7 +20193,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="370.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="370.2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>133</v>
       </c>
@@ -20228,7 +20230,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>134</v>
       </c>
@@ -20265,7 +20267,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>135</v>
       </c>
@@ -20302,7 +20304,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>136</v>
       </c>
@@ -20339,7 +20341,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>137</v>
       </c>
@@ -20376,7 +20378,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>138</v>
       </c>
@@ -20413,7 +20415,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>139</v>
       </c>
@@ -20450,7 +20452,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>140</v>
       </c>
@@ -20487,7 +20489,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>141</v>
       </c>
@@ -20524,7 +20526,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>142</v>
       </c>
@@ -20561,7 +20563,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>143</v>
       </c>
@@ -20598,7 +20600,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>144</v>
       </c>
@@ -20635,7 +20637,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>145</v>
       </c>
@@ -20672,7 +20674,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>146</v>
       </c>
@@ -20709,7 +20711,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>147</v>
       </c>
@@ -20746,7 +20748,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>148</v>
       </c>
@@ -20783,7 +20785,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>149</v>
       </c>
@@ -20820,7 +20822,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>153</v>
       </c>
@@ -20860,7 +20862,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>154</v>
       </c>
@@ -20897,7 +20899,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>155</v>
       </c>
@@ -20934,7 +20936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>156</v>
       </c>
@@ -20971,7 +20973,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>158</v>
       </c>
@@ -21006,7 +21008,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>159</v>
       </c>
@@ -21043,7 +21045,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>166</v>
       </c>
@@ -21078,7 +21080,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>167</v>
       </c>
@@ -21115,7 +21117,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>170</v>
       </c>
@@ -21150,7 +21152,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>171</v>
       </c>
@@ -21187,7 +21189,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>172</v>
       </c>
@@ -21224,7 +21226,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>173</v>
       </c>
@@ -21263,7 +21265,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>174</v>
       </c>
@@ -21302,7 +21304,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>175</v>
       </c>
@@ -21341,7 +21343,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>176</v>
       </c>
@@ -21380,7 +21382,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>177</v>
       </c>
@@ -21420,7 +21422,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>178</v>
       </c>
@@ -21460,7 +21462,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>179</v>
       </c>
@@ -21499,7 +21501,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>180</v>
       </c>
@@ -21539,7 +21541,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>182</v>
       </c>
@@ -21579,7 +21581,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>183</v>
       </c>
@@ -21616,7 +21618,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>185</v>
       </c>
@@ -21653,7 +21655,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>187</v>
       </c>
@@ -21690,7 +21692,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>189</v>
       </c>
@@ -21727,7 +21729,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>192</v>
       </c>
@@ -21764,7 +21766,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>193</v>
       </c>
@@ -21803,7 +21805,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>194</v>
       </c>
@@ -21842,7 +21844,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>196</v>
       </c>
@@ -21881,7 +21883,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>197</v>
       </c>
@@ -21918,7 +21920,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>199</v>
       </c>
@@ -21955,7 +21957,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>200</v>
       </c>
@@ -21992,7 +21994,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>202</v>
       </c>
@@ -22029,7 +22031,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>203</v>
       </c>
@@ -22066,7 +22068,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>204</v>
       </c>
@@ -22103,7 +22105,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>205</v>
       </c>
@@ -22143,7 +22145,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>206</v>
       </c>
@@ -22183,7 +22185,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="357" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="357" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>207</v>
       </c>
@@ -22297,7 +22299,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>210</v>
       </c>
@@ -22338,7 +22340,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>211</v>
       </c>
@@ -22379,7 +22381,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>212</v>
       </c>
@@ -22420,7 +22422,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>213</v>
       </c>
@@ -22458,7 +22460,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>214</v>
       </c>
@@ -22496,7 +22498,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>221</v>
       </c>
@@ -22537,7 +22539,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>222</v>
       </c>
@@ -22578,7 +22580,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>223</v>
       </c>
@@ -22613,7 +22615,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>224</v>
       </c>
@@ -22651,7 +22653,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>225</v>
       </c>
@@ -22686,7 +22688,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>227</v>
       </c>
@@ -22724,7 +22726,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>228</v>
       </c>
@@ -22762,7 +22764,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>231</v>
       </c>
@@ -22800,7 +22802,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>232</v>
       </c>
@@ -22835,7 +22837,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>233</v>
       </c>
@@ -22870,7 +22872,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>234</v>
       </c>
@@ -22905,7 +22907,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>235</v>
       </c>
@@ -22946,7 +22948,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>236</v>
       </c>
@@ -22981,7 +22983,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>237</v>
       </c>
@@ -23016,7 +23018,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>238</v>
       </c>
@@ -23051,7 +23053,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>239</v>
       </c>
@@ -23089,7 +23091,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>240</v>
       </c>
@@ -23127,7 +23129,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>241</v>
       </c>
@@ -23162,7 +23164,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>242</v>
       </c>
@@ -23200,7 +23202,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>243</v>
       </c>
@@ -23235,7 +23237,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>244</v>
       </c>
@@ -23273,7 +23275,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>245</v>
       </c>
@@ -23314,7 +23316,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>246</v>
       </c>
@@ -23349,7 +23351,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>247</v>
       </c>
@@ -23384,7 +23386,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>248</v>
       </c>
@@ -23427,7 +23429,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>249</v>
       </c>
@@ -23462,7 +23464,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>250</v>
       </c>
@@ -23497,7 +23499,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>251</v>
       </c>
@@ -23567,7 +23569,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>253</v>
       </c>
@@ -23605,7 +23607,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>256</v>
       </c>
@@ -23643,7 +23645,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="179" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>257</v>
       </c>
@@ -23678,7 +23680,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>258</v>
       </c>
@@ -23713,7 +23715,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>259</v>
       </c>
@@ -23748,7 +23750,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>260</v>
       </c>
@@ -23789,7 +23791,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>261</v>
       </c>
@@ -23824,7 +23826,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>262</v>
       </c>
@@ -23859,7 +23861,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>263</v>
       </c>
@@ -23894,7 +23896,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>264</v>
       </c>
@@ -23929,7 +23931,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>274</v>
       </c>
@@ -23962,7 +23964,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>275</v>
       </c>
@@ -23995,7 +23997,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>276</v>
       </c>
@@ -24028,7 +24030,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>277</v>
       </c>
@@ -24061,7 +24063,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>278</v>
       </c>
@@ -24094,7 +24096,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="192" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>279</v>
       </c>
@@ -24127,7 +24129,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>280</v>
       </c>
@@ -24160,7 +24162,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>281</v>
       </c>
@@ -24193,7 +24195,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>282</v>
       </c>
@@ -24226,7 +24228,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>283</v>
       </c>
@@ -24259,7 +24261,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>284</v>
       </c>
@@ -24292,7 +24294,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>285</v>
       </c>
@@ -24325,7 +24327,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>286</v>
       </c>
@@ -24360,7 +24362,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>287</v>
       </c>
@@ -24395,7 +24397,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>288</v>
       </c>
@@ -24430,7 +24432,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>289</v>
       </c>
@@ -24465,7 +24467,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>290</v>
       </c>
@@ -24500,7 +24502,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>291</v>
       </c>
@@ -24535,7 +24537,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>292</v>
       </c>
@@ -24570,7 +24572,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>295</v>
       </c>
@@ -24605,7 +24607,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>296</v>
       </c>
@@ -24640,7 +24642,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>297</v>
       </c>
@@ -24675,7 +24677,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>298</v>
       </c>
@@ -24710,7 +24712,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>299</v>
       </c>
@@ -24745,7 +24747,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>300</v>
       </c>
@@ -24780,7 +24782,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>301</v>
       </c>
@@ -24815,7 +24817,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>302</v>
       </c>
@@ -24850,7 +24852,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>303</v>
       </c>
@@ -24885,7 +24887,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>304</v>
       </c>
@@ -24920,7 +24922,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>305</v>
       </c>
@@ -24955,7 +24957,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>306</v>
       </c>
@@ -24990,7 +24992,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>307</v>
       </c>
@@ -25025,7 +25027,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>308</v>
       </c>
@@ -25060,7 +25062,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>309</v>
       </c>
@@ -25095,7 +25097,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>310</v>
       </c>
@@ -25130,7 +25132,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>311</v>
       </c>
@@ -25168,7 +25170,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>312</v>
       </c>
@@ -25244,7 +25246,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>314</v>
       </c>
@@ -25279,7 +25281,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>315</v>
       </c>
@@ -25314,7 +25316,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>316</v>
       </c>
@@ -25349,7 +25351,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>317</v>
       </c>
@@ -25384,7 +25386,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>318</v>
       </c>
@@ -25419,7 +25421,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>319</v>
       </c>
@@ -25454,7 +25456,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>320</v>
       </c>
@@ -25489,7 +25491,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>321</v>
       </c>
@@ -25524,7 +25526,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>322</v>
       </c>
@@ -25557,7 +25559,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="234" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>323</v>
       </c>
@@ -25590,7 +25592,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>324</v>
       </c>
@@ -25629,7 +25631,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>325</v>
       </c>
@@ -25668,7 +25670,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>328</v>
       </c>
@@ -25707,7 +25709,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>329</v>
       </c>
@@ -25746,7 +25748,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>331</v>
       </c>
@@ -25785,7 +25787,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>332</v>
       </c>
@@ -25820,7 +25822,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>333</v>
       </c>
@@ -25858,7 +25860,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>334</v>
       </c>
@@ -25893,7 +25895,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>335</v>
       </c>
@@ -25931,7 +25933,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>336</v>
       </c>
@@ -25969,7 +25971,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>337</v>
       </c>
@@ -26007,7 +26009,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>338</v>
       </c>
@@ -26042,7 +26044,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>339</v>
       </c>
@@ -26077,7 +26079,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>341</v>
       </c>
@@ -26115,7 +26117,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>342</v>
       </c>
@@ -26153,7 +26155,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>343</v>
       </c>
@@ -26188,7 +26190,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>344</v>
       </c>
@@ -26223,7 +26225,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>345</v>
       </c>
@@ -26261,7 +26263,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>346</v>
       </c>
@@ -26299,7 +26301,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>347</v>
       </c>
@@ -26334,7 +26336,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>348</v>
       </c>
@@ -26372,7 +26374,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>349</v>
       </c>
@@ -26410,7 +26412,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>350</v>
       </c>
@@ -26445,7 +26447,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>351</v>
       </c>
@@ -26488,7 +26490,9 @@
         <v>1256</v>
       </c>
       <c r="C259" s="58"/>
-      <c r="D259" s="58"/>
+      <c r="D259" s="58" t="s">
+        <v>2243</v>
+      </c>
       <c r="E259" s="58"/>
       <c r="F259" s="3" t="s">
         <v>1106</v>
@@ -26553,7 +26557,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>355</v>
       </c>
@@ -26588,7 +26592,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>356</v>
       </c>
@@ -26629,7 +26633,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>359</v>
       </c>
@@ -26664,7 +26668,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>360</v>
       </c>
@@ -26699,7 +26703,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>362</v>
       </c>
@@ -26734,7 +26738,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>363</v>
       </c>
@@ -26804,7 +26808,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>365</v>
       </c>
@@ -26839,7 +26843,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>366</v>
       </c>
@@ -26877,7 +26881,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>367</v>
       </c>
@@ -26915,7 +26919,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>368</v>
       </c>
@@ -26953,7 +26957,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>369</v>
       </c>
@@ -26988,7 +26992,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>370</v>
       </c>
@@ -27023,7 +27027,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>371</v>
       </c>
@@ -27061,7 +27065,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>372</v>
       </c>
@@ -27099,7 +27103,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>373</v>
       </c>
@@ -27134,7 +27138,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>374</v>
       </c>
@@ -27169,7 +27173,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>375</v>
       </c>
@@ -27204,7 +27208,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>376</v>
       </c>
@@ -27239,7 +27243,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>377</v>
       </c>
@@ -27274,7 +27278,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>378</v>
       </c>
@@ -27309,7 +27313,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>379</v>
       </c>
@@ -27379,7 +27383,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>381</v>
       </c>
@@ -27414,7 +27418,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>382</v>
       </c>
@@ -27457,7 +27461,9 @@
         <v>1167</v>
       </c>
       <c r="C286" s="58"/>
-      <c r="D286" s="58"/>
+      <c r="D286" s="58" t="s">
+        <v>2243</v>
+      </c>
       <c r="E286" s="58"/>
       <c r="F286" s="4" t="s">
         <v>1106</v>
@@ -27487,7 +27493,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>386</v>
       </c>
@@ -27531,7 +27537,9 @@
         <v>1160</v>
       </c>
       <c r="C288" s="58"/>
-      <c r="D288" s="58"/>
+      <c r="D288" s="58" t="s">
+        <v>2243</v>
+      </c>
       <c r="E288" s="58"/>
       <c r="F288" s="4" t="s">
         <v>1106</v>
@@ -27561,7 +27569,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>388</v>
       </c>
@@ -27645,7 +27653,9 @@
         <v>1150</v>
       </c>
       <c r="C291" s="58"/>
-      <c r="D291" s="58"/>
+      <c r="D291" s="58" t="s">
+        <v>2243</v>
+      </c>
       <c r="E291" s="58"/>
       <c r="F291" s="3" t="s">
         <v>1106</v>
@@ -27712,7 +27722,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>392</v>
       </c>
@@ -27788,7 +27798,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>394</v>
       </c>
@@ -27829,7 +27839,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>395</v>
       </c>
@@ -27905,7 +27915,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>397</v>
       </c>
@@ -28051,7 +28061,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>401</v>
       </c>
@@ -28092,7 +28102,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="303" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>402</v>
       </c>
@@ -28129,7 +28139,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="304" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>403</v>
       </c>
@@ -28166,7 +28176,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>404</v>
       </c>
@@ -28203,7 +28213,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>405</v>
       </c>
@@ -28240,7 +28250,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>406</v>
       </c>
@@ -28277,7 +28287,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>407</v>
       </c>
@@ -28314,7 +28324,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>408</v>
       </c>
@@ -28351,7 +28361,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="310" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>409</v>
       </c>
@@ -28388,7 +28398,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>410</v>
       </c>
@@ -28425,7 +28435,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>411</v>
       </c>
@@ -28462,7 +28472,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>412</v>
       </c>
@@ -28499,7 +28509,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>413</v>
       </c>
@@ -28534,7 +28544,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>415</v>
       </c>
@@ -28569,7 +28579,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>417</v>
       </c>
@@ -28606,7 +28616,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>418</v>
       </c>
@@ -28643,7 +28653,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>419</v>
       </c>
@@ -28680,7 +28690,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>420</v>
       </c>
@@ -28717,7 +28727,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>421</v>
       </c>
@@ -28754,7 +28764,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>422</v>
       </c>
@@ -28791,7 +28801,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>423</v>
       </c>
@@ -28828,7 +28838,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="323" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>424</v>
       </c>
@@ -28865,7 +28875,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>426</v>
       </c>
@@ -28900,7 +28910,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>427</v>
       </c>
@@ -28935,7 +28945,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>429</v>
       </c>
@@ -28972,7 +28982,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>430</v>
       </c>
@@ -29009,7 +29019,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>431</v>
       </c>
@@ -29046,7 +29056,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>432</v>
       </c>
@@ -29083,7 +29093,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>433</v>
       </c>
@@ -29120,7 +29130,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>434</v>
       </c>
@@ -29157,7 +29167,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>435</v>
       </c>
@@ -29192,7 +29202,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>436</v>
       </c>
@@ -29227,7 +29237,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>437</v>
       </c>
@@ -29262,7 +29272,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>440</v>
       </c>
@@ -29299,7 +29309,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>441</v>
       </c>
@@ -29336,7 +29346,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="337" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>442</v>
       </c>
@@ -29373,7 +29383,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="338" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>443</v>
       </c>
@@ -29410,7 +29420,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="339" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>444</v>
       </c>
@@ -29447,7 +29457,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="340" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>445</v>
       </c>
@@ -29484,7 +29494,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="341" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>448</v>
       </c>
@@ -29521,7 +29531,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="342" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>449</v>
       </c>
@@ -29558,7 +29568,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="343" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>450</v>
       </c>
@@ -29595,7 +29605,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="344" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>451</v>
       </c>
@@ -29632,7 +29642,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>452</v>
       </c>
@@ -29669,7 +29679,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="346" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>453</v>
       </c>
@@ -29706,7 +29716,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="347" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>455</v>
       </c>
@@ -29743,7 +29753,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="348" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>456</v>
       </c>
@@ -29780,7 +29790,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>457</v>
       </c>
@@ -29817,7 +29827,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="350" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>458</v>
       </c>
@@ -29854,7 +29864,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="351" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>459</v>
       </c>
@@ -29891,7 +29901,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="352" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>460</v>
       </c>
@@ -29928,7 +29938,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>461</v>
       </c>
@@ -29965,7 +29975,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>463</v>
       </c>
@@ -30002,7 +30012,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>464</v>
       </c>
@@ -30039,7 +30049,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>465</v>
       </c>
@@ -30076,7 +30086,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="357" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>469</v>
       </c>
@@ -30113,7 +30123,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>470</v>
       </c>
@@ -30150,7 +30160,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>471</v>
       </c>
@@ -30187,7 +30197,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>472</v>
       </c>
@@ -30224,7 +30234,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>473</v>
       </c>
@@ -30298,7 +30308,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>475</v>
       </c>
@@ -30335,7 +30345,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>476</v>
       </c>
@@ -30372,7 +30382,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>477</v>
       </c>
@@ -30409,7 +30419,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>479</v>
       </c>
@@ -30444,7 +30454,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>480</v>
       </c>
@@ -30479,7 +30489,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>481</v>
       </c>
@@ -30514,7 +30524,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="330.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:16" ht="330.6" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>482</v>
       </c>
@@ -30549,7 +30559,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>483</v>
       </c>
@@ -30586,7 +30596,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>484</v>
       </c>
@@ -30621,7 +30631,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>485</v>
       </c>
@@ -30656,7 +30666,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>486</v>
       </c>
@@ -30691,7 +30701,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>487</v>
       </c>
@@ -30726,7 +30736,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>489</v>
       </c>
@@ -30761,7 +30771,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>490</v>
       </c>
@@ -30796,7 +30806,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>491</v>
       </c>
@@ -30831,7 +30841,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>492</v>
       </c>
@@ -30866,7 +30876,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>493</v>
       </c>
@@ -30901,7 +30911,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>494</v>
       </c>
@@ -30936,7 +30946,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>495</v>
       </c>
@@ -30971,7 +30981,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>498</v>
       </c>
@@ -31006,7 +31016,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>499</v>
       </c>
@@ -31041,7 +31051,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>500</v>
       </c>
@@ -31076,7 +31086,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>501</v>
       </c>
@@ -31111,7 +31121,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>503</v>
       </c>
@@ -31146,7 +31156,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>504</v>
       </c>
@@ -31181,7 +31191,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>505</v>
       </c>
@@ -31216,7 +31226,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="389" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>506</v>
       </c>
@@ -31249,7 +31259,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="390" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>507</v>
       </c>
@@ -31280,7 +31290,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="391" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>508</v>
       </c>
@@ -31313,7 +31323,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>509</v>
       </c>
@@ -31391,7 +31401,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>511</v>
       </c>
@@ -31428,7 +31438,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="395" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>512</v>
       </c>
@@ -31465,7 +31475,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="396" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>513</v>
       </c>
@@ -31502,7 +31512,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>514</v>
       </c>
@@ -31539,7 +31549,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>515</v>
       </c>
@@ -31576,7 +31586,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>516</v>
       </c>
@@ -31685,7 +31695,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>529</v>
       </c>
@@ -31788,7 +31798,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>548</v>
       </c>
@@ -31821,7 +31831,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="406" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>564</v>
       </c>
@@ -31858,7 +31868,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="407" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>565</v>
       </c>
@@ -31895,7 +31905,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="408" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>570</v>
       </c>
@@ -31932,7 +31942,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="409" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>571</v>
       </c>
@@ -31969,7 +31979,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="410" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>574</v>
       </c>
@@ -32006,7 +32016,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="411" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>575</v>
       </c>
@@ -32043,7 +32053,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="412" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>576</v>
       </c>
@@ -32080,7 +32090,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="413" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>577</v>
       </c>
@@ -32117,7 +32127,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="414" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>580</v>
       </c>
@@ -32154,7 +32164,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="415" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>581</v>
       </c>
@@ -32191,7 +32201,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="416" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>582</v>
       </c>
@@ -32226,7 +32236,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="417" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>583</v>
       </c>
@@ -32261,7 +32271,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="418" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>584</v>
       </c>
@@ -32296,7 +32306,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="419" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>585</v>
       </c>
@@ -32331,7 +32341,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="420" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>586</v>
       </c>
@@ -32366,7 +32376,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="421" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>587</v>
       </c>
@@ -32403,7 +32413,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="422" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>588</v>
       </c>
@@ -32438,7 +32448,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="423" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>589</v>
       </c>
@@ -32473,7 +32483,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="424" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>590</v>
       </c>
@@ -32508,7 +32518,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="425" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>591</v>
       </c>
@@ -32543,7 +32553,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="426" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>592</v>
       </c>
@@ -32578,7 +32588,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="427" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>593</v>
       </c>
@@ -32613,7 +32623,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="428" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>594</v>
       </c>
@@ -32648,7 +32658,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="429" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>595</v>
       </c>
@@ -32683,7 +32693,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="430" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>596</v>
       </c>
@@ -32718,7 +32728,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="431" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>597</v>
       </c>
@@ -32753,7 +32763,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="432" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>598</v>
       </c>
@@ -32790,7 +32800,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="433" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>599</v>
       </c>
@@ -32827,7 +32837,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="434" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>600</v>
       </c>
@@ -32862,7 +32872,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="435" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>601</v>
       </c>
@@ -32897,7 +32907,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="436" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>602</v>
       </c>
@@ -32934,7 +32944,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="437" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>603</v>
       </c>
@@ -32971,7 +32981,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="438" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>604</v>
       </c>
@@ -33008,7 +33018,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="439" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>605</v>
       </c>
@@ -33043,7 +33053,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="440" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>606</v>
       </c>
@@ -33078,7 +33088,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="441" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>607</v>
       </c>
@@ -33113,7 +33123,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="442" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>608</v>
       </c>
@@ -33149,35 +33159,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P442">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Ankit"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P442"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33454,7 +33448,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -33482,7 +33476,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -33520,7 +33514,7 @@
       <c r="U9" s="43"/>
       <c r="V9" s="43"/>
     </row>
-    <row r="10" spans="1:22" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="130.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -33558,7 +33552,7 @@
       <c r="U10" s="43"/>
       <c r="V10" s="43"/>
     </row>
-    <row r="11" spans="1:22" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -33596,7 +33590,7 @@
       <c r="U11" s="43"/>
       <c r="V11" s="43"/>
     </row>
-    <row r="12" spans="1:22" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="88.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -33677,7 +33671,7 @@
       <c r="U13" s="43"/>
       <c r="V13" s="43"/>
     </row>
-    <row r="14" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -33811,7 +33805,7 @@
       <c r="D17" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -33841,7 +33835,7 @@
       <c r="U17" s="43"/>
       <c r="V17" s="43"/>
     </row>
-    <row r="18" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -33891,7 +33885,7 @@
       <c r="D19" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -34007,7 +34001,7 @@
       <c r="U21" s="43"/>
       <c r="V21" s="43"/>
     </row>
-    <row r="22" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -34100,7 +34094,7 @@
       <c r="D24" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -34143,7 +34137,7 @@
       <c r="D25" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -34227,7 +34221,7 @@
       <c r="D27" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -34255,7 +34249,7 @@
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
     </row>
-    <row r="28" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -34303,7 +34297,7 @@
       <c r="D29" s="6" t="s">
         <v>599</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="6" t="s">
         <v>2238</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -34333,7 +34327,7 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
     </row>
-    <row r="30" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -34370,7 +34364,7 @@
       <c r="U30" s="43"/>
       <c r="V30" s="43"/>
     </row>
-    <row r="31" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -34502,7 +34496,13 @@
       <c r="V33" s="43"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V33"/>
+  <autoFilter ref="A1:V33">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
commit Test case sheet
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5552" uniqueCount="2244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5571" uniqueCount="2245">
   <si>
     <t>Name</t>
   </si>
@@ -11438,6 +11438,9 @@
   </si>
   <si>
     <t>Sprint 8 Sep - 15 Sep</t>
+  </si>
+  <si>
+    <t>Reminder Feature not yet implemented</t>
   </si>
 </sst>
 </file>
@@ -16967,11 +16970,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B286" sqref="B286"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
@@ -21143,15 +21146,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>171</v>
       </c>
       <c r="B113" s="21" t="s">
         <v>1704</v>
       </c>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
+      <c r="C113" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F113" s="21" t="s">
         <v>1106</v>
       </c>
@@ -21180,15 +21187,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>172</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>1700</v>
       </c>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
+      <c r="C114" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F114" s="18" t="s">
         <v>1106</v>
       </c>
@@ -22644,12 +22655,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>225</v>
       </c>
       <c r="B152" s="21" t="s">
         <v>1575</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>2243</v>
       </c>
       <c r="F152" s="18" t="s">
         <v>1106</v>
@@ -22793,12 +22810,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>232</v>
       </c>
       <c r="B156" s="18" t="s">
         <v>1559</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>2243</v>
       </c>
       <c r="F156" s="18" t="s">
         <v>1106</v>
@@ -22828,12 +22851,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>233</v>
       </c>
       <c r="B157" s="21" t="s">
         <v>1555</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>2243</v>
       </c>
       <c r="F157" s="18" t="s">
         <v>1106</v>
@@ -22863,12 +22892,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>234</v>
       </c>
       <c r="B158" s="18" t="s">
         <v>1551</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>2243</v>
       </c>
       <c r="F158" s="18" t="s">
         <v>1106</v>
@@ -29312,15 +29347,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>441</v>
       </c>
       <c r="B336" s="21" t="s">
         <v>986</v>
       </c>
-      <c r="C336" s="27"/>
-      <c r="D336" s="27"/>
+      <c r="C336" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D336" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F336" s="21" t="s">
         <v>1106</v>
       </c>
@@ -29793,15 +29832,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>457</v>
       </c>
       <c r="B349" s="21" t="s">
         <v>945</v>
       </c>
-      <c r="C349" s="27"/>
-      <c r="D349" s="27"/>
+      <c r="C349" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D349" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F349" s="21" t="s">
         <v>1106</v>
       </c>
@@ -31945,15 +31988,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="409" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>571</v>
       </c>
       <c r="B409" s="21" t="s">
         <v>783</v>
       </c>
-      <c r="C409" s="27"/>
-      <c r="D409" s="27"/>
+      <c r="C409" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D409" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F409" s="21" t="s">
         <v>1106</v>
       </c>
@@ -33163,14 +33210,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P442">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="Sprint 8 Sep - 15 Sep"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Ankit"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -33183,9 +33230,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33270,7 +33317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="111.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -33303,7 +33350,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="121.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -33336,7 +33383,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -33369,7 +33416,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="229.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="229.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -33402,7 +33449,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="141" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -33432,7 +33479,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="192.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -33462,7 +33509,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -33473,12 +33520,14 @@
         <v>1106</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>599</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>2243</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>689</v>
+        <v>612</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>2087</v>
@@ -33641,7 +33690,7 @@
       <c r="U12" s="36"/>
       <c r="V12" s="36"/>
     </row>
-    <row r="13" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -33719,7 +33768,7 @@
       <c r="U14" s="36"/>
       <c r="V14" s="36"/>
     </row>
-    <row r="15" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -33762,7 +33811,7 @@
       <c r="U15" s="36"/>
       <c r="V15" s="36"/>
     </row>
-    <row r="16" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -33806,7 +33855,7 @@
       <c r="U16" s="36"/>
       <c r="V16" s="36"/>
     </row>
-    <row r="17" spans="1:22" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -33886,7 +33935,7 @@
       <c r="U18" s="36"/>
       <c r="V18" s="36"/>
     </row>
-    <row r="19" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -33929,7 +33978,7 @@
       <c r="U19" s="36"/>
       <c r="V19" s="36"/>
     </row>
-    <row r="20" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="53.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -33972,7 +34021,7 @@
       <c r="U20" s="36"/>
       <c r="V20" s="36"/>
     </row>
-    <row r="21" spans="1:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="51.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -34052,7 +34101,7 @@
       <c r="U22" s="36"/>
       <c r="V22" s="36"/>
     </row>
-    <row r="23" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -34095,7 +34144,7 @@
       <c r="U23" s="36"/>
       <c r="V23" s="36"/>
     </row>
-    <row r="24" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="57" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -34138,7 +34187,7 @@
       <c r="U24" s="36"/>
       <c r="V24" s="36"/>
     </row>
-    <row r="25" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="50.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -34181,7 +34230,7 @@
       <c r="U25" s="36"/>
       <c r="V25" s="36"/>
     </row>
-    <row r="26" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -34224,7 +34273,7 @@
       <c r="U26" s="36"/>
       <c r="V26" s="36"/>
     </row>
-    <row r="27" spans="1:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="43.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -34298,7 +34347,7 @@
       <c r="U28" s="36"/>
       <c r="V28" s="36"/>
     </row>
-    <row r="29" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -34386,7 +34435,7 @@
         <v>2133</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>1106</v>
+        <v>2244</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>494</v>
@@ -34421,7 +34470,7 @@
       <c r="U31" s="36"/>
       <c r="V31" s="36"/>
     </row>
-    <row r="32" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -34465,7 +34514,7 @@
       <c r="U32" s="36"/>
       <c r="V32" s="36"/>
     </row>
-    <row r="33" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -34511,7 +34560,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V33">
-    <filterColumn colId="3">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Sprint 8 Sep - 15 Sep"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>

</xml_diff>

<commit_message>
bug fixing in regression
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5571" uniqueCount="2245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5571" uniqueCount="2244">
   <si>
     <t>Name</t>
   </si>
@@ -11426,9 +11426,6 @@
   </si>
   <si>
     <t>Sprint 1-Sep  - 8Sep</t>
-  </si>
-  <si>
-    <t>No(Upsellable functionbality not working )</t>
   </si>
   <si>
     <t>NO(Change sorting category is depend on TM)</t>
@@ -16049,8 +16046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16970,8 +16967,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P442"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18740,7 +18737,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>91</v>
       </c>
@@ -18779,7 +18776,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>92</v>
       </c>
@@ -18789,7 +18786,7 @@
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="F49" s="21" t="s">
-        <v>2240</v>
+        <v>1106</v>
       </c>
       <c r="G49" s="21"/>
       <c r="H49" s="21" t="s">
@@ -18853,7 +18850,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>94</v>
       </c>
@@ -18890,7 +18887,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>95</v>
       </c>
@@ -18927,7 +18924,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>96</v>
       </c>
@@ -18964,7 +18961,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>97</v>
       </c>
@@ -19001,7 +18998,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>98</v>
       </c>
@@ -19038,7 +19035,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>99</v>
       </c>
@@ -20816,7 +20813,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>153</v>
       </c>
@@ -20930,7 +20927,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>156</v>
       </c>
@@ -20940,7 +20937,7 @@
       <c r="C107" s="18"/>
       <c r="D107" s="18"/>
       <c r="F107" s="18" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="G107" s="18"/>
       <c r="H107" s="18" t="s">
@@ -21146,7 +21143,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>171</v>
       </c>
@@ -21157,7 +21154,7 @@
         <v>496</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F113" s="21" t="s">
         <v>1106</v>
@@ -21187,7 +21184,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>172</v>
       </c>
@@ -21198,7 +21195,7 @@
         <v>496</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F114" s="18" t="s">
         <v>1106</v>
@@ -22107,7 +22104,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>205</v>
       </c>
@@ -22147,7 +22144,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>206</v>
       </c>
@@ -22187,7 +22184,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="357" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="357" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>207</v>
       </c>
@@ -22227,7 +22224,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>208</v>
       </c>
@@ -22264,7 +22261,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>209</v>
       </c>
@@ -22301,7 +22298,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>210</v>
       </c>
@@ -22342,7 +22339,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>211</v>
       </c>
@@ -22383,7 +22380,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -22424,7 +22421,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>213</v>
       </c>
@@ -22462,7 +22459,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>214</v>
       </c>
@@ -22500,7 +22497,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>221</v>
       </c>
@@ -22541,7 +22538,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>222</v>
       </c>
@@ -22655,7 +22652,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>225</v>
       </c>
@@ -22666,7 +22663,7 @@
         <v>496</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F152" s="18" t="s">
         <v>1106</v>
@@ -22810,7 +22807,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>232</v>
       </c>
@@ -22821,7 +22818,7 @@
         <v>496</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F156" s="18" t="s">
         <v>1106</v>
@@ -22851,7 +22848,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>233</v>
       </c>
@@ -22862,7 +22859,7 @@
         <v>496</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F157" s="18" t="s">
         <v>1106</v>
@@ -22892,7 +22889,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>234</v>
       </c>
@@ -22903,7 +22900,7 @@
         <v>496</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F158" s="18" t="s">
         <v>1106</v>
@@ -23412,7 +23409,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>248</v>
       </c>
@@ -23560,7 +23557,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>252</v>
       </c>
@@ -23595,7 +23592,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>253</v>
       </c>
@@ -23633,7 +23630,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>256</v>
       </c>
@@ -23776,7 +23773,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>260</v>
       </c>
@@ -25158,7 +25155,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>311</v>
       </c>
@@ -25196,7 +25193,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>312</v>
       </c>
@@ -25245,7 +25242,7 @@
         <v>496</v>
       </c>
       <c r="D224" s="53" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E224" s="53"/>
       <c r="F224" s="51" t="s">
@@ -26523,7 +26520,7 @@
         <v>496</v>
       </c>
       <c r="D259" s="53" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E259" s="53"/>
       <c r="F259" s="52" t="s">
@@ -26554,7 +26551,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>354</v>
       </c>
@@ -26805,7 +26802,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>364</v>
       </c>
@@ -27380,7 +27377,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>380</v>
       </c>
@@ -27496,7 +27493,7 @@
         <v>496</v>
       </c>
       <c r="D286" s="53" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E286" s="53"/>
       <c r="F286" s="51" t="s">
@@ -27574,7 +27571,7 @@
         <v>496</v>
       </c>
       <c r="D288" s="53" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E288" s="53"/>
       <c r="F288" s="51" t="s">
@@ -27605,7 +27602,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>388</v>
       </c>
@@ -27646,7 +27643,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>389</v>
       </c>
@@ -27692,14 +27689,14 @@
         <v>496</v>
       </c>
       <c r="D291" s="53" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E291" s="53"/>
       <c r="F291" s="52" t="s">
         <v>1106</v>
       </c>
       <c r="G291" s="52" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="H291" s="52" t="s">
         <v>604</v>
@@ -27725,7 +27722,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>391</v>
       </c>
@@ -27801,7 +27798,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>393</v>
       </c>
@@ -27836,7 +27833,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>394</v>
       </c>
@@ -27877,7 +27874,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>395</v>
       </c>
@@ -27918,7 +27915,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>396</v>
       </c>
@@ -27953,7 +27950,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>397</v>
       </c>
@@ -27994,7 +27991,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="299" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>398</v>
       </c>
@@ -28029,7 +28026,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>399</v>
       </c>
@@ -28064,7 +28061,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="301" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>400</v>
       </c>
@@ -28099,7 +28096,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>401</v>
       </c>
@@ -29347,7 +29344,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>441</v>
       </c>
@@ -29358,7 +29355,7 @@
         <v>496</v>
       </c>
       <c r="D336" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F336" s="21" t="s">
         <v>1106</v>
@@ -29832,7 +29829,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>457</v>
       </c>
@@ -29843,7 +29840,7 @@
         <v>496</v>
       </c>
       <c r="D349" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F349" s="21" t="s">
         <v>1106</v>
@@ -30317,7 +30314,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>474</v>
       </c>
@@ -31410,7 +31407,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>510</v>
       </c>
@@ -31667,7 +31664,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>517</v>
       </c>
@@ -31704,7 +31701,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>518</v>
       </c>
@@ -31778,7 +31775,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="403" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A403" s="1">
         <v>541</v>
       </c>
@@ -31811,7 +31808,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="404" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>547</v>
       </c>
@@ -31988,7 +31985,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="409" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>571</v>
       </c>
@@ -31999,7 +31996,7 @@
         <v>496</v>
       </c>
       <c r="D409" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F409" s="21" t="s">
         <v>1106</v>
@@ -33210,14 +33207,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P442">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="3">
+    <filterColumn colId="7">
       <filters>
-        <filter val="Sprint 8 Sep - 15 Sep"/>
+        <filter val="Ankit"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -33230,9 +33222,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33350,7 +33342,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="121.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -33449,7 +33441,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="141" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="141" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -33509,7 +33501,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -33523,7 +33515,7 @@
         <v>599</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
@@ -33768,7 +33760,7 @@
       <c r="U14" s="36"/>
       <c r="V14" s="36"/>
     </row>
-    <row r="15" spans="1:22" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -34144,7 +34136,7 @@
       <c r="U23" s="36"/>
       <c r="V23" s="36"/>
     </row>
-    <row r="24" spans="1:22" ht="57" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -34230,7 +34222,7 @@
       <c r="U25" s="36"/>
       <c r="V25" s="36"/>
     </row>
-    <row r="26" spans="1:22" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -34347,7 +34339,7 @@
       <c r="U28" s="36"/>
       <c r="V28" s="36"/>
     </row>
-    <row r="29" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -34435,7 +34427,7 @@
         <v>2133</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>494</v>
@@ -34470,7 +34462,7 @@
       <c r="U31" s="36"/>
       <c r="V31" s="36"/>
     </row>
-    <row r="32" spans="1:22" ht="92.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -34565,15 +34557,10 @@
         <filter val="Yes"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="4">
+    <filterColumn colId="6">
       <filters>
-        <filter val="Sprint 8 Sep - 15 Sep"/>
+        <filter val="Ankit"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit test cases and bug fix
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5598" uniqueCount="2260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5608" uniqueCount="2261">
   <si>
     <t>Name</t>
   </si>
@@ -11479,6 +11479,9 @@
 3. playout returns to what was playing (TV/TSTV/CUTV or RADIO), or if playout is not available then the last watched TV channel is played</t>
   </si>
   <si>
+    <t>Sprint 15 Sep - 22 Sep</t>
+  </si>
+  <si>
     <t xml:space="preserve">Step 1
 1. the TV channel tuned before pressing MENU will be tuned
 2. The Radio channel tuned before pressing MENU will be tuned
@@ -11491,7 +11494,7 @@
 2. HUB is shown over tuned Radio channel.
 3. a. Close menu &amp; return to full-screen media (Radio);
 stream not affected
-b.Close menu &amp; return to full-screen media (Radio);
+b.Close menu &amp; return to full-screen media (TV);
 stream not affected
 </t>
   </si>
@@ -17031,12 +17034,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P446"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A403" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A401" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H403" sqref="H403"/>
+      <selection pane="bottomLeft" activeCell="K401" sqref="K401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17108,7 +17112,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -17145,7 +17149,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -17182,7 +17186,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>41</v>
       </c>
@@ -17219,7 +17223,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42</v>
       </c>
@@ -17256,7 +17260,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43</v>
       </c>
@@ -17293,7 +17297,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44</v>
       </c>
@@ -17330,7 +17334,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45</v>
       </c>
@@ -17367,7 +17371,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>46</v>
       </c>
@@ -17404,7 +17408,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>47</v>
       </c>
@@ -17441,7 +17445,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>48</v>
       </c>
@@ -17476,7 +17480,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>49</v>
       </c>
@@ -17511,7 +17515,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>54</v>
       </c>
@@ -17548,7 +17552,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>55</v>
       </c>
@@ -17585,7 +17589,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>56</v>
       </c>
@@ -17622,7 +17626,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>57</v>
       </c>
@@ -17659,7 +17663,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>58</v>
       </c>
@@ -17696,7 +17700,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>59</v>
       </c>
@@ -17733,7 +17737,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>60</v>
       </c>
@@ -17770,7 +17774,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -17807,7 +17811,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>62</v>
       </c>
@@ -17844,7 +17848,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>63</v>
       </c>
@@ -17881,7 +17885,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>64</v>
       </c>
@@ -17918,7 +17922,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>65</v>
       </c>
@@ -17955,7 +17959,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>67</v>
       </c>
@@ -17992,7 +17996,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>68</v>
       </c>
@@ -18029,7 +18033,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>69</v>
       </c>
@@ -18066,7 +18070,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -18103,7 +18107,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>71</v>
       </c>
@@ -18140,7 +18144,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>72</v>
       </c>
@@ -18177,7 +18181,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>73</v>
       </c>
@@ -18214,7 +18218,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>74</v>
       </c>
@@ -18251,7 +18255,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>75</v>
       </c>
@@ -18288,7 +18292,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>76</v>
       </c>
@@ -18325,7 +18329,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>77</v>
       </c>
@@ -18362,7 +18366,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>78</v>
       </c>
@@ -18399,7 +18403,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>79</v>
       </c>
@@ -18436,7 +18440,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>80</v>
       </c>
@@ -18473,7 +18477,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>82</v>
       </c>
@@ -18510,7 +18514,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>83</v>
       </c>
@@ -18547,7 +18551,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>84</v>
       </c>
@@ -18584,7 +18588,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>85</v>
       </c>
@@ -18621,7 +18625,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>86</v>
       </c>
@@ -18658,7 +18662,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>87</v>
       </c>
@@ -18695,7 +18699,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>88</v>
       </c>
@@ -18732,7 +18736,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>89</v>
       </c>
@@ -18769,7 +18773,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>90</v>
       </c>
@@ -18806,7 +18810,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>91</v>
       </c>
@@ -18845,7 +18849,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>92</v>
       </c>
@@ -18884,7 +18888,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>93</v>
       </c>
@@ -18921,7 +18925,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>94</v>
       </c>
@@ -18960,7 +18964,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>95</v>
       </c>
@@ -18999,7 +19003,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>96</v>
       </c>
@@ -19038,7 +19042,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>97</v>
       </c>
@@ -19077,7 +19081,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>98</v>
       </c>
@@ -19116,7 +19120,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>99</v>
       </c>
@@ -19155,7 +19159,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>100</v>
       </c>
@@ -19192,7 +19196,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>101</v>
       </c>
@@ -19229,7 +19233,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>102</v>
       </c>
@@ -19266,7 +19270,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>103</v>
       </c>
@@ -19303,7 +19307,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>104</v>
       </c>
@@ -19340,7 +19344,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>105</v>
       </c>
@@ -19377,7 +19381,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>106</v>
       </c>
@@ -19414,7 +19418,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>107</v>
       </c>
@@ -19451,7 +19455,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>108</v>
       </c>
@@ -19488,7 +19492,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>109</v>
       </c>
@@ -19525,7 +19529,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>110</v>
       </c>
@@ -19562,7 +19566,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>111</v>
       </c>
@@ -19599,7 +19603,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>112</v>
       </c>
@@ -19636,7 +19640,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>113</v>
       </c>
@@ -19673,7 +19677,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>114</v>
       </c>
@@ -19710,7 +19714,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>115</v>
       </c>
@@ -19747,7 +19751,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>116</v>
       </c>
@@ -19784,7 +19788,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>117</v>
       </c>
@@ -19821,7 +19825,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>118</v>
       </c>
@@ -19858,7 +19862,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>119</v>
       </c>
@@ -19895,7 +19899,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>120</v>
       </c>
@@ -19932,7 +19936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>121</v>
       </c>
@@ -19969,7 +19973,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>122</v>
       </c>
@@ -20006,7 +20010,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>123</v>
       </c>
@@ -20043,7 +20047,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>127</v>
       </c>
@@ -20080,7 +20084,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>128</v>
       </c>
@@ -20117,7 +20121,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>129</v>
       </c>
@@ -20154,7 +20158,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>130</v>
       </c>
@@ -20193,7 +20197,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>131</v>
       </c>
@@ -20230,7 +20234,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>132</v>
       </c>
@@ -20267,7 +20271,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="370.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="370.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>133</v>
       </c>
@@ -20304,7 +20308,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>134</v>
       </c>
@@ -20341,7 +20345,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>135</v>
       </c>
@@ -20378,7 +20382,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>136</v>
       </c>
@@ -20415,7 +20419,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>137</v>
       </c>
@@ -20452,7 +20456,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>138</v>
       </c>
@@ -20489,7 +20493,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>139</v>
       </c>
@@ -20526,7 +20530,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>140</v>
       </c>
@@ -20563,7 +20567,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>141</v>
       </c>
@@ -20600,7 +20604,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>142</v>
       </c>
@@ -20637,7 +20641,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>143</v>
       </c>
@@ -20674,7 +20678,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>144</v>
       </c>
@@ -20711,7 +20715,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>145</v>
       </c>
@@ -20748,7 +20752,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>146</v>
       </c>
@@ -20785,7 +20789,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>147</v>
       </c>
@@ -20822,7 +20826,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>148</v>
       </c>
@@ -20859,7 +20863,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>149</v>
       </c>
@@ -20896,7 +20900,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>153</v>
       </c>
@@ -20936,7 +20940,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>154</v>
       </c>
@@ -20973,7 +20977,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>155</v>
       </c>
@@ -21010,7 +21014,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>156</v>
       </c>
@@ -21047,7 +21051,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>158</v>
       </c>
@@ -21082,7 +21086,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>159</v>
       </c>
@@ -21119,7 +21123,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>166</v>
       </c>
@@ -21154,7 +21158,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>167</v>
       </c>
@@ -21191,7 +21195,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>170</v>
       </c>
@@ -21226,7 +21230,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>171</v>
       </c>
@@ -21267,7 +21271,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>172</v>
       </c>
@@ -21308,7 +21312,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>173</v>
       </c>
@@ -21347,7 +21351,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>174</v>
       </c>
@@ -21386,7 +21390,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>175</v>
       </c>
@@ -21425,7 +21429,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>176</v>
       </c>
@@ -21464,7 +21468,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>177</v>
       </c>
@@ -21504,7 +21508,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>178</v>
       </c>
@@ -21544,7 +21548,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>179</v>
       </c>
@@ -21583,7 +21587,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>180</v>
       </c>
@@ -21623,7 +21627,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>182</v>
       </c>
@@ -21663,7 +21667,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>183</v>
       </c>
@@ -21700,7 +21704,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>185</v>
       </c>
@@ -21737,7 +21741,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>187</v>
       </c>
@@ -21774,7 +21778,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>189</v>
       </c>
@@ -21811,7 +21815,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>192</v>
       </c>
@@ -21848,7 +21852,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>193</v>
       </c>
@@ -21887,7 +21891,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>194</v>
       </c>
@@ -21926,7 +21930,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>196</v>
       </c>
@@ -21965,7 +21969,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>197</v>
       </c>
@@ -22002,7 +22006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>199</v>
       </c>
@@ -22039,7 +22043,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>200</v>
       </c>
@@ -22076,7 +22080,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>202</v>
       </c>
@@ -22113,7 +22117,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>203</v>
       </c>
@@ -22150,7 +22154,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>204</v>
       </c>
@@ -22187,7 +22191,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>205</v>
       </c>
@@ -22227,7 +22231,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>206</v>
       </c>
@@ -22267,7 +22271,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="357" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="357" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>207</v>
       </c>
@@ -22307,7 +22311,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>208</v>
       </c>
@@ -22344,7 +22348,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>209</v>
       </c>
@@ -22381,7 +22385,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>210</v>
       </c>
@@ -22422,7 +22426,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>211</v>
       </c>
@@ -22463,7 +22467,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -22504,7 +22508,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>213</v>
       </c>
@@ -22542,7 +22546,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>214</v>
       </c>
@@ -22580,7 +22584,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>221</v>
       </c>
@@ -22621,7 +22625,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>222</v>
       </c>
@@ -22662,7 +22666,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>223</v>
       </c>
@@ -22697,7 +22701,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>224</v>
       </c>
@@ -22735,7 +22739,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>225</v>
       </c>
@@ -22776,7 +22780,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>227</v>
       </c>
@@ -22814,7 +22818,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>228</v>
       </c>
@@ -22852,7 +22856,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>231</v>
       </c>
@@ -22890,7 +22894,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>232</v>
       </c>
@@ -22931,7 +22935,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>233</v>
       </c>
@@ -22972,7 +22976,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>234</v>
       </c>
@@ -23013,7 +23017,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>235</v>
       </c>
@@ -23054,7 +23058,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>236</v>
       </c>
@@ -23089,7 +23093,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>237</v>
       </c>
@@ -23124,7 +23128,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>238</v>
       </c>
@@ -23159,7 +23163,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>239</v>
       </c>
@@ -23197,7 +23201,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>240</v>
       </c>
@@ -23235,7 +23239,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>241</v>
       </c>
@@ -23270,7 +23274,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>242</v>
       </c>
@@ -23308,7 +23312,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>243</v>
       </c>
@@ -23343,7 +23347,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>244</v>
       </c>
@@ -23381,7 +23385,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>245</v>
       </c>
@@ -23422,7 +23426,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>246</v>
       </c>
@@ -23457,7 +23461,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>247</v>
       </c>
@@ -23492,7 +23496,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>248</v>
       </c>
@@ -23535,7 +23539,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>249</v>
       </c>
@@ -23570,7 +23574,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>250</v>
       </c>
@@ -23605,7 +23609,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>251</v>
       </c>
@@ -23640,7 +23644,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>252</v>
       </c>
@@ -23675,7 +23679,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>253</v>
       </c>
@@ -23713,7 +23717,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>256</v>
       </c>
@@ -23751,7 +23755,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="179" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>257</v>
       </c>
@@ -23786,7 +23790,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>258</v>
       </c>
@@ -23821,7 +23825,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>259</v>
       </c>
@@ -23856,7 +23860,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>260</v>
       </c>
@@ -23897,7 +23901,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>261</v>
       </c>
@@ -23932,7 +23936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>262</v>
       </c>
@@ -23967,7 +23971,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>263</v>
       </c>
@@ -24002,7 +24006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>264</v>
       </c>
@@ -24037,7 +24041,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>274</v>
       </c>
@@ -24070,7 +24074,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>275</v>
       </c>
@@ -24103,7 +24107,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>276</v>
       </c>
@@ -24136,7 +24140,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>277</v>
       </c>
@@ -24169,7 +24173,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>278</v>
       </c>
@@ -24202,7 +24206,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>279</v>
       </c>
@@ -24235,7 +24239,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>280</v>
       </c>
@@ -24268,7 +24272,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>281</v>
       </c>
@@ -24301,7 +24305,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>282</v>
       </c>
@@ -24334,7 +24338,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>283</v>
       </c>
@@ -24367,7 +24371,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>284</v>
       </c>
@@ -24400,7 +24404,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>285</v>
       </c>
@@ -24433,7 +24437,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>286</v>
       </c>
@@ -24468,7 +24472,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>287</v>
       </c>
@@ -24503,7 +24507,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>288</v>
       </c>
@@ -24538,7 +24542,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>289</v>
       </c>
@@ -24573,7 +24577,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>290</v>
       </c>
@@ -24608,7 +24612,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>291</v>
       </c>
@@ -24643,7 +24647,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>292</v>
       </c>
@@ -24678,7 +24682,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>295</v>
       </c>
@@ -24713,7 +24717,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>296</v>
       </c>
@@ -24748,7 +24752,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>297</v>
       </c>
@@ -24783,7 +24787,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>298</v>
       </c>
@@ -24818,7 +24822,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>299</v>
       </c>
@@ -24853,7 +24857,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>300</v>
       </c>
@@ -24888,7 +24892,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>301</v>
       </c>
@@ -24923,7 +24927,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>302</v>
       </c>
@@ -24958,7 +24962,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>303</v>
       </c>
@@ -24993,7 +24997,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>304</v>
       </c>
@@ -25028,7 +25032,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>305</v>
       </c>
@@ -25063,7 +25067,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>306</v>
       </c>
@@ -25098,7 +25102,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>307</v>
       </c>
@@ -25133,7 +25137,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>308</v>
       </c>
@@ -25168,7 +25172,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>309</v>
       </c>
@@ -25203,7 +25207,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>310</v>
       </c>
@@ -25238,7 +25242,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>311</v>
       </c>
@@ -25276,7 +25280,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>312</v>
       </c>
@@ -25314,7 +25318,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="53">
         <v>313</v>
       </c>
@@ -25356,7 +25360,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>314</v>
       </c>
@@ -25391,7 +25395,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>315</v>
       </c>
@@ -25426,7 +25430,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>316</v>
       </c>
@@ -25461,7 +25465,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>317</v>
       </c>
@@ -25496,7 +25500,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>318</v>
       </c>
@@ -25531,7 +25535,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>319</v>
       </c>
@@ -25566,7 +25570,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>320</v>
       </c>
@@ -25601,7 +25605,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>321</v>
       </c>
@@ -25636,7 +25640,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>322</v>
       </c>
@@ -25669,7 +25673,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="234" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>323</v>
       </c>
@@ -25702,7 +25706,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>324</v>
       </c>
@@ -25741,7 +25745,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>325</v>
       </c>
@@ -25780,7 +25784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>328</v>
       </c>
@@ -25819,7 +25823,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>329</v>
       </c>
@@ -25858,7 +25862,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>331</v>
       </c>
@@ -25897,7 +25901,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>332</v>
       </c>
@@ -25932,7 +25936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>333</v>
       </c>
@@ -25970,7 +25974,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>334</v>
       </c>
@@ -26005,7 +26009,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>335</v>
       </c>
@@ -26043,7 +26047,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>336</v>
       </c>
@@ -26081,7 +26085,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>337</v>
       </c>
@@ -26119,7 +26123,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>338</v>
       </c>
@@ -26154,7 +26158,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>339</v>
       </c>
@@ -26189,7 +26193,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>341</v>
       </c>
@@ -26227,7 +26231,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>342</v>
       </c>
@@ -26265,7 +26269,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>343</v>
       </c>
@@ -26300,7 +26304,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>344</v>
       </c>
@@ -26335,7 +26339,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>345</v>
       </c>
@@ -26373,7 +26377,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>346</v>
       </c>
@@ -26411,7 +26415,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>347</v>
       </c>
@@ -26446,7 +26450,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>348</v>
       </c>
@@ -26484,7 +26488,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>349</v>
       </c>
@@ -26522,7 +26526,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>350</v>
       </c>
@@ -26557,7 +26561,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>351</v>
       </c>
@@ -26592,7 +26596,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="53">
         <v>352</v>
       </c>
@@ -26634,7 +26638,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>354</v>
       </c>
@@ -26669,7 +26673,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>355</v>
       </c>
@@ -26704,7 +26708,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>356</v>
       </c>
@@ -26745,7 +26749,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>359</v>
       </c>
@@ -26780,7 +26784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>360</v>
       </c>
@@ -26815,7 +26819,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>362</v>
       </c>
@@ -26850,7 +26854,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>363</v>
       </c>
@@ -26885,7 +26889,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>364</v>
       </c>
@@ -26920,7 +26924,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>365</v>
       </c>
@@ -26955,7 +26959,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>366</v>
       </c>
@@ -26993,7 +26997,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>367</v>
       </c>
@@ -27031,7 +27035,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>368</v>
       </c>
@@ -27069,7 +27073,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>369</v>
       </c>
@@ -27104,7 +27108,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>370</v>
       </c>
@@ -27139,7 +27143,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>371</v>
       </c>
@@ -27177,7 +27181,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>372</v>
       </c>
@@ -27215,7 +27219,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>373</v>
       </c>
@@ -27250,7 +27254,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>374</v>
       </c>
@@ -27285,7 +27289,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>375</v>
       </c>
@@ -27320,7 +27324,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>376</v>
       </c>
@@ -27355,7 +27359,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>377</v>
       </c>
@@ -27390,7 +27394,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>378</v>
       </c>
@@ -27425,7 +27429,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>379</v>
       </c>
@@ -27460,7 +27464,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>380</v>
       </c>
@@ -27495,7 +27499,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>381</v>
       </c>
@@ -27530,7 +27534,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>382</v>
       </c>
@@ -27565,7 +27569,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="53">
         <v>385</v>
       </c>
@@ -27607,7 +27611,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>386</v>
       </c>
@@ -27643,7 +27647,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="53">
         <v>387</v>
       </c>
@@ -27685,7 +27689,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>388</v>
       </c>
@@ -27726,7 +27730,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>389</v>
       </c>
@@ -27761,7 +27765,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="53">
         <v>390</v>
       </c>
@@ -27805,7 +27809,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>391</v>
       </c>
@@ -27840,7 +27844,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>392</v>
       </c>
@@ -27881,7 +27885,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>393</v>
       </c>
@@ -27916,7 +27920,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>394</v>
       </c>
@@ -27957,7 +27961,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>395</v>
       </c>
@@ -27998,7 +28002,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>396</v>
       </c>
@@ -28033,7 +28037,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>397</v>
       </c>
@@ -28074,7 +28078,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="299" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>398</v>
       </c>
@@ -28109,7 +28113,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>399</v>
       </c>
@@ -28144,7 +28148,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="301" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>400</v>
       </c>
@@ -28179,7 +28183,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>401</v>
       </c>
@@ -28220,7 +28224,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="303" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>402</v>
       </c>
@@ -28257,7 +28261,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="304" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>403</v>
       </c>
@@ -28294,7 +28298,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>404</v>
       </c>
@@ -28331,7 +28335,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>405</v>
       </c>
@@ -28368,7 +28372,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>406</v>
       </c>
@@ -28405,7 +28409,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>407</v>
       </c>
@@ -28442,7 +28446,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>408</v>
       </c>
@@ -28479,7 +28483,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="310" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>409</v>
       </c>
@@ -28516,7 +28520,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>410</v>
       </c>
@@ -28553,7 +28557,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>411</v>
       </c>
@@ -28590,7 +28594,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>412</v>
       </c>
@@ -28627,7 +28631,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>413</v>
       </c>
@@ -28662,7 +28666,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>415</v>
       </c>
@@ -28697,7 +28701,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>417</v>
       </c>
@@ -28734,7 +28738,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>418</v>
       </c>
@@ -28771,7 +28775,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>419</v>
       </c>
@@ -28808,7 +28812,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>420</v>
       </c>
@@ -28845,7 +28849,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>421</v>
       </c>
@@ -28882,7 +28886,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>422</v>
       </c>
@@ -28919,7 +28923,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>423</v>
       </c>
@@ -28956,7 +28960,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="323" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>424</v>
       </c>
@@ -28993,7 +28997,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>426</v>
       </c>
@@ -29028,7 +29032,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>427</v>
       </c>
@@ -29063,7 +29067,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>429</v>
       </c>
@@ -29100,7 +29104,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>430</v>
       </c>
@@ -29137,7 +29141,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>431</v>
       </c>
@@ -29174,7 +29178,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>432</v>
       </c>
@@ -29211,7 +29215,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>433</v>
       </c>
@@ -29248,7 +29252,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>434</v>
       </c>
@@ -29285,7 +29289,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1">
         <v>435</v>
       </c>
@@ -29320,7 +29324,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1">
         <v>436</v>
       </c>
@@ -29355,7 +29359,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="1">
         <v>437</v>
       </c>
@@ -29390,7 +29394,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="1">
         <v>440</v>
       </c>
@@ -29427,7 +29431,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>441</v>
       </c>
@@ -29468,7 +29472,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="337" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="1">
         <v>442</v>
       </c>
@@ -29505,7 +29509,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="338" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>443</v>
       </c>
@@ -29542,7 +29546,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="339" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="1">
         <v>444</v>
       </c>
@@ -29579,7 +29583,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="340" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>445</v>
       </c>
@@ -29616,7 +29620,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="341" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="1">
         <v>448</v>
       </c>
@@ -29653,7 +29657,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="342" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="1">
         <v>449</v>
       </c>
@@ -29690,7 +29694,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="343" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
         <v>450</v>
       </c>
@@ -29727,7 +29731,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="344" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
         <v>451</v>
       </c>
@@ -29764,7 +29768,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="1">
         <v>452</v>
       </c>
@@ -29801,7 +29805,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="346" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="1">
         <v>453</v>
       </c>
@@ -29838,7 +29842,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="347" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="1">
         <v>455</v>
       </c>
@@ -29875,7 +29879,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="348" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>456</v>
       </c>
@@ -29912,7 +29916,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>457</v>
       </c>
@@ -29953,7 +29957,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="350" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="1">
         <v>458</v>
       </c>
@@ -29990,7 +29994,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="351" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>459</v>
       </c>
@@ -30027,7 +30031,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="352" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="1">
         <v>460</v>
       </c>
@@ -30064,7 +30068,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="1">
         <v>461</v>
       </c>
@@ -30101,7 +30105,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="1">
         <v>463</v>
       </c>
@@ -30138,7 +30142,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="1">
         <v>464</v>
       </c>
@@ -30175,7 +30179,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="1">
         <v>465</v>
       </c>
@@ -30212,7 +30216,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="357" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="1">
         <v>469</v>
       </c>
@@ -30249,7 +30253,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="1">
         <v>470</v>
       </c>
@@ -30286,7 +30290,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="1">
         <v>471</v>
       </c>
@@ -30323,7 +30327,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="1">
         <v>472</v>
       </c>
@@ -30360,7 +30364,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="1">
         <v>473</v>
       </c>
@@ -30397,7 +30401,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>474</v>
       </c>
@@ -30434,7 +30438,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="1">
         <v>475</v>
       </c>
@@ -30471,7 +30475,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
         <v>476</v>
       </c>
@@ -30508,7 +30512,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="1">
         <v>477</v>
       </c>
@@ -30545,7 +30549,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="1">
         <v>479</v>
       </c>
@@ -30580,7 +30584,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="1">
         <v>480</v>
       </c>
@@ -30615,7 +30619,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="1">
         <v>481</v>
       </c>
@@ -30650,7 +30654,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="330.6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:16" ht="330.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="1">
         <v>482</v>
       </c>
@@ -30685,7 +30689,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="1">
         <v>483</v>
       </c>
@@ -30722,7 +30726,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="1">
         <v>484</v>
       </c>
@@ -30757,7 +30761,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="1">
         <v>485</v>
       </c>
@@ -30792,7 +30796,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="1">
         <v>486</v>
       </c>
@@ -30827,7 +30831,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="1">
         <v>487</v>
       </c>
@@ -30862,7 +30866,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="1">
         <v>489</v>
       </c>
@@ -30897,7 +30901,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" s="1">
         <v>490</v>
       </c>
@@ -30932,7 +30936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="1">
         <v>491</v>
       </c>
@@ -30967,7 +30971,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" s="1">
         <v>492</v>
       </c>
@@ -31002,7 +31006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="1">
         <v>493</v>
       </c>
@@ -31037,7 +31041,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="291" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="1">
         <v>494</v>
       </c>
@@ -31072,7 +31076,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" s="1">
         <v>495</v>
       </c>
@@ -31107,7 +31111,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" s="1">
         <v>498</v>
       </c>
@@ -31142,7 +31146,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="1">
         <v>499</v>
       </c>
@@ -31177,7 +31181,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="1">
         <v>500</v>
       </c>
@@ -31212,7 +31216,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="1">
         <v>501</v>
       </c>
@@ -31247,7 +31251,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="1">
         <v>503</v>
       </c>
@@ -31282,7 +31286,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
         <v>504</v>
       </c>
@@ -31317,7 +31321,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="1">
         <v>505</v>
       </c>
@@ -31352,7 +31356,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>506</v>
       </c>
@@ -31385,7 +31389,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="390" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="1">
         <v>507</v>
       </c>
@@ -31416,7 +31420,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="391" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>508</v>
       </c>
@@ -31449,7 +31453,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="1">
         <v>509</v>
       </c>
@@ -31497,8 +31501,12 @@
       <c r="B393" s="18" t="s">
         <v>831</v>
       </c>
-      <c r="C393" s="18"/>
-      <c r="D393" s="18"/>
+      <c r="C393" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D393" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F393" s="18" t="s">
         <v>1102</v>
       </c>
@@ -31529,8 +31537,12 @@
     </row>
     <row r="394" spans="1:16" ht="343.8" x14ac:dyDescent="0.3">
       <c r="B394" s="18"/>
-      <c r="C394" s="18"/>
-      <c r="D394" s="18"/>
+      <c r="C394" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D394" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F394" s="18"/>
       <c r="G394" s="18"/>
       <c r="H394" s="18" t="s">
@@ -31553,8 +31565,12 @@
     </row>
     <row r="395" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="B395" s="18"/>
-      <c r="C395" s="18"/>
-      <c r="D395" s="18"/>
+      <c r="C395" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D395" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F395" s="18"/>
       <c r="G395" s="18" t="s">
         <v>2251</v>
@@ -31577,7 +31593,7 @@
       <c r="O395" s="18"/>
       <c r="P395" s="18"/>
     </row>
-    <row r="396" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="1">
         <v>511</v>
       </c>
@@ -31614,7 +31630,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="1">
         <v>512</v>
       </c>
@@ -31651,7 +31667,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" s="1">
         <v>513</v>
       </c>
@@ -31688,7 +31704,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
         <v>514</v>
       </c>
@@ -31725,7 +31741,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>515</v>
       </c>
@@ -31769,8 +31785,12 @@
       <c r="B401" s="18" t="s">
         <v>809</v>
       </c>
-      <c r="C401" s="18"/>
-      <c r="D401" s="18"/>
+      <c r="C401" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D401" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F401" s="18" t="s">
         <v>1102</v>
       </c>
@@ -31785,7 +31805,7 @@
         <v>2256</v>
       </c>
       <c r="K401" s="18" t="s">
-        <v>2259</v>
+        <v>2260</v>
       </c>
       <c r="L401" s="18" t="s">
         <v>693</v>
@@ -31803,8 +31823,12 @@
       <c r="B402" s="18" t="s">
         <v>2252</v>
       </c>
-      <c r="C402" s="18"/>
-      <c r="D402" s="18"/>
+      <c r="C402" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D402" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F402" s="18"/>
       <c r="G402" s="18"/>
       <c r="H402" s="18" t="s">
@@ -31825,7 +31849,7 @@
       <c r="O402" s="18"/>
       <c r="P402" s="18"/>
     </row>
-    <row r="403" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B403" s="18" t="s">
         <v>2253</v>
       </c>
@@ -31851,7 +31875,7 @@
       <c r="O403" s="18"/>
       <c r="P403" s="18"/>
     </row>
-    <row r="404" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>517</v>
       </c>
@@ -31888,7 +31912,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>518</v>
       </c>
@@ -31925,7 +31949,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="406" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>529</v>
       </c>
@@ -31962,7 +31986,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="407" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>541</v>
       </c>
@@ -31995,7 +32019,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="408" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>547</v>
       </c>
@@ -32028,7 +32052,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="409" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>548</v>
       </c>
@@ -32061,7 +32085,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="410" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>564</v>
       </c>
@@ -32098,7 +32122,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="411" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>565</v>
       </c>
@@ -32135,7 +32159,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="412" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>570</v>
       </c>
@@ -32172,7 +32196,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="413" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>571</v>
       </c>
@@ -32213,7 +32237,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="414" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" s="1">
         <v>574</v>
       </c>
@@ -32250,7 +32274,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="415" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" s="1">
         <v>575</v>
       </c>
@@ -32287,7 +32311,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="416" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" s="1">
         <v>576</v>
       </c>
@@ -32324,7 +32348,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="417" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417" s="1">
         <v>577</v>
       </c>
@@ -32361,7 +32385,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="418" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418" s="1">
         <v>580</v>
       </c>
@@ -32398,7 +32422,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="419" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419" s="1">
         <v>581</v>
       </c>
@@ -32435,7 +32459,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="420" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>582</v>
       </c>
@@ -32470,7 +32494,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="421" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>583</v>
       </c>
@@ -32505,7 +32529,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="422" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" s="1">
         <v>584</v>
       </c>
@@ -32540,7 +32564,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="423" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
         <v>585</v>
       </c>
@@ -32575,7 +32599,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="424" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
         <v>586</v>
       </c>
@@ -32610,7 +32634,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="425" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>587</v>
       </c>
@@ -32647,7 +32671,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="426" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" s="1">
         <v>588</v>
       </c>
@@ -32682,7 +32706,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="427" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>589</v>
       </c>
@@ -32717,7 +32741,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="428" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
         <v>590</v>
       </c>
@@ -32752,7 +32776,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="429" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>591</v>
       </c>
@@ -32787,7 +32811,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="430" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>592</v>
       </c>
@@ -32822,7 +32846,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="431" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>593</v>
       </c>
@@ -32857,7 +32881,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="432" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>594</v>
       </c>
@@ -32892,7 +32916,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="433" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>595</v>
       </c>
@@ -32927,7 +32951,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="434" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>596</v>
       </c>
@@ -32962,7 +32986,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="435" spans="1:16" ht="225" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>597</v>
       </c>
@@ -32997,7 +33021,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="436" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>598</v>
       </c>
@@ -33034,7 +33058,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="437" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>599</v>
       </c>
@@ -33071,7 +33095,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="438" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>600</v>
       </c>
@@ -33106,7 +33130,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="439" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>601</v>
       </c>
@@ -33141,7 +33165,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="440" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>602</v>
       </c>
@@ -33178,7 +33202,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="441" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="1">
         <v>603</v>
       </c>
@@ -33215,7 +33239,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="442" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" s="1">
         <v>604</v>
       </c>
@@ -33252,7 +33276,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="443" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>605</v>
       </c>
@@ -33287,7 +33311,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="444" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" s="1">
         <v>606</v>
       </c>
@@ -33322,7 +33346,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="445" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445" s="1">
         <v>607</v>
       </c>
@@ -33357,7 +33381,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="446" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" s="1">
         <v>608</v>
       </c>
@@ -33393,7 +33417,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P446"/>
+  <autoFilter ref="A1:P446">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Sprint 15 Sep - 22 Sep"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Ankit"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
commit last sprint test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5608" uniqueCount="2261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5611" uniqueCount="2262">
   <si>
     <t>Name</t>
   </si>
@@ -11497,6 +11497,9 @@
 b.Close menu &amp; return to full-screen media (TV);
 stream not affected
 </t>
+  </si>
+  <si>
+    <t>Sprint 22 Sep - 29 Sep</t>
   </si>
 </sst>
 </file>
@@ -11866,7 +11869,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -11950,9 +11952,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -12004,7 +12004,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17038,9 +17037,9 @@
   <dimension ref="A1:P446"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A401" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K401" sqref="K401"/>
+      <selection pane="bottomLeft" activeCell="K292" sqref="K292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22311,7 +22310,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>208</v>
       </c>
@@ -22348,7 +22347,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>209</v>
       </c>
@@ -23644,7 +23643,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>252</v>
       </c>
@@ -26889,7 +26888,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>364</v>
       </c>
@@ -27464,7 +27463,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>380</v>
       </c>
@@ -27809,7 +27808,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>391</v>
       </c>
@@ -28002,7 +28001,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>396</v>
       </c>
@@ -28113,7 +28112,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>399</v>
       </c>
@@ -30401,7 +30400,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>474</v>
       </c>
@@ -31494,7 +31493,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="277.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="277.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>510</v>
       </c>
@@ -31535,7 +31534,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="343.8" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="343.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B394" s="18"/>
       <c r="C394" s="18" t="s">
         <v>496</v>
@@ -31563,7 +31562,7 @@
       <c r="O394" s="18"/>
       <c r="P394" s="18"/>
     </row>
-    <row r="395" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B395" s="18"/>
       <c r="C395" s="18" t="s">
         <v>496</v>
@@ -31778,7 +31777,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>516</v>
       </c>
@@ -31819,7 +31818,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="396.6" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="396.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B402" s="18" t="s">
         <v>2252</v>
       </c>
@@ -31849,13 +31848,19 @@
       <c r="O402" s="18"/>
       <c r="P402" s="18"/>
     </row>
-    <row r="403" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="B403" s="18" t="s">
         <v>2253</v>
       </c>
-      <c r="C403" s="18"/>
-      <c r="D403" s="18"/>
-      <c r="F403" s="18"/>
+      <c r="C403" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D403" s="18" t="s">
+        <v>2261</v>
+      </c>
+      <c r="F403" s="18" t="s">
+        <v>1102</v>
+      </c>
       <c r="G403" s="18"/>
       <c r="H403" s="18" t="s">
         <v>604</v>
@@ -31875,7 +31880,7 @@
       <c r="O403" s="18"/>
       <c r="P403" s="18"/>
     </row>
-    <row r="404" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>517</v>
       </c>
@@ -31912,7 +31917,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>518</v>
       </c>
@@ -31986,7 +31991,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="407" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>541</v>
       </c>
@@ -32019,7 +32024,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="408" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>547</v>
       </c>
@@ -33418,9 +33423,18 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P446">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
     <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="5">
       <filters>
-        <filter val="Sprint 15 Sep - 22 Sep"/>
+        <filter val="Yes"/>
       </filters>
     </filterColumn>
     <filterColumn colId="7">

</xml_diff>

<commit_message>
commit Test case of current sprint and comment code for Reboot STB
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5611" uniqueCount="2262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="2264">
   <si>
     <t>Name</t>
   </si>
@@ -11500,6 +11500,12 @@
   </si>
   <si>
     <t>Sprint 22 Sep - 29 Sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some moviw does not contain subtitle and version , so we does not include as a part of automation </t>
+  </si>
+  <si>
+    <t>Sprint</t>
   </si>
 </sst>
 </file>
@@ -17036,10 +17042,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K292" sqref="K292"/>
+      <selection pane="bottomLeft" activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26895,10 +26901,18 @@
       <c r="B267" s="18" t="s">
         <v>1226</v>
       </c>
+      <c r="C267" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>2263</v>
+      </c>
       <c r="F267" s="18" t="s">
         <v>1102</v>
       </c>
-      <c r="G267" s="18"/>
+      <c r="G267" s="18" t="s">
+        <v>2262</v>
+      </c>
       <c r="H267" s="18" t="s">
         <v>604</v>
       </c>
@@ -27808,12 +27822,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>391</v>
       </c>
       <c r="B292" s="21" t="s">
         <v>1142</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D292" s="18" t="s">
+        <v>2261</v>
       </c>
       <c r="F292" s="18" t="s">
         <v>1102</v>
@@ -30400,7 +30420,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>474</v>
       </c>
@@ -31848,7 +31868,7 @@
       <c r="O402" s="18"/>
       <c r="P402" s="18"/>
     </row>
-    <row r="403" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B403" s="18" t="s">
         <v>2253</v>
       </c>
@@ -31880,15 +31900,19 @@
       <c r="O403" s="18"/>
       <c r="P403" s="18"/>
     </row>
-    <row r="404" spans="1:16" ht="159" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>517</v>
       </c>
       <c r="B404" s="21" t="s">
         <v>807</v>
       </c>
-      <c r="C404" s="27"/>
-      <c r="D404" s="27"/>
+      <c r="C404" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D404" s="18" t="s">
+        <v>2261</v>
+      </c>
       <c r="F404" s="21" t="s">
         <v>1102</v>
       </c>
@@ -31917,7 +31941,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>518</v>
       </c>
@@ -31931,7 +31955,7 @@
       </c>
       <c r="G405" s="18"/>
       <c r="H405" s="18" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="I405" s="18" t="s">
         <v>802</v>

</xml_diff>

<commit_message>
commit bug fixes in regression
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
+    <workbookView minimized="1" xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -17042,10 +17042,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P446"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="C267" sqref="C267"/>
+      <selection pane="bottomLeft" activeCell="J144" sqref="J144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22390,7 +22390,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>210</v>
       </c>
@@ -22431,7 +22431,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>211</v>
       </c>
@@ -22472,7 +22472,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -22589,7 +22589,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>221</v>
       </c>
@@ -22630,7 +22630,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>222</v>
       </c>
@@ -23501,7 +23501,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>248</v>
       </c>
@@ -23865,7 +23865,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>260</v>
       </c>
@@ -25323,7 +25323,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A224" s="53">
         <v>313</v>
       </c>
@@ -26601,7 +26601,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A259" s="53">
         <v>352</v>
       </c>
@@ -27582,7 +27582,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A286" s="53">
         <v>385</v>
       </c>
@@ -27660,7 +27660,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A288" s="53">
         <v>387</v>
       </c>
@@ -27702,7 +27702,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>388</v>
       </c>
@@ -27778,7 +27778,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A291" s="53">
         <v>390</v>
       </c>
@@ -27939,7 +27939,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>394</v>
       </c>
@@ -27980,7 +27980,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>395</v>
       </c>
@@ -28056,7 +28056,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>397</v>
       </c>
@@ -28202,7 +28202,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>401</v>
       </c>
@@ -31513,7 +31513,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="277.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="277.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>510</v>
       </c>
@@ -31554,7 +31554,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="343.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="343.8" x14ac:dyDescent="0.3">
       <c r="B394" s="18"/>
       <c r="C394" s="18" t="s">
         <v>496</v>
@@ -31582,7 +31582,7 @@
       <c r="O394" s="18"/>
       <c r="P394" s="18"/>
     </row>
-    <row r="395" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="B395" s="18"/>
       <c r="C395" s="18" t="s">
         <v>496</v>
@@ -31797,7 +31797,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>516</v>
       </c>
@@ -31838,7 +31838,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="396.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="396.6" x14ac:dyDescent="0.3">
       <c r="B402" s="18" t="s">
         <v>2252</v>
       </c>
@@ -33447,10 +33447,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P446">
-    <filterColumn colId="3">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Sprint"/>
-        <filter val="Sprint 22 Sep - 29 Sep"/>
+        <filter val="Completed"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Ankit"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
commit this week test cases
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="21072" windowHeight="8892" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Automation_Status" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="2264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="2263">
   <si>
     <t>Name</t>
   </si>
@@ -11500,9 +11500,6 @@
   </si>
   <si>
     <t>Sprint 22 Sep - 29 Sep</t>
-  </si>
-  <si>
-    <t>Sprint</t>
   </si>
   <si>
     <t xml:space="preserve">Some movie does not contain subtitle and version , so we does not include as a part of automation </t>
@@ -17042,10 +17039,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="J144" sqref="J144"/>
+      <selection pane="bottomLeft" activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22390,7 +22387,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>210</v>
       </c>
@@ -22431,7 +22428,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>211</v>
       </c>
@@ -22472,7 +22469,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -22589,7 +22586,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>221</v>
       </c>
@@ -22630,7 +22627,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>222</v>
       </c>
@@ -23501,7 +23498,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>248</v>
       </c>
@@ -23865,7 +23862,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>260</v>
       </c>
@@ -25323,7 +25320,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="53">
         <v>313</v>
       </c>
@@ -26601,7 +26598,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="53">
         <v>352</v>
       </c>
@@ -26904,14 +26901,14 @@
       <c r="C267" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="D267" s="1" t="s">
-        <v>2262</v>
+      <c r="D267" s="18" t="s">
+        <v>2261</v>
       </c>
       <c r="F267" s="18" t="s">
         <v>1102</v>
       </c>
       <c r="G267" s="18" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="H267" s="18" t="s">
         <v>604</v>
@@ -27582,7 +27579,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="53">
         <v>385</v>
       </c>
@@ -27660,7 +27657,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="93" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="53">
         <v>387</v>
       </c>
@@ -27702,7 +27699,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>388</v>
       </c>
@@ -27778,7 +27775,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="53">
         <v>390</v>
       </c>
@@ -27939,7 +27936,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>394</v>
       </c>
@@ -27980,7 +27977,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>395</v>
       </c>
@@ -28056,7 +28053,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>397</v>
       </c>
@@ -28202,7 +28199,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="27" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>401</v>
       </c>
@@ -31513,7 +31510,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="277.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="277.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>510</v>
       </c>
@@ -31554,7 +31551,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="343.8" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="343.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B394" s="18"/>
       <c r="C394" s="18" t="s">
         <v>496</v>
@@ -31582,7 +31579,7 @@
       <c r="O394" s="18"/>
       <c r="P394" s="18"/>
     </row>
-    <row r="395" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B395" s="18"/>
       <c r="C395" s="18" t="s">
         <v>496</v>
@@ -31797,7 +31794,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>516</v>
       </c>
@@ -31838,7 +31835,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="396.6" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="396.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B402" s="18" t="s">
         <v>2252</v>
       </c>
@@ -33447,14 +33444,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P446">
-    <filterColumn colId="2">
+    <filterColumn colId="3">
       <filters>
-        <filter val="Completed"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Ankit"/>
+        <filter val="Sprint"/>
+        <filter val="Sprint 22 Sep - 29 Sep"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
commit Test case completion status
</commit_message>
<xml_diff>
--- a/TestCases/TestCaseSheet.xlsx
+++ b/TestCases/TestCaseSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Desktop\Rahul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="2263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5643" uniqueCount="2264">
   <si>
     <t>Name</t>
   </si>
@@ -11503,6 +11503,9 @@
   </si>
   <si>
     <t xml:space="preserve">Some movie does not contain subtitle and version , so we does not include as a part of automation </t>
+  </si>
+  <si>
+    <t>Sprint 3 Oct - 7 Oct</t>
   </si>
 </sst>
 </file>
@@ -17036,13 +17039,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="C267" sqref="C267"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17114,7 +17116,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -17151,7 +17153,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -17188,7 +17190,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>41</v>
       </c>
@@ -17225,7 +17227,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42</v>
       </c>
@@ -17262,7 +17264,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43</v>
       </c>
@@ -17299,7 +17301,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44</v>
       </c>
@@ -17336,7 +17338,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45</v>
       </c>
@@ -17373,7 +17375,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>46</v>
       </c>
@@ -17410,7 +17412,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>47</v>
       </c>
@@ -17447,7 +17449,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>48</v>
       </c>
@@ -17482,7 +17484,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>49</v>
       </c>
@@ -17517,7 +17519,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>54</v>
       </c>
@@ -17554,7 +17556,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>55</v>
       </c>
@@ -17591,7 +17593,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>56</v>
       </c>
@@ -17628,7 +17630,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>57</v>
       </c>
@@ -17665,7 +17667,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>58</v>
       </c>
@@ -17702,7 +17704,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>59</v>
       </c>
@@ -17739,7 +17741,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>60</v>
       </c>
@@ -17776,7 +17778,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -17813,7 +17815,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>62</v>
       </c>
@@ -17850,7 +17852,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>63</v>
       </c>
@@ -17887,7 +17889,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>64</v>
       </c>
@@ -17924,7 +17926,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>65</v>
       </c>
@@ -17961,7 +17963,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>67</v>
       </c>
@@ -17998,7 +18000,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>68</v>
       </c>
@@ -18035,7 +18037,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>69</v>
       </c>
@@ -18072,7 +18074,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -18109,7 +18111,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>71</v>
       </c>
@@ -18146,7 +18148,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>72</v>
       </c>
@@ -18183,7 +18185,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>73</v>
       </c>
@@ -18220,7 +18222,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>74</v>
       </c>
@@ -18257,7 +18259,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>75</v>
       </c>
@@ -18294,7 +18296,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>76</v>
       </c>
@@ -18331,7 +18333,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>77</v>
       </c>
@@ -18368,7 +18370,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>78</v>
       </c>
@@ -18405,7 +18407,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>79</v>
       </c>
@@ -18442,7 +18444,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>80</v>
       </c>
@@ -18479,7 +18481,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>82</v>
       </c>
@@ -18516,7 +18518,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>83</v>
       </c>
@@ -18553,7 +18555,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>84</v>
       </c>
@@ -18590,7 +18592,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>85</v>
       </c>
@@ -18627,7 +18629,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>86</v>
       </c>
@@ -18664,7 +18666,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>87</v>
       </c>
@@ -18701,7 +18703,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>88</v>
       </c>
@@ -18738,7 +18740,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>89</v>
       </c>
@@ -18775,7 +18777,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>90</v>
       </c>
@@ -18812,7 +18814,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>91</v>
       </c>
@@ -18851,7 +18853,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>92</v>
       </c>
@@ -18890,7 +18892,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>93</v>
       </c>
@@ -18927,7 +18929,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>94</v>
       </c>
@@ -18966,7 +18968,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>95</v>
       </c>
@@ -19005,7 +19007,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>96</v>
       </c>
@@ -19044,7 +19046,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>97</v>
       </c>
@@ -19083,7 +19085,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>98</v>
       </c>
@@ -19122,7 +19124,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>99</v>
       </c>
@@ -19161,7 +19163,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>100</v>
       </c>
@@ -19198,7 +19200,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>101</v>
       </c>
@@ -19235,7 +19237,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>102</v>
       </c>
@@ -19272,7 +19274,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>103</v>
       </c>
@@ -19309,7 +19311,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>104</v>
       </c>
@@ -19346,7 +19348,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>105</v>
       </c>
@@ -19383,7 +19385,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>106</v>
       </c>
@@ -19420,7 +19422,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>107</v>
       </c>
@@ -19457,7 +19459,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>108</v>
       </c>
@@ -19494,7 +19496,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>109</v>
       </c>
@@ -19531,7 +19533,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>110</v>
       </c>
@@ -19568,7 +19570,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>111</v>
       </c>
@@ -19605,7 +19607,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>112</v>
       </c>
@@ -19642,7 +19644,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>113</v>
       </c>
@@ -19679,7 +19681,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>114</v>
       </c>
@@ -19716,7 +19718,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>115</v>
       </c>
@@ -19753,7 +19755,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>116</v>
       </c>
@@ -19790,7 +19792,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>117</v>
       </c>
@@ -19827,7 +19829,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>118</v>
       </c>
@@ -19864,7 +19866,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>119</v>
       </c>
@@ -19901,7 +19903,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>120</v>
       </c>
@@ -19938,7 +19940,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>121</v>
       </c>
@@ -19975,7 +19977,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>122</v>
       </c>
@@ -20012,7 +20014,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>123</v>
       </c>
@@ -20049,7 +20051,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>127</v>
       </c>
@@ -20086,7 +20088,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>128</v>
       </c>
@@ -20123,7 +20125,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>129</v>
       </c>
@@ -20160,7 +20162,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>130</v>
       </c>
@@ -20199,7 +20201,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>131</v>
       </c>
@@ -20236,7 +20238,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>132</v>
       </c>
@@ -20273,7 +20275,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="370.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="370.2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>133</v>
       </c>
@@ -20310,7 +20312,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>134</v>
       </c>
@@ -20347,7 +20349,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>135</v>
       </c>
@@ -20384,7 +20386,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>136</v>
       </c>
@@ -20421,7 +20423,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>137</v>
       </c>
@@ -20458,7 +20460,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>138</v>
       </c>
@@ -20495,7 +20497,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>139</v>
       </c>
@@ -20532,7 +20534,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>140</v>
       </c>
@@ -20569,7 +20571,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>141</v>
       </c>
@@ -20606,7 +20608,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>142</v>
       </c>
@@ -20643,7 +20645,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>143</v>
       </c>
@@ -20680,7 +20682,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>144</v>
       </c>
@@ -20717,7 +20719,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>145</v>
       </c>
@@ -20754,7 +20756,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>146</v>
       </c>
@@ -20791,7 +20793,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>147</v>
       </c>
@@ -20828,7 +20830,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>148</v>
       </c>
@@ -20865,7 +20867,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>149</v>
       </c>
@@ -20902,7 +20904,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="291" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>153</v>
       </c>
@@ -20942,7 +20944,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>154</v>
       </c>
@@ -20979,7 +20981,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>155</v>
       </c>
@@ -21016,7 +21018,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>156</v>
       </c>
@@ -21053,7 +21055,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>158</v>
       </c>
@@ -21088,7 +21090,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>159</v>
       </c>
@@ -21125,7 +21127,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>166</v>
       </c>
@@ -21160,7 +21162,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>167</v>
       </c>
@@ -21197,7 +21199,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>170</v>
       </c>
@@ -21232,7 +21234,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="238.2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>171</v>
       </c>
@@ -21273,7 +21275,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>172</v>
       </c>
@@ -21314,7 +21316,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>173</v>
       </c>
@@ -21353,7 +21355,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>174</v>
       </c>
@@ -21392,7 +21394,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>175</v>
       </c>
@@ -21431,7 +21433,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>176</v>
       </c>
@@ -21470,7 +21472,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>177</v>
       </c>
@@ -21510,7 +21512,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>178</v>
       </c>
@@ -21550,7 +21552,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>179</v>
       </c>
@@ -21589,7 +21591,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>180</v>
       </c>
@@ -21629,7 +21631,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>182</v>
       </c>
@@ -21669,15 +21671,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>183</v>
       </c>
       <c r="B124" s="21" t="s">
         <v>1671</v>
       </c>
-      <c r="C124" s="27"/>
-      <c r="D124" s="27"/>
+      <c r="C124" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D124" s="27" t="s">
+        <v>2259</v>
+      </c>
       <c r="F124" s="21" t="s">
         <v>1102</v>
       </c>
@@ -21706,7 +21712,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>185</v>
       </c>
@@ -21743,15 +21749,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>187</v>
       </c>
       <c r="B126" s="21" t="s">
         <v>1663</v>
       </c>
-      <c r="C126" s="27"/>
-      <c r="D126" s="27"/>
+      <c r="C126" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D126" s="27" t="s">
+        <v>2259</v>
+      </c>
       <c r="F126" s="21" t="s">
         <v>1102</v>
       </c>
@@ -21780,15 +21790,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>189</v>
       </c>
       <c r="B127" s="21" t="s">
         <v>1659</v>
       </c>
-      <c r="C127" s="27"/>
-      <c r="D127" s="27"/>
+      <c r="C127" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D127" s="27" t="s">
+        <v>2259</v>
+      </c>
       <c r="F127" s="21" t="s">
         <v>1102</v>
       </c>
@@ -21817,15 +21831,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>192</v>
       </c>
       <c r="B128" s="18" t="s">
         <v>1655</v>
       </c>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
+      <c r="C128" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D128" s="18" t="s">
+        <v>2259</v>
+      </c>
       <c r="F128" s="18" t="s">
         <v>1102</v>
       </c>
@@ -21854,7 +21872,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>193</v>
       </c>
@@ -21893,7 +21911,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>194</v>
       </c>
@@ -21932,7 +21950,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>196</v>
       </c>
@@ -21971,7 +21989,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>197</v>
       </c>
@@ -22008,7 +22026,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>199</v>
       </c>
@@ -22045,7 +22063,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>200</v>
       </c>
@@ -22082,7 +22100,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>202</v>
       </c>
@@ -22119,7 +22137,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>203</v>
       </c>
@@ -22156,7 +22174,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>204</v>
       </c>
@@ -22193,7 +22211,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>205</v>
       </c>
@@ -22233,7 +22251,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>206</v>
       </c>
@@ -22273,7 +22291,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="357" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="357" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>207</v>
       </c>
@@ -22313,7 +22331,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>208</v>
       </c>
@@ -22350,7 +22368,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>209</v>
       </c>
@@ -22387,7 +22405,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="238.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>210</v>
       </c>
@@ -22428,7 +22446,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>211</v>
       </c>
@@ -22469,7 +22487,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -22510,7 +22528,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>213</v>
       </c>
@@ -22548,7 +22566,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>214</v>
       </c>
@@ -22586,7 +22604,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>221</v>
       </c>
@@ -22627,7 +22645,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>222</v>
       </c>
@@ -22668,7 +22686,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>223</v>
       </c>
@@ -22703,7 +22721,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>224</v>
       </c>
@@ -22741,7 +22759,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>225</v>
       </c>
@@ -22782,7 +22800,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>227</v>
       </c>
@@ -22820,7 +22838,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>228</v>
       </c>
@@ -22858,7 +22876,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>231</v>
       </c>
@@ -22896,7 +22914,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>232</v>
       </c>
@@ -22937,7 +22955,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>233</v>
       </c>
@@ -22978,7 +22996,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>234</v>
       </c>
@@ -23019,7 +23037,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>235</v>
       </c>
@@ -23060,12 +23078,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>236</v>
       </c>
       <c r="B160" s="18" t="s">
         <v>1539</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>2261</v>
       </c>
       <c r="F160" s="18" t="s">
         <v>1102</v>
@@ -23095,7 +23119,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>237</v>
       </c>
@@ -23130,7 +23154,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>238</v>
       </c>
@@ -23165,7 +23189,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>239</v>
       </c>
@@ -23203,7 +23227,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>240</v>
       </c>
@@ -23241,7 +23265,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>241</v>
       </c>
@@ -23276,7 +23300,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>242</v>
       </c>
@@ -23314,7 +23338,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>243</v>
       </c>
@@ -23349,7 +23373,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>244</v>
       </c>
@@ -23387,7 +23411,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>245</v>
       </c>
@@ -23428,7 +23452,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>246</v>
       </c>
@@ -23463,12 +23487,18 @@
         <v>691</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>247</v>
       </c>
       <c r="B171" s="21" t="s">
         <v>1500</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>2259</v>
       </c>
       <c r="F171" s="21" t="s">
         <v>1102</v>
@@ -23498,7 +23528,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>248</v>
       </c>
@@ -23541,7 +23571,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>249</v>
       </c>
@@ -23576,7 +23606,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>250</v>
       </c>
@@ -23611,7 +23641,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>251</v>
       </c>
@@ -23646,7 +23676,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>252</v>
       </c>
@@ -23681,7 +23711,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>253</v>
       </c>
@@ -23719,7 +23749,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>256</v>
       </c>
@@ -23757,7 +23787,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="179" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>257</v>
       </c>
@@ -23792,7 +23822,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>258</v>
       </c>
@@ -23827,7 +23857,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>259</v>
       </c>
@@ -23862,7 +23892,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>260</v>
       </c>
@@ -23903,7 +23933,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>261</v>
       </c>
@@ -23938,7 +23968,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>262</v>
       </c>
@@ -23973,7 +24003,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>263</v>
       </c>
@@ -24008,7 +24038,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>264</v>
       </c>
@@ -24043,7 +24073,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>274</v>
       </c>
@@ -24076,7 +24106,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>275</v>
       </c>
@@ -24109,7 +24139,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>276</v>
       </c>
@@ -24142,7 +24172,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>277</v>
       </c>
@@ -24175,7 +24205,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>278</v>
       </c>
@@ -24208,7 +24238,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="192" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>279</v>
       </c>
@@ -24241,7 +24271,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>280</v>
       </c>
@@ -24274,7 +24304,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>281</v>
       </c>
@@ -24307,7 +24337,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>282</v>
       </c>
@@ -24340,7 +24370,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>283</v>
       </c>
@@ -24373,7 +24403,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>284</v>
       </c>
@@ -24406,7 +24436,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>285</v>
       </c>
@@ -24439,7 +24469,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>286</v>
       </c>
@@ -24474,7 +24504,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>287</v>
       </c>
@@ -24509,7 +24539,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>288</v>
       </c>
@@ -24544,7 +24574,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>289</v>
       </c>
@@ -24579,7 +24609,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>290</v>
       </c>
@@ -24614,7 +24644,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>291</v>
       </c>
@@ -24649,7 +24679,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>292</v>
       </c>
@@ -24684,7 +24714,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>295</v>
       </c>
@@ -24719,7 +24749,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>296</v>
       </c>
@@ -24754,7 +24784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>297</v>
       </c>
@@ -24789,7 +24819,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>298</v>
       </c>
@@ -24824,7 +24854,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>299</v>
       </c>
@@ -24859,7 +24889,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>300</v>
       </c>
@@ -24894,7 +24924,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>301</v>
       </c>
@@ -24929,7 +24959,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>302</v>
       </c>
@@ -24964,7 +24994,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>303</v>
       </c>
@@ -24999,7 +25029,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>304</v>
       </c>
@@ -25034,7 +25064,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>305</v>
       </c>
@@ -25069,7 +25099,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>306</v>
       </c>
@@ -25104,7 +25134,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>307</v>
       </c>
@@ -25139,7 +25169,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>308</v>
       </c>
@@ -25174,7 +25204,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>309</v>
       </c>
@@ -25209,7 +25239,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>310</v>
       </c>
@@ -25244,7 +25274,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>311</v>
       </c>
@@ -25282,7 +25312,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>312</v>
       </c>
@@ -25320,7 +25350,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A224" s="53">
         <v>313</v>
       </c>
@@ -25362,7 +25392,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>314</v>
       </c>
@@ -25397,7 +25427,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>315</v>
       </c>
@@ -25432,7 +25462,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>316</v>
       </c>
@@ -25467,7 +25497,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>317</v>
       </c>
@@ -25502,7 +25532,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>318</v>
       </c>
@@ -25537,7 +25567,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>319</v>
       </c>
@@ -25572,7 +25602,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>320</v>
       </c>
@@ -25607,7 +25637,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>321</v>
       </c>
@@ -25642,7 +25672,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>322</v>
       </c>
@@ -25675,7 +25705,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="234" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>323</v>
       </c>
@@ -25708,7 +25738,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>324</v>
       </c>
@@ -25747,7 +25777,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>325</v>
       </c>
@@ -25786,7 +25816,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>328</v>
       </c>
@@ -25825,7 +25855,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>329</v>
       </c>
@@ -25864,7 +25894,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>331</v>
       </c>
@@ -25903,7 +25933,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>332</v>
       </c>
@@ -25938,7 +25968,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>333</v>
       </c>
@@ -25976,7 +26006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>334</v>
       </c>
@@ -26011,7 +26041,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>335</v>
       </c>
@@ -26049,7 +26079,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>336</v>
       </c>
@@ -26087,7 +26117,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>337</v>
       </c>
@@ -26125,7 +26155,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>338</v>
       </c>
@@ -26160,7 +26190,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>339</v>
       </c>
@@ -26195,7 +26225,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>341</v>
       </c>
@@ -26233,7 +26263,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>342</v>
       </c>
@@ -26271,7 +26301,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>343</v>
       </c>
@@ -26306,7 +26336,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>344</v>
       </c>
@@ -26341,7 +26371,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>345</v>
       </c>
@@ -26379,7 +26409,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>346</v>
       </c>
@@ -26417,7 +26447,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>347</v>
       </c>
@@ -26452,7 +26482,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>348</v>
       </c>
@@ -26490,7 +26520,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>349</v>
       </c>
@@ -26528,7 +26558,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>350</v>
       </c>
@@ -26563,7 +26593,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>351</v>
       </c>
@@ -26598,7 +26628,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A259" s="53">
         <v>352</v>
       </c>
@@ -26640,7 +26670,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>354</v>
       </c>
@@ -26675,7 +26705,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>355</v>
       </c>
@@ -26710,7 +26740,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>356</v>
       </c>
@@ -26751,7 +26781,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>359</v>
       </c>
@@ -26786,7 +26816,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>360</v>
       </c>
@@ -26821,7 +26851,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:16" ht="277.8" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>362</v>
       </c>
@@ -26856,7 +26886,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>363</v>
       </c>
@@ -26934,7 +26964,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>365</v>
       </c>
@@ -26969,7 +26999,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>366</v>
       </c>
@@ -27007,7 +27037,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>367</v>
       </c>
@@ -27045,7 +27075,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>368</v>
       </c>
@@ -27083,7 +27113,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>369</v>
       </c>
@@ -27118,7 +27148,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>370</v>
       </c>
@@ -27153,7 +27183,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>371</v>
       </c>
@@ -27191,7 +27221,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>372</v>
       </c>
@@ -27229,7 +27259,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>373</v>
       </c>
@@ -27264,7 +27294,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>374</v>
       </c>
@@ -27299,7 +27329,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>375</v>
       </c>
@@ -27334,7 +27364,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>376</v>
       </c>
@@ -27369,7 +27399,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>377</v>
       </c>
@@ -27404,7 +27434,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>378</v>
       </c>
@@ -27439,7 +27469,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>379</v>
       </c>
@@ -27474,7 +27504,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>380</v>
       </c>
@@ -27509,7 +27539,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>381</v>
       </c>
@@ -27544,7 +27574,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>382</v>
       </c>
@@ -27579,7 +27609,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A286" s="53">
         <v>385</v>
       </c>
@@ -27621,7 +27651,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>386</v>
       </c>
@@ -27657,7 +27687,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A288" s="53">
         <v>387</v>
       </c>
@@ -27699,7 +27729,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>388</v>
       </c>
@@ -27740,7 +27770,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>389</v>
       </c>
@@ -27775,7 +27805,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A291" s="53">
         <v>390</v>
       </c>
@@ -27860,7 +27890,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>392</v>
       </c>
@@ -27901,7 +27931,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>393</v>
       </c>
@@ -27936,7 +27966,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>394</v>
       </c>
@@ -27977,7 +28007,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>395</v>
       </c>
@@ -28018,7 +28048,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>396</v>
       </c>
@@ -28053,7 +28083,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>397</v>
       </c>
@@ -28094,7 +28124,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="299" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>398</v>
       </c>
@@ -28129,7 +28159,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>399</v>
       </c>
@@ -28164,7 +28194,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="301" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>400</v>
       </c>
@@ -28199,7 +28229,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>401</v>
       </c>
@@ -28240,7 +28270,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="303" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>402</v>
       </c>
@@ -28277,7 +28307,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="304" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>403</v>
       </c>
@@ -28314,7 +28344,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>404</v>
       </c>
@@ -28351,7 +28381,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>405</v>
       </c>
@@ -28388,7 +28418,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>406</v>
       </c>
@@ -28425,7 +28455,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>407</v>
       </c>
@@ -28462,7 +28492,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>408</v>
       </c>
@@ -28499,7 +28529,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="310" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>409</v>
       </c>
@@ -28536,7 +28566,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>410</v>
       </c>
@@ -28573,7 +28603,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>411</v>
       </c>
@@ -28610,7 +28640,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>412</v>
       </c>
@@ -28647,7 +28677,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>413</v>
       </c>
@@ -28682,7 +28712,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>415</v>
       </c>
@@ -28717,7 +28747,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>417</v>
       </c>
@@ -28754,7 +28784,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>418</v>
       </c>
@@ -28791,7 +28821,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>419</v>
       </c>
@@ -28828,7 +28858,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>420</v>
       </c>
@@ -28865,7 +28895,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>421</v>
       </c>
@@ -28902,7 +28932,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>422</v>
       </c>
@@ -28939,7 +28969,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>423</v>
       </c>
@@ -28976,7 +29006,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="323" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>424</v>
       </c>
@@ -29013,7 +29043,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>426</v>
       </c>
@@ -29048,7 +29078,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>427</v>
       </c>
@@ -29083,7 +29113,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>429</v>
       </c>
@@ -29120,7 +29150,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>430</v>
       </c>
@@ -29157,7 +29187,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>431</v>
       </c>
@@ -29194,7 +29224,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>432</v>
       </c>
@@ -29231,7 +29261,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>433</v>
       </c>
@@ -29268,7 +29298,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>434</v>
       </c>
@@ -29305,7 +29335,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A332" s="1">
         <v>435</v>
       </c>
@@ -29340,7 +29370,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A333" s="1">
         <v>436</v>
       </c>
@@ -29375,7 +29405,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A334" s="1">
         <v>437</v>
       </c>
@@ -29410,7 +29440,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A335" s="1">
         <v>440</v>
       </c>
@@ -29447,7 +29477,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>441</v>
       </c>
@@ -29488,7 +29518,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="337" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A337" s="1">
         <v>442</v>
       </c>
@@ -29525,7 +29555,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="338" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>443</v>
       </c>
@@ -29562,7 +29592,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="339" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A339" s="1">
         <v>444</v>
       </c>
@@ -29599,7 +29629,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="340" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>445</v>
       </c>
@@ -29636,7 +29666,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="341" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A341" s="1">
         <v>448</v>
       </c>
@@ -29673,7 +29703,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="342" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A342" s="1">
         <v>449</v>
       </c>
@@ -29710,7 +29740,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="343" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
         <v>450</v>
       </c>
@@ -29747,7 +29777,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="344" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
         <v>451</v>
       </c>
@@ -29784,7 +29814,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A345" s="1">
         <v>452</v>
       </c>
@@ -29821,7 +29851,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="346" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A346" s="1">
         <v>453</v>
       </c>
@@ -29858,7 +29888,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="347" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A347" s="1">
         <v>455</v>
       </c>
@@ -29895,7 +29925,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="348" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>456</v>
       </c>
@@ -29932,7 +29962,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>457</v>
       </c>
@@ -29973,7 +30003,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="350" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A350" s="1">
         <v>458</v>
       </c>
@@ -30010,7 +30040,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="351" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>459</v>
       </c>
@@ -30047,7 +30077,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="352" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A352" s="1">
         <v>460</v>
       </c>
@@ -30084,7 +30114,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A353" s="1">
         <v>461</v>
       </c>
@@ -30121,7 +30151,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A354" s="1">
         <v>463</v>
       </c>
@@ -30158,7 +30188,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A355" s="1">
         <v>464</v>
       </c>
@@ -30195,7 +30225,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A356" s="1">
         <v>465</v>
       </c>
@@ -30232,7 +30262,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="357" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A357" s="1">
         <v>469</v>
       </c>
@@ -30269,7 +30299,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A358" s="1">
         <v>470</v>
       </c>
@@ -30306,15 +30336,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A359" s="1">
         <v>471</v>
       </c>
       <c r="B359" s="21" t="s">
         <v>911</v>
       </c>
-      <c r="C359" s="27"/>
-      <c r="D359" s="27"/>
+      <c r="C359" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D359" s="27" t="s">
+        <v>2261</v>
+      </c>
       <c r="F359" s="21" t="s">
         <v>1102</v>
       </c>
@@ -30343,7 +30377,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A360" s="1">
         <v>472</v>
       </c>
@@ -30380,7 +30414,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A361" s="1">
         <v>473</v>
       </c>
@@ -30417,7 +30451,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>474</v>
       </c>
@@ -30454,7 +30488,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A363" s="1">
         <v>475</v>
       </c>
@@ -30491,7 +30525,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
         <v>476</v>
       </c>
@@ -30528,7 +30562,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A365" s="1">
         <v>477</v>
       </c>
@@ -30565,7 +30599,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A366" s="1">
         <v>479</v>
       </c>
@@ -30600,7 +30634,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A367" s="1">
         <v>480</v>
       </c>
@@ -30635,7 +30669,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A368" s="1">
         <v>481</v>
       </c>
@@ -30670,7 +30704,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="330.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A369" s="1">
         <v>482</v>
       </c>
@@ -30705,7 +30739,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A370" s="1">
         <v>483</v>
       </c>
@@ -30742,7 +30776,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A371" s="1">
         <v>484</v>
       </c>
@@ -30777,7 +30811,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="145.80000000000001" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A372" s="1">
         <v>485</v>
       </c>
@@ -30812,7 +30846,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A373" s="1">
         <v>486</v>
       </c>
@@ -30847,7 +30881,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" ht="383.4" x14ac:dyDescent="0.3">
       <c r="A374" s="1">
         <v>487</v>
       </c>
@@ -30882,7 +30916,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A375" s="1">
         <v>489</v>
       </c>
@@ -30917,7 +30951,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" ht="330.6" x14ac:dyDescent="0.3">
       <c r="A376" s="1">
         <v>490</v>
       </c>
@@ -30952,7 +30986,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A377" s="1">
         <v>491</v>
       </c>
@@ -30987,7 +31021,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" ht="383.4" x14ac:dyDescent="0.3">
       <c r="A378" s="1">
         <v>492</v>
       </c>
@@ -31022,7 +31056,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A379" s="1">
         <v>493</v>
       </c>
@@ -31057,7 +31091,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="291" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A380" s="1">
         <v>494</v>
       </c>
@@ -31092,7 +31126,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" ht="159" x14ac:dyDescent="0.3">
       <c r="A381" s="1">
         <v>495</v>
       </c>
@@ -31127,7 +31161,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="277.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A382" s="1">
         <v>498</v>
       </c>
@@ -31162,7 +31196,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A383" s="1">
         <v>499</v>
       </c>
@@ -31197,7 +31231,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A384" s="1">
         <v>500</v>
       </c>
@@ -31232,7 +31266,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="383.4" x14ac:dyDescent="0.3">
       <c r="A385" s="1">
         <v>501</v>
       </c>
@@ -31267,7 +31301,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="317.39999999999998" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A386" s="1">
         <v>503</v>
       </c>
@@ -31302,7 +31336,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="330.6" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
         <v>504</v>
       </c>
@@ -31337,7 +31371,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="357" x14ac:dyDescent="0.3">
       <c r="A388" s="1">
         <v>505</v>
       </c>
@@ -31372,7 +31406,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="389" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>506</v>
       </c>
@@ -31405,7 +31439,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="390" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A390" s="1">
         <v>507</v>
       </c>
@@ -31436,7 +31470,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="391" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>508</v>
       </c>
@@ -31469,7 +31503,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A392" s="1">
         <v>509</v>
       </c>
@@ -31510,7 +31544,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="277.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="277.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>510</v>
       </c>
@@ -31551,15 +31585,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="343.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B394" s="18"/>
+    <row r="394" spans="1:16" ht="343.8" x14ac:dyDescent="0.3">
+      <c r="B394" s="18" t="s">
+        <v>2243</v>
+      </c>
       <c r="C394" s="18" t="s">
         <v>496</v>
       </c>
       <c r="D394" s="18" t="s">
         <v>2259</v>
       </c>
-      <c r="F394" s="18"/>
+      <c r="F394" s="18" t="s">
+        <v>1102</v>
+      </c>
       <c r="G394" s="18"/>
       <c r="H394" s="18" t="s">
         <v>604</v>
@@ -31579,15 +31617,19 @@
       <c r="O394" s="18"/>
       <c r="P394" s="18"/>
     </row>
-    <row r="395" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B395" s="18"/>
+    <row r="395" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
+      <c r="B395" s="18" t="s">
+        <v>2244</v>
+      </c>
       <c r="C395" s="18" t="s">
         <v>496</v>
       </c>
       <c r="D395" s="18" t="s">
         <v>2259</v>
       </c>
-      <c r="F395" s="18"/>
+      <c r="F395" s="18" t="s">
+        <v>1102</v>
+      </c>
       <c r="G395" s="18" t="s">
         <v>2251</v>
       </c>
@@ -31609,7 +31651,7 @@
       <c r="O395" s="18"/>
       <c r="P395" s="18"/>
     </row>
-    <row r="396" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A396" s="1">
         <v>511</v>
       </c>
@@ -31646,7 +31688,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="264.60000000000002" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:16" ht="264.60000000000002" x14ac:dyDescent="0.3">
       <c r="A397" s="1">
         <v>512</v>
       </c>
@@ -31683,15 +31725,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A398" s="1">
         <v>513</v>
       </c>
       <c r="B398" s="21" t="s">
         <v>821</v>
       </c>
-      <c r="C398" s="27"/>
-      <c r="D398" s="27"/>
+      <c r="C398" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D398" s="27" t="s">
+        <v>2261</v>
+      </c>
       <c r="F398" s="21" t="s">
         <v>1102</v>
       </c>
@@ -31720,15 +31766,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="172.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:16" ht="172.2" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
         <v>514</v>
       </c>
       <c r="B399" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="C399" s="18"/>
-      <c r="D399" s="18"/>
+      <c r="C399" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="D399" s="18" t="s">
+        <v>2261</v>
+      </c>
       <c r="F399" s="18" t="s">
         <v>1102</v>
       </c>
@@ -31757,15 +31807,19 @@
         <v>691</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>515</v>
       </c>
       <c r="B400" s="21" t="s">
         <v>813</v>
       </c>
-      <c r="C400" s="27"/>
-      <c r="D400" s="27"/>
+      <c r="C400" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="D400" s="27" t="s">
+        <v>2261</v>
+      </c>
       <c r="F400" s="21" t="s">
         <v>1102</v>
       </c>
@@ -31794,7 +31848,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="304.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:16" ht="304.2" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>516</v>
       </c>
@@ -31835,7 +31889,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="396.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:16" ht="396.6" x14ac:dyDescent="0.3">
       <c r="B402" s="18" t="s">
         <v>2252</v>
       </c>
@@ -31845,7 +31899,9 @@
       <c r="D402" s="18" t="s">
         <v>2259</v>
       </c>
-      <c r="F402" s="18"/>
+      <c r="F402" s="18" t="s">
+        <v>1102</v>
+      </c>
       <c r="G402" s="18"/>
       <c r="H402" s="18" t="s">
         <v>604</v>
@@ -31870,10 +31926,10 @@
         <v>2253</v>
       </c>
       <c r="C403" s="18" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D403" s="18" t="s">
-        <v>2261</v>
+        <v>2263</v>
       </c>
       <c r="F403" s="18" t="s">
         <v>1102</v>
@@ -31938,7 +31994,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>518</v>
       </c>
@@ -31975,7 +32031,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="406" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>529</v>
       </c>
@@ -32012,7 +32068,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="407" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>541</v>
       </c>
@@ -32045,7 +32101,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="408" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>547</v>
       </c>
@@ -32078,7 +32134,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="409" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>548</v>
       </c>
@@ -32111,7 +32167,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="410" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>564</v>
       </c>
@@ -32148,7 +32204,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="411" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>565</v>
       </c>
@@ -32185,7 +32241,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="412" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>570</v>
       </c>
@@ -32222,7 +32278,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="413" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>571</v>
       </c>
@@ -32263,7 +32319,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="414" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A414" s="1">
         <v>574</v>
       </c>
@@ -32300,7 +32356,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="415" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A415" s="1">
         <v>575</v>
       </c>
@@ -32337,7 +32393,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="416" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A416" s="1">
         <v>576</v>
       </c>
@@ -32374,7 +32430,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="417" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:16" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A417" s="1">
         <v>577</v>
       </c>
@@ -32411,7 +32467,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="418" spans="1:16" ht="66.599999999999994" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:16" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A418" s="1">
         <v>580</v>
       </c>
@@ -32448,7 +32504,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="419" spans="1:16" ht="40.200000000000003" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A419" s="1">
         <v>581</v>
       </c>
@@ -32485,7 +32541,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="420" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>582</v>
       </c>
@@ -32520,7 +32576,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="421" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>583</v>
       </c>
@@ -32555,7 +32611,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="422" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A422" s="1">
         <v>584</v>
       </c>
@@ -32590,7 +32646,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="423" spans="1:16" ht="106.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:16" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
         <v>585</v>
       </c>
@@ -32625,7 +32681,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="424" spans="1:16" ht="119.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
         <v>586</v>
       </c>
@@ -32660,7 +32716,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="425" spans="1:16" ht="53.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:16" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>587</v>
       </c>
@@ -32697,7 +32753,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="426" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A426" s="1">
         <v>588</v>
       </c>
@@ -32732,7 +32788,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="427" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>589</v>
       </c>
@@ -32767,7 +32823,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="428" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
         <v>590</v>
       </c>
@@ -32802,7 +32858,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="429" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>591</v>
       </c>
@@ -32837,7 +32893,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="430" spans="1:16" ht="132.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:16" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>592</v>
       </c>
@@ -32872,7 +32928,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="431" spans="1:16" ht="185.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:16" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>593</v>
       </c>
@@ -32907,7 +32963,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="432" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>594</v>
       </c>
@@ -32942,7 +32998,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="433" spans="1:16" ht="211.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:16" ht="211.8" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>595</v>
       </c>
@@ -32977,7 +33033,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="434" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>596</v>
       </c>
@@ -33012,7 +33068,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="435" spans="1:16" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:16" ht="225" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>597</v>
       </c>
@@ -33047,7 +33103,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="436" spans="1:16" ht="198.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:16" ht="198.6" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>598</v>
       </c>
@@ -33084,7 +33140,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="437" spans="1:16" ht="27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>599</v>
       </c>
@@ -33121,7 +33177,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="438" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:16" ht="93" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>600</v>
       </c>
@@ -33156,7 +33212,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="439" spans="1:16" ht="93" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>601</v>
       </c>
@@ -33191,7 +33247,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="440" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>602</v>
       </c>
@@ -33228,7 +33284,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="441" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A441" s="1">
         <v>603</v>
       </c>
@@ -33265,7 +33321,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="442" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A442" s="1">
         <v>604</v>
       </c>
@@ -33302,7 +33358,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="443" spans="1:16" ht="251.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:16" ht="251.4" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>605</v>
       </c>
@@ -33337,7 +33393,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="444" spans="1:16" ht="159" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:16" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A444" s="1">
         <v>606</v>
       </c>
@@ -33372,7 +33428,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="445" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A445" s="1">
         <v>607</v>
       </c>
@@ -33407,7 +33463,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="446" spans="1:16" ht="79.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:16" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A446" s="1">
         <v>608</v>
       </c>
@@ -33443,14 +33499,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P446">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Sprint"/>
-        <filter val="Sprint 22 Sep - 29 Sep"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>